<commit_message>
Updated cli-client.js; Updated genedruglist.js to be drug based
</commit_message>
<xml_diff>
--- a/cpicPairs.xlsx
+++ b/cpicPairs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14115" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14115" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="cpicPairs" sheetId="1" r:id="rId1"/>
@@ -1382,7 +1382,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1571,6 +1571,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEEEEEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1783,7 +1795,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1834,13 +1846,14 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1858,13 +1871,30 @@
     <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1911,7 +1941,133 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="45">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <right style="thin">
@@ -6649,8 +6805,8 @@
   <dataFields count="1">
     <dataField name="Count of Guideline" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="27">
-    <format dxfId="26">
+  <formats count="45">
+    <format dxfId="44">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14" selected="0">
@@ -6672,13 +6828,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="43">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="42">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="41">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14">
@@ -6700,10 +6856,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="40">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="21">
+    <format dxfId="39">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14" selected="0">
@@ -6725,13 +6881,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="38">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="19">
+    <format dxfId="37">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="18">
+    <format dxfId="36">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14">
@@ -6753,10 +6909,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="35">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="16">
+    <format dxfId="34">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -6765,17 +6921,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="33">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="32">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="13">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6784,7 +6940,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="30">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -6793,17 +6949,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="29">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="28">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="9">
+    <format dxfId="27">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6812,7 +6968,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="26">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -6821,17 +6977,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="25">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="24">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="5">
+    <format dxfId="23">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6840,16 +6996,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="22">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="21">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="20">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="1">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="38">
@@ -6895,8 +7051,378 @@
         </references>
       </pivotArea>
     </format>
+    <format dxfId="18">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="17">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="64"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="16">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="42"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="15">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="45"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="14">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="72"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="13">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="39"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="47"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="12">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="64"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="11">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="118"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="10">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="22"/>
+          </reference>
+          <reference field="1" count="17">
+            <x v="0"/>
+            <x v="5"/>
+            <x v="7"/>
+            <x v="14"/>
+            <x v="17"/>
+            <x v="25"/>
+            <x v="27"/>
+            <x v="42"/>
+            <x v="44"/>
+            <x v="45"/>
+            <x v="47"/>
+            <x v="54"/>
+            <x v="65"/>
+            <x v="72"/>
+            <x v="80"/>
+            <x v="85"/>
+            <x v="99"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="22"/>
+          </reference>
+          <reference field="1" count="20">
+            <x v="116"/>
+            <x v="141"/>
+            <x v="144"/>
+            <x v="147"/>
+            <x v="151"/>
+            <x v="153"/>
+            <x v="154"/>
+            <x v="159"/>
+            <x v="174"/>
+            <x v="175"/>
+            <x v="183"/>
+            <x v="186"/>
+            <x v="198"/>
+            <x v="199"/>
+            <x v="201"/>
+            <x v="205"/>
+            <x v="212"/>
+            <x v="213"/>
+            <x v="219"/>
+            <x v="221"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="123"/>
+          </reference>
+          <reference field="1" count="37">
+            <x v="0"/>
+            <x v="5"/>
+            <x v="7"/>
+            <x v="14"/>
+            <x v="17"/>
+            <x v="25"/>
+            <x v="27"/>
+            <x v="42"/>
+            <x v="44"/>
+            <x v="45"/>
+            <x v="47"/>
+            <x v="54"/>
+            <x v="65"/>
+            <x v="72"/>
+            <x v="80"/>
+            <x v="85"/>
+            <x v="99"/>
+            <x v="105"/>
+            <x v="116"/>
+            <x v="141"/>
+            <x v="144"/>
+            <x v="147"/>
+            <x v="151"/>
+            <x v="153"/>
+            <x v="154"/>
+            <x v="159"/>
+            <x v="174"/>
+            <x v="175"/>
+            <x v="183"/>
+            <x v="186"/>
+            <x v="198"/>
+            <x v="199"/>
+            <x v="201"/>
+            <x v="205"/>
+            <x v="212"/>
+            <x v="213"/>
+            <x v="219"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="118"/>
+          </reference>
+          <reference field="1" count="3">
+            <x v="0"/>
+            <x v="5"/>
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="118"/>
+          </reference>
+          <reference field="1" count="34">
+            <x v="17"/>
+            <x v="25"/>
+            <x v="27"/>
+            <x v="42"/>
+            <x v="44"/>
+            <x v="45"/>
+            <x v="47"/>
+            <x v="54"/>
+            <x v="65"/>
+            <x v="72"/>
+            <x v="80"/>
+            <x v="85"/>
+            <x v="99"/>
+            <x v="105"/>
+            <x v="116"/>
+            <x v="141"/>
+            <x v="144"/>
+            <x v="147"/>
+            <x v="151"/>
+            <x v="153"/>
+            <x v="154"/>
+            <x v="159"/>
+            <x v="174"/>
+            <x v="175"/>
+            <x v="183"/>
+            <x v="186"/>
+            <x v="198"/>
+            <x v="199"/>
+            <x v="201"/>
+            <x v="205"/>
+            <x v="212"/>
+            <x v="213"/>
+            <x v="219"/>
+            <x v="221"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="12" selected="0">
+            <x v="36"/>
+            <x v="38"/>
+            <x v="39"/>
+            <x v="41"/>
+            <x v="42"/>
+            <x v="43"/>
+            <x v="54"/>
+            <x v="63"/>
+            <x v="64"/>
+            <x v="74"/>
+            <x v="108"/>
+            <x v="115"/>
+          </reference>
+          <reference field="1" count="38">
+            <x v="0"/>
+            <x v="5"/>
+            <x v="7"/>
+            <x v="14"/>
+            <x v="17"/>
+            <x v="25"/>
+            <x v="27"/>
+            <x v="42"/>
+            <x v="44"/>
+            <x v="45"/>
+            <x v="47"/>
+            <x v="54"/>
+            <x v="65"/>
+            <x v="72"/>
+            <x v="80"/>
+            <x v="85"/>
+            <x v="99"/>
+            <x v="105"/>
+            <x v="116"/>
+            <x v="141"/>
+            <x v="144"/>
+            <x v="147"/>
+            <x v="151"/>
+            <x v="153"/>
+            <x v="154"/>
+            <x v="159"/>
+            <x v="174"/>
+            <x v="175"/>
+            <x v="183"/>
+            <x v="186"/>
+            <x v="198"/>
+            <x v="199"/>
+            <x v="201"/>
+            <x v="205"/>
+            <x v="212"/>
+            <x v="213"/>
+            <x v="219"/>
+            <x v="221"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="42"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="45"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="72"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="39"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="47"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="0">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
     </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -7173,7 +7699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G356"/>
   <sheetViews>
-    <sheetView topLeftCell="A220" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -12665,7 +13191,7 @@
   <dimension ref="A3:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A4:A23"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -13033,8 +13559,8 @@
   </sheetPr>
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -13215,23 +13741,23 @@
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8">
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="34">
         <v>1</v>
       </c>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
       <c r="Q5" s="9">
         <v>1</v>
       </c>
@@ -13240,23 +13766,23 @@
       <c r="A6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8">
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="34">
         <v>1</v>
       </c>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
       <c r="Q6" s="9">
         <v>1</v>
       </c>
@@ -13265,25 +13791,25 @@
       <c r="A7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7">
+      <c r="B7" s="35"/>
+      <c r="C7" s="36">
         <v>1</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8">
+      <c r="D7" s="33"/>
+      <c r="E7" s="34">
         <v>1</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
       <c r="Q7" s="9">
         <v>2</v>
       </c>
@@ -13292,23 +13818,23 @@
       <c r="A8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8">
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="31">
         <v>1</v>
       </c>
-      <c r="P8" s="8"/>
+      <c r="P8" s="33"/>
       <c r="Q8" s="9">
         <v>1</v>
       </c>
@@ -13317,23 +13843,23 @@
       <c r="A9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8">
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="34">
         <v>1</v>
       </c>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="33"/>
       <c r="Q9" s="9">
         <v>1</v>
       </c>
@@ -13342,23 +13868,23 @@
       <c r="A10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8">
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="34">
         <v>1</v>
       </c>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="33"/>
       <c r="Q10" s="9">
         <v>1</v>
       </c>
@@ -13367,25 +13893,25 @@
       <c r="A11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8">
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="34">
         <v>1</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11" s="34">
         <v>1</v>
       </c>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="33"/>
+      <c r="P11" s="33"/>
       <c r="Q11" s="9">
         <v>2</v>
       </c>
@@ -13394,23 +13920,23 @@
       <c r="A12" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7">
+      <c r="B12" s="35"/>
+      <c r="C12" s="32">
         <v>1</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="33"/>
       <c r="Q12" s="9">
         <v>1</v>
       </c>
@@ -13419,25 +13945,25 @@
       <c r="A13" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7">
+      <c r="B13" s="35"/>
+      <c r="C13" s="35">
         <v>1</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8">
+      <c r="D13" s="33"/>
+      <c r="E13" s="34">
         <v>1</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="33"/>
+      <c r="P13" s="33"/>
       <c r="Q13" s="9">
         <v>2</v>
       </c>
@@ -13446,23 +13972,23 @@
       <c r="A14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7">
+      <c r="B14" s="35"/>
+      <c r="C14" s="32">
         <v>1</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="33"/>
+      <c r="O14" s="33"/>
+      <c r="P14" s="33"/>
       <c r="Q14" s="9">
         <v>1</v>
       </c>
@@ -13471,23 +13997,23 @@
       <c r="A15" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8">
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="31">
         <v>1</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="33"/>
+      <c r="O15" s="33"/>
+      <c r="P15" s="33"/>
       <c r="Q15" s="9">
         <v>1</v>
       </c>
@@ -13496,23 +14022,23 @@
       <c r="A16" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8">
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="34">
         <v>1</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
+      <c r="O16" s="33"/>
+      <c r="P16" s="33"/>
       <c r="Q16" s="9">
         <v>1</v>
       </c>
@@ -13521,25 +14047,25 @@
       <c r="A17" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7">
+      <c r="B17" s="35"/>
+      <c r="C17" s="35">
         <v>1</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8">
+      <c r="D17" s="33"/>
+      <c r="E17" s="34">
         <v>1</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="33"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="33"/>
       <c r="Q17" s="9">
         <v>2</v>
       </c>
@@ -13548,23 +14074,23 @@
       <c r="A18" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7">
+      <c r="B18" s="35"/>
+      <c r="C18" s="32">
         <v>1</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="33"/>
+      <c r="P18" s="33"/>
       <c r="Q18" s="9">
         <v>1</v>
       </c>
@@ -13573,23 +14099,23 @@
       <c r="A19" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8">
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="34">
         <v>1</v>
       </c>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
+      <c r="O19" s="33"/>
+      <c r="P19" s="33"/>
       <c r="Q19" s="9">
         <v>1</v>
       </c>
@@ -13598,23 +14124,23 @@
       <c r="A20" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8">
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="34">
         <v>1</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="33"/>
+      <c r="P20" s="33"/>
       <c r="Q20" s="9">
         <v>1</v>
       </c>
@@ -13623,25 +14149,25 @@
       <c r="A21" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7">
+      <c r="B21" s="35"/>
+      <c r="C21" s="36">
         <v>1</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8">
+      <c r="D21" s="33"/>
+      <c r="E21" s="34">
         <v>1</v>
       </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
+      <c r="O21" s="33"/>
+      <c r="P21" s="33"/>
       <c r="Q21" s="9">
         <v>2</v>
       </c>
@@ -13653,20 +14179,20 @@
       <c r="B22" s="7">
         <v>1</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="33"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="33"/>
       <c r="Q22" s="9">
         <v>1</v>
       </c>
@@ -13675,23 +14201,23 @@
       <c r="A23" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8">
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="33"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="34">
         <v>1</v>
       </c>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
+      <c r="O23" s="33"/>
+      <c r="P23" s="33"/>
       <c r="Q23" s="9">
         <v>1</v>
       </c>
@@ -13700,23 +14226,23 @@
       <c r="A24" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8">
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="34">
         <v>1</v>
       </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="33"/>
+      <c r="O24" s="33"/>
+      <c r="P24" s="33"/>
       <c r="Q24" s="9">
         <v>1</v>
       </c>
@@ -13725,23 +14251,23 @@
       <c r="A25" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8">
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="34">
         <v>1</v>
       </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="33"/>
+      <c r="P25" s="33"/>
       <c r="Q25" s="9">
         <v>1</v>
       </c>
@@ -13750,23 +14276,23 @@
       <c r="A26" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8">
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="34">
         <v>1</v>
       </c>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="33"/>
+      <c r="N26" s="33"/>
+      <c r="O26" s="33"/>
+      <c r="P26" s="33"/>
       <c r="Q26" s="9">
         <v>1</v>
       </c>
@@ -13775,23 +14301,23 @@
       <c r="A27" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8">
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="34">
         <v>1</v>
       </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="33"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="33"/>
+      <c r="O27" s="33"/>
+      <c r="P27" s="33"/>
       <c r="Q27" s="9">
         <v>1</v>
       </c>
@@ -13800,23 +14326,23 @@
       <c r="A28" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8">
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="34">
         <v>1</v>
       </c>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
+      <c r="O28" s="33"/>
+      <c r="P28" s="33"/>
       <c r="Q28" s="9">
         <v>1</v>
       </c>
@@ -13825,23 +14351,23 @@
       <c r="A29" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8">
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="34">
         <v>1</v>
       </c>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="33"/>
+      <c r="O29" s="33"/>
+      <c r="P29" s="33"/>
       <c r="Q29" s="9">
         <v>1</v>
       </c>
@@ -13850,25 +14376,25 @@
       <c r="A30" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="8">
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="34">
         <v>1</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8">
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="34">
         <v>1</v>
       </c>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="33"/>
+      <c r="O30" s="33"/>
+      <c r="P30" s="33"/>
       <c r="Q30" s="9">
         <v>2</v>
       </c>
@@ -13877,23 +14403,23 @@
       <c r="A31" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8">
+      <c r="B31" s="35"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="34">
         <v>1</v>
       </c>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="33"/>
+      <c r="N31" s="33"/>
+      <c r="O31" s="33"/>
+      <c r="P31" s="33"/>
       <c r="Q31" s="9">
         <v>1</v>
       </c>
@@ -13902,23 +14428,23 @@
       <c r="A32" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8">
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="34">
         <v>1</v>
       </c>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="33"/>
+      <c r="O32" s="33"/>
+      <c r="P32" s="33"/>
       <c r="Q32" s="9">
         <v>1</v>
       </c>
@@ -13927,23 +14453,23 @@
       <c r="A33" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7">
+      <c r="B33" s="35"/>
+      <c r="C33" s="36">
         <v>1</v>
       </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
+      <c r="N33" s="33"/>
+      <c r="O33" s="33"/>
+      <c r="P33" s="33"/>
       <c r="Q33" s="9">
         <v>1</v>
       </c>
@@ -13952,23 +14478,23 @@
       <c r="A34" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8">
+      <c r="B34" s="35"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="33"/>
+      <c r="L34" s="33"/>
+      <c r="M34" s="34">
         <v>1</v>
       </c>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
+      <c r="N34" s="33"/>
+      <c r="O34" s="33"/>
+      <c r="P34" s="33"/>
       <c r="Q34" s="9">
         <v>1</v>
       </c>
@@ -13977,23 +14503,23 @@
       <c r="A35" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8">
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="34">
         <v>1</v>
       </c>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="33"/>
+      <c r="K35" s="33"/>
+      <c r="L35" s="33"/>
+      <c r="M35" s="33"/>
+      <c r="N35" s="33"/>
+      <c r="O35" s="33"/>
+      <c r="P35" s="33"/>
       <c r="Q35" s="9">
         <v>1</v>
       </c>
@@ -14002,23 +14528,23 @@
       <c r="A36" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8">
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="34">
         <v>1</v>
       </c>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="33"/>
+      <c r="K36" s="33"/>
+      <c r="L36" s="33"/>
+      <c r="M36" s="33"/>
+      <c r="N36" s="33"/>
+      <c r="O36" s="33"/>
+      <c r="P36" s="33"/>
       <c r="Q36" s="9">
         <v>1</v>
       </c>
@@ -14027,23 +14553,23 @@
       <c r="A37" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8">
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="34">
         <v>1</v>
       </c>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="33"/>
+      <c r="K37" s="33"/>
+      <c r="L37" s="33"/>
+      <c r="M37" s="33"/>
+      <c r="N37" s="33"/>
+      <c r="O37" s="33"/>
+      <c r="P37" s="33"/>
       <c r="Q37" s="9">
         <v>1</v>
       </c>
@@ -14052,23 +14578,23 @@
       <c r="A38" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8">
+      <c r="B38" s="35"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="33"/>
+      <c r="K38" s="33"/>
+      <c r="L38" s="33"/>
+      <c r="M38" s="33"/>
+      <c r="N38" s="34">
         <v>1</v>
       </c>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
+      <c r="O38" s="33"/>
+      <c r="P38" s="33"/>
       <c r="Q38" s="9">
         <v>1</v>
       </c>
@@ -14077,25 +14603,25 @@
       <c r="A39" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7">
+      <c r="B39" s="35"/>
+      <c r="C39" s="36">
         <v>1</v>
       </c>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8">
+      <c r="D39" s="33"/>
+      <c r="E39" s="34">
         <v>1</v>
       </c>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="33"/>
+      <c r="K39" s="33"/>
+      <c r="L39" s="33"/>
+      <c r="M39" s="33"/>
+      <c r="N39" s="33"/>
+      <c r="O39" s="33"/>
+      <c r="P39" s="33"/>
       <c r="Q39" s="9">
         <v>2</v>
       </c>
@@ -14104,23 +14630,23 @@
       <c r="A40" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8">
+      <c r="B40" s="35"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="34">
         <v>1</v>
       </c>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="33"/>
+      <c r="L40" s="33"/>
+      <c r="M40" s="33"/>
+      <c r="N40" s="33"/>
+      <c r="O40" s="33"/>
+      <c r="P40" s="33"/>
       <c r="Q40" s="9">
         <v>1</v>
       </c>
@@ -14129,23 +14655,23 @@
       <c r="A41" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7">
+      <c r="B41" s="35"/>
+      <c r="C41" s="36">
         <v>1</v>
       </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="8"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="33"/>
+      <c r="J41" s="33"/>
+      <c r="K41" s="33"/>
+      <c r="L41" s="33"/>
+      <c r="M41" s="33"/>
+      <c r="N41" s="33"/>
+      <c r="O41" s="33"/>
+      <c r="P41" s="33"/>
       <c r="Q41" s="9">
         <v>1</v>
       </c>
@@ -14154,24 +14680,24 @@
       <c r="A42" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="8">
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="34">
         <v>1</v>
       </c>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8">
+      <c r="E42" s="33"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="34">
         <v>1</v>
       </c>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="8"/>
-      <c r="O42" s="8"/>
+      <c r="H42" s="33"/>
+      <c r="I42" s="33"/>
+      <c r="J42" s="33"/>
+      <c r="K42" s="33"/>
+      <c r="L42" s="33"/>
+      <c r="M42" s="33"/>
+      <c r="N42" s="33"/>
+      <c r="O42" s="33"/>
       <c r="P42" s="8">
         <v>1</v>
       </c>
@@ -14245,7 +14771,7 @@
   </sheetPr>
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -14256,13 +14782,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
     </row>
@@ -14289,22 +14815,22 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="21" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="23" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="23"/>
+      <c r="C5" s="24"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
@@ -14354,10 +14880,10 @@
       <c r="A10" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="27" t="s">
         <v>407</v>
       </c>
     </row>
@@ -14365,26 +14891,26 @@
       <c r="A11" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="27"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="28"/>
     </row>
     <row r="12" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="21" t="s">
         <v>115</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="23" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="23"/>
+      <c r="C13" s="24"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
@@ -14420,22 +14946,22 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="21" t="s">
         <v>122</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="23" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="23"/>
+      <c r="C18" s="24"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
@@ -14460,22 +14986,22 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="25" t="s">
         <v>131</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="27" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="27"/>
+      <c r="C22" s="28"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
@@ -14547,10 +15073,10 @@
       <c r="A29" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="23" t="s">
         <v>407</v>
       </c>
     </row>
@@ -14558,33 +15084,33 @@
       <c r="A30" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="22"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="30"/>
     </row>
     <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="23"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="24"/>
     </row>
     <row r="32" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="25" t="s">
         <v>65</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="26" t="s">
+      <c r="C32" s="27" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="27"/>
+      <c r="C33" s="28"/>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
@@ -14664,22 +15190,22 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="24" t="s">
+      <c r="A41" s="25" t="s">
         <v>166</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="26" t="s">
+      <c r="C41" s="27" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="25"/>
+      <c r="A42" s="26"/>
       <c r="B42" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="27"/>
+      <c r="C42" s="28"/>
     </row>
     <row r="43" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
@@ -14704,38 +15230,36 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="28" t="s">
+      <c r="A45" s="21" t="s">
         <v>87</v>
       </c>
       <c r="B45" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C45" s="29" t="s">
+      <c r="C45" s="23" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="20"/>
+      <c r="A46" s="29"/>
       <c r="B46" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="22"/>
+      <c r="C46" s="30"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="20"/>
+      <c r="A47" s="29"/>
       <c r="B47" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="22"/>
+      <c r="C47" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
     <mergeCell ref="A41:A42"/>
     <mergeCell ref="C41:C42"/>
     <mergeCell ref="A45:A47"/>
@@ -14744,10 +15268,12 @@
     <mergeCell ref="C29:C31"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="C21:C22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://cpicpgx.org/guidelines/guideline-for-abacavir-and-hla-b/"/>

</xml_diff>

<commit_message>
Updated the remodeling of 99999-fk4mc97w6m
</commit_message>
<xml_diff>
--- a/cpicPairs.xlsx
+++ b/cpicPairs.xlsx
@@ -1382,7 +1382,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1583,6 +1583,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1795,7 +1801,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1847,36 +1853,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="14" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1894,6 +1870,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="14" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1941,7 +1956,98 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="58">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -6805,8 +6911,8 @@
   <dataFields count="1">
     <dataField name="Count of Guideline" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="45">
-    <format dxfId="44">
+  <formats count="58">
+    <format dxfId="57">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14" selected="0">
@@ -6828,13 +6934,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="43">
+    <format dxfId="56">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="55">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="54">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14">
@@ -6856,10 +6962,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="40">
+    <format dxfId="53">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="39">
+    <format dxfId="52">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14" selected="0">
@@ -6881,13 +6987,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="51">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="37">
+    <format dxfId="50">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="36">
+    <format dxfId="49">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14">
@@ -6909,10 +7015,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="35">
+    <format dxfId="48">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="34">
+    <format dxfId="47">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -6921,17 +7027,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="33">
+    <format dxfId="46">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="45">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="31">
+    <format dxfId="44">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6940,7 +7046,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="43">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -6949,17 +7055,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="42">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="41">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="27">
+    <format dxfId="40">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6968,7 +7074,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
+    <format dxfId="39">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -6977,17 +7083,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="38">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="24">
+    <format dxfId="37">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="36">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6996,16 +7102,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="35">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="21">
+    <format dxfId="34">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="20">
+    <format dxfId="33">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="19">
+    <format dxfId="32">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="38">
@@ -7051,10 +7157,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="17">
+    <format dxfId="30">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7066,7 +7172,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="29">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7078,7 +7184,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="28">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7090,7 +7196,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="27">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7102,7 +7208,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="26">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7114,7 +7220,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="25">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7126,7 +7232,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="24">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7138,7 +7244,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="23">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7166,7 +7272,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="22">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7197,7 +7303,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="21">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7245,7 +7351,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="20">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7259,7 +7365,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="19">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7304,7 +7410,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="18">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="12" selected="0">
@@ -7364,7 +7470,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="17">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7376,7 +7482,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="16">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7388,7 +7494,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="15">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7400,7 +7506,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="14">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7412,7 +7518,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="13">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7420,6 +7526,141 @@
           </reference>
           <reference field="1" count="1">
             <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="12">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="25"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="11">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="80"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="10">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="201"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="221"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="43"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="25"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="43"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="80"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="43"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="201"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="38"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="221"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="42"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="221"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="123"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="221"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="43"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="42"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="0">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="123"/>
           </reference>
         </references>
       </pivotArea>
@@ -13560,7 +13801,7 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+      <selection activeCell="R39" sqref="R39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -13703,10 +13944,10 @@
       <c r="F4" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="29" t="s">
         <v>31</v>
       </c>
       <c r="I4" s="5" t="s">
@@ -13730,7 +13971,7 @@
       <c r="O4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="29" t="s">
         <v>91</v>
       </c>
       <c r="Q4" s="6" t="s">
@@ -13741,23 +13982,23 @@
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="34">
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="24">
         <v>1</v>
       </c>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
       <c r="Q5" s="9">
         <v>1</v>
       </c>
@@ -13766,23 +14007,23 @@
       <c r="A6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="34">
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="24">
         <v>1</v>
       </c>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
       <c r="Q6" s="9">
         <v>1</v>
       </c>
@@ -13791,25 +14032,25 @@
       <c r="A7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="36">
+      <c r="B7" s="25"/>
+      <c r="C7" s="26">
         <v>1</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34">
+      <c r="D7" s="23"/>
+      <c r="E7" s="24">
         <v>1</v>
       </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
       <c r="Q7" s="9">
         <v>2</v>
       </c>
@@ -13818,23 +14059,23 @@
       <c r="A8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="31">
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="21">
         <v>1</v>
       </c>
-      <c r="P8" s="33"/>
+      <c r="P8" s="23"/>
       <c r="Q8" s="9">
         <v>1</v>
       </c>
@@ -13843,48 +14084,48 @@
       <c r="A9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="34">
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="24">
         <v>1</v>
       </c>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
       <c r="Q9" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="34">
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="28">
         <v>1</v>
       </c>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="33"/>
-      <c r="O10" s="33"/>
-      <c r="P10" s="33"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
       <c r="Q10" s="9">
         <v>1</v>
       </c>
@@ -13893,25 +14134,25 @@
       <c r="A11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="34">
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="24">
         <v>1</v>
       </c>
-      <c r="K11" s="34">
+      <c r="K11" s="24">
         <v>1</v>
       </c>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
       <c r="Q11" s="9">
         <v>2</v>
       </c>
@@ -13920,23 +14161,23 @@
       <c r="A12" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="32">
+      <c r="B12" s="25"/>
+      <c r="C12" s="22">
         <v>1</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="33"/>
-      <c r="P12" s="33"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
       <c r="Q12" s="9">
         <v>1</v>
       </c>
@@ -13945,25 +14186,25 @@
       <c r="A13" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35">
+      <c r="B13" s="25"/>
+      <c r="C13" s="25">
         <v>1</v>
       </c>
-      <c r="D13" s="33"/>
-      <c r="E13" s="34">
+      <c r="D13" s="23"/>
+      <c r="E13" s="24">
         <v>1</v>
       </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="33"/>
-      <c r="P13" s="33"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
       <c r="Q13" s="9">
         <v>2</v>
       </c>
@@ -13972,23 +14213,23 @@
       <c r="A14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="35"/>
-      <c r="C14" s="32">
+      <c r="B14" s="25"/>
+      <c r="C14" s="22">
         <v>1</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="33"/>
-      <c r="N14" s="33"/>
-      <c r="O14" s="33"/>
-      <c r="P14" s="33"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
       <c r="Q14" s="9">
         <v>1</v>
       </c>
@@ -13997,23 +14238,23 @@
       <c r="A15" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="31">
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="21">
         <v>1</v>
       </c>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="33"/>
-      <c r="O15" s="33"/>
-      <c r="P15" s="33"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
       <c r="Q15" s="9">
         <v>1</v>
       </c>
@@ -14022,23 +14263,23 @@
       <c r="A16" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="34">
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="24">
         <v>1</v>
       </c>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
       <c r="Q16" s="9">
         <v>1</v>
       </c>
@@ -14047,25 +14288,25 @@
       <c r="A17" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35">
+      <c r="B17" s="25"/>
+      <c r="C17" s="25">
         <v>1</v>
       </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="34">
+      <c r="D17" s="23"/>
+      <c r="E17" s="24">
         <v>1</v>
       </c>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="33"/>
-      <c r="O17" s="33"/>
-      <c r="P17" s="33"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
       <c r="Q17" s="9">
         <v>2</v>
       </c>
@@ -14074,48 +14315,48 @@
       <c r="A18" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="32">
+      <c r="B18" s="25"/>
+      <c r="C18" s="22">
         <v>1</v>
       </c>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
-      <c r="N18" s="33"/>
-      <c r="O18" s="33"/>
-      <c r="P18" s="33"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
       <c r="Q18" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="34">
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="28">
         <v>1</v>
       </c>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33"/>
-      <c r="O19" s="33"/>
-      <c r="P19" s="33"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
       <c r="Q19" s="9">
         <v>1</v>
       </c>
@@ -14124,23 +14365,23 @@
       <c r="A20" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="34">
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="24">
         <v>1</v>
       </c>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
-      <c r="P20" s="33"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
       <c r="Q20" s="9">
         <v>1</v>
       </c>
@@ -14149,25 +14390,25 @@
       <c r="A21" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="36">
+      <c r="B21" s="25"/>
+      <c r="C21" s="26">
         <v>1</v>
       </c>
-      <c r="D21" s="33"/>
-      <c r="E21" s="34">
+      <c r="D21" s="23"/>
+      <c r="E21" s="24">
         <v>1</v>
       </c>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="33"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="23"/>
       <c r="Q21" s="9">
         <v>2</v>
       </c>
@@ -14179,20 +14420,20 @@
       <c r="B22" s="7">
         <v>1</v>
       </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
       <c r="Q22" s="9">
         <v>1</v>
       </c>
@@ -14201,23 +14442,23 @@
       <c r="A23" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="34">
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="24">
         <v>1</v>
       </c>
-      <c r="O23" s="33"/>
-      <c r="P23" s="33"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
       <c r="Q23" s="9">
         <v>1</v>
       </c>
@@ -14226,23 +14467,23 @@
       <c r="A24" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="34">
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="24">
         <v>1</v>
       </c>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
-      <c r="O24" s="33"/>
-      <c r="P24" s="33"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
       <c r="Q24" s="9">
         <v>1</v>
       </c>
@@ -14251,23 +14492,23 @@
       <c r="A25" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="34">
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="24">
         <v>1</v>
       </c>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="33"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="33"/>
-      <c r="O25" s="33"/>
-      <c r="P25" s="33"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
       <c r="Q25" s="9">
         <v>1</v>
       </c>
@@ -14276,23 +14517,23 @@
       <c r="A26" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="34">
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="24">
         <v>1</v>
       </c>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
-      <c r="N26" s="33"/>
-      <c r="O26" s="33"/>
-      <c r="P26" s="33"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
       <c r="Q26" s="9">
         <v>1</v>
       </c>
@@ -14301,23 +14542,23 @@
       <c r="A27" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="34">
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24">
         <v>1</v>
       </c>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
-      <c r="N27" s="33"/>
-      <c r="O27" s="33"/>
-      <c r="P27" s="33"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
       <c r="Q27" s="9">
         <v>1</v>
       </c>
@@ -14326,23 +14567,23 @@
       <c r="A28" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="34">
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="24">
         <v>1</v>
       </c>
-      <c r="M28" s="33"/>
-      <c r="N28" s="33"/>
-      <c r="O28" s="33"/>
-      <c r="P28" s="33"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
       <c r="Q28" s="9">
         <v>1</v>
       </c>
@@ -14351,23 +14592,23 @@
       <c r="A29" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="34">
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="24">
         <v>1</v>
       </c>
-      <c r="M29" s="33"/>
-      <c r="N29" s="33"/>
-      <c r="O29" s="33"/>
-      <c r="P29" s="33"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
       <c r="Q29" s="9">
         <v>1</v>
       </c>
@@ -14376,25 +14617,25 @@
       <c r="A30" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="34">
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="24">
         <v>1</v>
       </c>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="34">
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="24">
         <v>1</v>
       </c>
-      <c r="L30" s="33"/>
-      <c r="M30" s="33"/>
-      <c r="N30" s="33"/>
-      <c r="O30" s="33"/>
-      <c r="P30" s="33"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
       <c r="Q30" s="9">
         <v>2</v>
       </c>
@@ -14403,23 +14644,23 @@
       <c r="A31" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="35"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="34">
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="24">
         <v>1</v>
       </c>
-      <c r="J31" s="33"/>
-      <c r="K31" s="33"/>
-      <c r="L31" s="33"/>
-      <c r="M31" s="33"/>
-      <c r="N31" s="33"/>
-      <c r="O31" s="33"/>
-      <c r="P31" s="33"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23"/>
+      <c r="L31" s="23"/>
+      <c r="M31" s="23"/>
+      <c r="N31" s="23"/>
+      <c r="O31" s="23"/>
+      <c r="P31" s="23"/>
       <c r="Q31" s="9">
         <v>1</v>
       </c>
@@ -14428,23 +14669,23 @@
       <c r="A32" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B32" s="35"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="33"/>
-      <c r="K32" s="33"/>
-      <c r="L32" s="34">
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="24">
         <v>1</v>
       </c>
-      <c r="M32" s="33"/>
-      <c r="N32" s="33"/>
-      <c r="O32" s="33"/>
-      <c r="P32" s="33"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
       <c r="Q32" s="9">
         <v>1</v>
       </c>
@@ -14453,23 +14694,23 @@
       <c r="A33" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="B33" s="35"/>
-      <c r="C33" s="36">
+      <c r="B33" s="25"/>
+      <c r="C33" s="26">
         <v>1</v>
       </c>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="33"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="33"/>
-      <c r="N33" s="33"/>
-      <c r="O33" s="33"/>
-      <c r="P33" s="33"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="23"/>
       <c r="Q33" s="9">
         <v>1</v>
       </c>
@@ -14478,23 +14719,23 @@
       <c r="A34" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="35"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="33"/>
-      <c r="K34" s="33"/>
-      <c r="L34" s="33"/>
-      <c r="M34" s="34">
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="24">
         <v>1</v>
       </c>
-      <c r="N34" s="33"/>
-      <c r="O34" s="33"/>
-      <c r="P34" s="33"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="23"/>
+      <c r="P34" s="23"/>
       <c r="Q34" s="9">
         <v>1</v>
       </c>
@@ -14503,23 +14744,23 @@
       <c r="A35" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="35"/>
-      <c r="C35" s="35"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="34">
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="24">
         <v>1</v>
       </c>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="33"/>
-      <c r="J35" s="33"/>
-      <c r="K35" s="33"/>
-      <c r="L35" s="33"/>
-      <c r="M35" s="33"/>
-      <c r="N35" s="33"/>
-      <c r="O35" s="33"/>
-      <c r="P35" s="33"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="23"/>
+      <c r="N35" s="23"/>
+      <c r="O35" s="23"/>
+      <c r="P35" s="23"/>
       <c r="Q35" s="9">
         <v>1</v>
       </c>
@@ -14528,48 +14769,48 @@
       <c r="A36" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="35"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="34">
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="24">
         <v>1</v>
       </c>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="33"/>
-      <c r="I36" s="33"/>
-      <c r="J36" s="33"/>
-      <c r="K36" s="33"/>
-      <c r="L36" s="33"/>
-      <c r="M36" s="33"/>
-      <c r="N36" s="33"/>
-      <c r="O36" s="33"/>
-      <c r="P36" s="33"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="23"/>
+      <c r="M36" s="23"/>
+      <c r="N36" s="23"/>
+      <c r="O36" s="23"/>
+      <c r="P36" s="23"/>
       <c r="Q36" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A37" s="12" t="s">
+      <c r="A37" s="27" t="s">
         <v>255</v>
       </c>
-      <c r="B37" s="35"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="33"/>
-      <c r="H37" s="34">
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="28">
         <v>1</v>
       </c>
-      <c r="I37" s="33"/>
-      <c r="J37" s="33"/>
-      <c r="K37" s="33"/>
-      <c r="L37" s="33"/>
-      <c r="M37" s="33"/>
-      <c r="N37" s="33"/>
-      <c r="O37" s="33"/>
-      <c r="P37" s="33"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="23"/>
+      <c r="K37" s="23"/>
+      <c r="L37" s="23"/>
+      <c r="M37" s="23"/>
+      <c r="N37" s="23"/>
+      <c r="O37" s="23"/>
+      <c r="P37" s="23"/>
       <c r="Q37" s="9">
         <v>1</v>
       </c>
@@ -14578,23 +14819,23 @@
       <c r="A38" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B38" s="35"/>
-      <c r="C38" s="35"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="33"/>
-      <c r="J38" s="33"/>
-      <c r="K38" s="33"/>
-      <c r="L38" s="33"/>
-      <c r="M38" s="33"/>
-      <c r="N38" s="34">
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="23"/>
+      <c r="K38" s="23"/>
+      <c r="L38" s="23"/>
+      <c r="M38" s="23"/>
+      <c r="N38" s="24">
         <v>1</v>
       </c>
-      <c r="O38" s="33"/>
-      <c r="P38" s="33"/>
+      <c r="O38" s="23"/>
+      <c r="P38" s="23"/>
       <c r="Q38" s="9">
         <v>1</v>
       </c>
@@ -14603,25 +14844,25 @@
       <c r="A39" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="B39" s="35"/>
-      <c r="C39" s="36">
+      <c r="B39" s="25"/>
+      <c r="C39" s="26">
         <v>1</v>
       </c>
-      <c r="D39" s="33"/>
-      <c r="E39" s="34">
+      <c r="D39" s="23"/>
+      <c r="E39" s="24">
         <v>1</v>
       </c>
-      <c r="F39" s="33"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="33"/>
-      <c r="J39" s="33"/>
-      <c r="K39" s="33"/>
-      <c r="L39" s="33"/>
-      <c r="M39" s="33"/>
-      <c r="N39" s="33"/>
-      <c r="O39" s="33"/>
-      <c r="P39" s="33"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="23"/>
+      <c r="L39" s="23"/>
+      <c r="M39" s="23"/>
+      <c r="N39" s="23"/>
+      <c r="O39" s="23"/>
+      <c r="P39" s="23"/>
       <c r="Q39" s="9">
         <v>2</v>
       </c>
@@ -14630,23 +14871,23 @@
       <c r="A40" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B40" s="35"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="34">
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="24">
         <v>1</v>
       </c>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="33"/>
-      <c r="J40" s="33"/>
-      <c r="K40" s="33"/>
-      <c r="L40" s="33"/>
-      <c r="M40" s="33"/>
-      <c r="N40" s="33"/>
-      <c r="O40" s="33"/>
-      <c r="P40" s="33"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="23"/>
+      <c r="K40" s="23"/>
+      <c r="L40" s="23"/>
+      <c r="M40" s="23"/>
+      <c r="N40" s="23"/>
+      <c r="O40" s="23"/>
+      <c r="P40" s="23"/>
       <c r="Q40" s="9">
         <v>1</v>
       </c>
@@ -14655,50 +14896,50 @@
       <c r="A41" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B41" s="35"/>
-      <c r="C41" s="36">
+      <c r="B41" s="25"/>
+      <c r="C41" s="26">
         <v>1</v>
       </c>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="33"/>
-      <c r="I41" s="33"/>
-      <c r="J41" s="33"/>
-      <c r="K41" s="33"/>
-      <c r="L41" s="33"/>
-      <c r="M41" s="33"/>
-      <c r="N41" s="33"/>
-      <c r="O41" s="33"/>
-      <c r="P41" s="33"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="23"/>
+      <c r="K41" s="23"/>
+      <c r="L41" s="23"/>
+      <c r="M41" s="23"/>
+      <c r="N41" s="23"/>
+      <c r="O41" s="23"/>
+      <c r="P41" s="23"/>
       <c r="Q41" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="B42" s="35"/>
-      <c r="C42" s="35"/>
-      <c r="D42" s="34">
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="28">
         <v>1</v>
       </c>
-      <c r="E42" s="33"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="34">
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="28">
         <v>1</v>
       </c>
-      <c r="H42" s="33"/>
-      <c r="I42" s="33"/>
-      <c r="J42" s="33"/>
-      <c r="K42" s="33"/>
-      <c r="L42" s="33"/>
-      <c r="M42" s="33"/>
-      <c r="N42" s="33"/>
-      <c r="O42" s="33"/>
-      <c r="P42" s="8">
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
+      <c r="J42" s="23"/>
+      <c r="K42" s="23"/>
+      <c r="L42" s="23"/>
+      <c r="M42" s="23"/>
+      <c r="N42" s="23"/>
+      <c r="O42" s="23"/>
+      <c r="P42" s="28">
         <v>1</v>
       </c>
       <c r="Q42" s="9">
@@ -14815,22 +15056,22 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="30" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="32" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="24"/>
+      <c r="C5" s="35"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
@@ -14880,10 +15121,10 @@
       <c r="A10" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="38" t="s">
         <v>407</v>
       </c>
     </row>
@@ -14891,26 +15132,26 @@
       <c r="A11" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="28"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="39"/>
     </row>
     <row r="12" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="30" t="s">
         <v>115</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="32" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="24"/>
+      <c r="C13" s="35"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
@@ -14946,22 +15187,22 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="30" t="s">
         <v>122</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="32" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="24"/>
+      <c r="C18" s="35"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
@@ -14986,22 +15227,22 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="36" t="s">
         <v>131</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="38" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
+      <c r="A22" s="37"/>
       <c r="B22" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="28"/>
+      <c r="C22" s="39"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
@@ -15073,10 +15314,10 @@
       <c r="A29" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="32" t="s">
         <v>407</v>
       </c>
     </row>
@@ -15084,33 +15325,33 @@
       <c r="A30" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="30"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="33"/>
     </row>
     <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="22"/>
-      <c r="C31" s="24"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="35"/>
     </row>
     <row r="32" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="36" t="s">
         <v>65</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="27" t="s">
+      <c r="C32" s="38" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
+      <c r="A33" s="37"/>
       <c r="B33" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="28"/>
+      <c r="C33" s="39"/>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
@@ -15190,22 +15431,22 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="25" t="s">
+      <c r="A41" s="36" t="s">
         <v>166</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="27" t="s">
+      <c r="C41" s="38" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
+      <c r="A42" s="37"/>
       <c r="B42" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="28"/>
+      <c r="C42" s="39"/>
     </row>
     <row r="43" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
@@ -15230,29 +15471,29 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="21" t="s">
+      <c r="A45" s="30" t="s">
         <v>87</v>
       </c>
       <c r="B45" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C45" s="23" t="s">
+      <c r="C45" s="32" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="29"/>
+      <c r="A46" s="31"/>
       <c r="B46" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="30"/>
+      <c r="C46" s="33"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="29"/>
+      <c r="A47" s="31"/>
       <c r="B47" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="30"/>
+      <c r="C47" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="18">
@@ -15262,18 +15503,18 @@
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="A41:A42"/>
     <mergeCell ref="C41:C42"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="C21:C22"/>
     <mergeCell ref="A45:A47"/>
     <mergeCell ref="C45:C47"/>
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="C29:C31"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="C21:C22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://cpicpgx.org/guidelines/guideline-for-abacavir-and-hla-b/"/>

</xml_diff>

<commit_message>
Minor fix for 99999-fk4d79nq4z; Updated cpicpairs.xlsx
</commit_message>
<xml_diff>
--- a/cpicPairs.xlsx
+++ b/cpicPairs.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1726" uniqueCount="413">
   <si>
     <t>Gene</t>
   </si>
@@ -1250,6 +1250,21 @@
   </si>
   <si>
     <t>guideline</t>
+  </si>
+  <si>
+    <t>HLA-B*5801</t>
+  </si>
+  <si>
+    <t>HLA-B*57:01</t>
+  </si>
+  <si>
+    <t>HLA-A*31:01 &amp; HLA-B*15:02</t>
+  </si>
+  <si>
+    <t>HLA-B*15:02</t>
+  </si>
+  <si>
+    <t>HLA-B*15:02 &amp; CYP2C9</t>
   </si>
 </sst>
 </file>
@@ -1883,16 +1898,10 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1908,6 +1917,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -13798,10 +13813,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q43"/>
+  <dimension ref="A1:S43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R39" sqref="R39"/>
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -13809,9 +13824,9 @@
     <col min="1" max="1" width="17.875" style="13" customWidth="1"/>
     <col min="2" max="3" width="9.125" style="4" customWidth="1"/>
     <col min="4" max="16" width="9.125" style="5" customWidth="1"/>
-    <col min="17" max="17" width="11.375" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5" customWidth="1"/>
-    <col min="19" max="19" width="5.875" customWidth="1"/>
+    <col min="17" max="17" width="11.375" style="6" customWidth="1"/>
+    <col min="18" max="18" width="3" customWidth="1"/>
+    <col min="19" max="19" width="46.375" customWidth="1"/>
     <col min="20" max="20" width="6" customWidth="1"/>
     <col min="21" max="21" width="8.75" customWidth="1"/>
     <col min="22" max="22" width="5.75" customWidth="1"/>
@@ -13909,7 +13924,7 @@
     <col min="130" max="130" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
@@ -13917,7 +13932,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>405</v>
       </c>
@@ -13925,7 +13940,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>401</v>
       </c>
@@ -13978,7 +13993,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
@@ -14002,8 +14017,11 @@
       <c r="Q5" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>14</v>
       </c>
@@ -14027,8 +14045,11 @@
       <c r="Q6" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S6" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>18</v>
       </c>
@@ -14055,7 +14076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>24</v>
       </c>
@@ -14080,7 +14101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>27</v>
       </c>
@@ -14105,7 +14126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
         <v>32</v>
       </c>
@@ -14130,7 +14151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>36</v>
       </c>
@@ -14156,8 +14177,11 @@
       <c r="Q11" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S11" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>92</v>
       </c>
@@ -14182,7 +14206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>115</v>
       </c>
@@ -14209,7 +14233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>38</v>
       </c>
@@ -14234,7 +14258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>41</v>
       </c>
@@ -14259,7 +14283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>117</v>
       </c>
@@ -14284,7 +14308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>122</v>
       </c>
@@ -14311,7 +14335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>93</v>
       </c>
@@ -14336,7 +14360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="s">
         <v>47</v>
       </c>
@@ -14361,7 +14385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>48</v>
       </c>
@@ -14386,7 +14410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>131</v>
       </c>
@@ -14413,7 +14437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>54</v>
       </c>
@@ -14438,7 +14462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>56</v>
       </c>
@@ -14463,7 +14487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>57</v>
       </c>
@@ -14488,7 +14512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>58</v>
       </c>
@@ -14513,7 +14537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>61</v>
       </c>
@@ -14537,8 +14561,11 @@
       <c r="Q26" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S26" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>63</v>
       </c>
@@ -14563,7 +14590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>95</v>
       </c>
@@ -14588,7 +14615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>97</v>
       </c>
@@ -14613,7 +14640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>65</v>
       </c>
@@ -14639,8 +14666,11 @@
       <c r="Q30" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S30" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>68</v>
       </c>
@@ -14665,7 +14695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>98</v>
       </c>
@@ -15067,11 +15097,11 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
+      <c r="A5" s="31"/>
       <c r="B5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="35"/>
+      <c r="C5" s="33"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
@@ -15121,10 +15151,10 @@
       <c r="A10" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="36" t="s">
         <v>407</v>
       </c>
     </row>
@@ -15132,8 +15162,8 @@
       <c r="A11" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="39"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="37"/>
     </row>
     <row r="12" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A12" s="30" t="s">
@@ -15147,11 +15177,11 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
+      <c r="A13" s="31"/>
       <c r="B13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="35"/>
+      <c r="C13" s="33"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
@@ -15198,11 +15228,11 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="35"/>
+      <c r="C18" s="33"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
@@ -15227,22 +15257,22 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="34" t="s">
         <v>131</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="36" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="39"/>
+      <c r="C22" s="37"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
@@ -15325,33 +15355,33 @@
       <c r="A30" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="33"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="39"/>
     </row>
     <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="35"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="33"/>
     </row>
     <row r="32" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="34" t="s">
         <v>65</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="36" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
+      <c r="A33" s="35"/>
       <c r="B33" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="39"/>
+      <c r="C33" s="37"/>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
@@ -15431,22 +15461,22 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="36" t="s">
+      <c r="A41" s="34" t="s">
         <v>166</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="38" t="s">
+      <c r="C41" s="36" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="37"/>
+      <c r="A42" s="35"/>
       <c r="B42" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="39"/>
+      <c r="C42" s="37"/>
     </row>
     <row r="43" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
@@ -15482,21 +15512,27 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="31"/>
+      <c r="A46" s="38"/>
       <c r="B46" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="33"/>
+      <c r="C46" s="39"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="31"/>
+      <c r="A47" s="38"/>
       <c r="B47" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="33"/>
+      <c r="C47" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="C32:C33"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B10:B11"/>
@@ -15509,12 +15545,6 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="C32:C33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://cpicpgx.org/guidelines/guideline-for-abacavir-and-hla-b/"/>

</xml_diff>

<commit_message>
Created the KO for amitriptyline (CYP2C19 and CYP2D6); Updated cpicPairs.xlsx
</commit_message>
<xml_diff>
--- a/cpicPairs.xlsx
+++ b/cpicPairs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14115" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20085" windowHeight="9615" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="cpicPairs" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -1840,7 +1840,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1923,16 +1923,10 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1949,6 +1943,15 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1996,7 +1999,56 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="58">
+  <dxfs count="65">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -6011,7 +6063,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -6134,7 +6186,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -6374,7 +6426,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:Q43" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField axis="axisCol" showAll="0">
@@ -6951,8 +7003,8 @@
   <dataFields count="1">
     <dataField name="Count of Guideline" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="58">
-    <format dxfId="57">
+  <formats count="65">
+    <format dxfId="64">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14" selected="0">
@@ -6974,13 +7026,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="56">
+    <format dxfId="63">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="55">
+    <format dxfId="62">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="54">
+    <format dxfId="61">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14">
@@ -7002,10 +7054,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="53">
+    <format dxfId="60">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="52">
+    <format dxfId="59">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14" selected="0">
@@ -7027,13 +7079,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="51">
+    <format dxfId="58">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="50">
+    <format dxfId="57">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="49">
+    <format dxfId="56">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14">
@@ -7055,10 +7107,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="48">
+    <format dxfId="55">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="54">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7067,17 +7119,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="46">
+    <format dxfId="53">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="45">
+    <format dxfId="52">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="44">
+    <format dxfId="51">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7086,7 +7138,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="43">
+    <format dxfId="50">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7095,17 +7147,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="42">
+    <format dxfId="49">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="41">
+    <format dxfId="48">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="40">
+    <format dxfId="47">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7114,7 +7166,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="39">
+    <format dxfId="46">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7123,17 +7175,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="45">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="37">
+    <format dxfId="44">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="36">
+    <format dxfId="43">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7142,16 +7194,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="35">
+    <format dxfId="42">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="34">
+    <format dxfId="41">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="40">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="32">
+    <format dxfId="39">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="38">
@@ -7197,10 +7249,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="38">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="30">
+    <format dxfId="37">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7212,7 +7264,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="36">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7224,7 +7276,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="35">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7236,7 +7288,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="34">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7248,7 +7300,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
+    <format dxfId="33">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7260,7 +7312,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="32">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7272,7 +7324,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="24">
+    <format dxfId="31">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7284,7 +7336,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="23">
+    <format dxfId="30">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7312,7 +7364,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="29">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7343,7 +7395,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="28">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7391,7 +7443,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="27">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7405,7 +7457,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
+    <format dxfId="26">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7450,7 +7502,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="25">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="12" selected="0">
@@ -7510,7 +7562,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="24">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7522,7 +7574,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="23">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7534,7 +7586,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="22">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7546,7 +7598,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="21">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7558,7 +7610,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="20">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7570,7 +7622,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7579,7 +7631,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7588,7 +7640,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7597,7 +7649,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="16">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7606,7 +7658,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="15">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7618,7 +7670,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="14">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7630,7 +7682,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="13">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7642,7 +7694,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="12">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7654,7 +7706,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="11">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7666,7 +7718,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="10">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7678,7 +7730,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7687,7 +7739,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7696,11 +7748,77 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
             <x v="123"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="42"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="45"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="47"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="72"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="0">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="64"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -13841,7 +13959,7 @@
   <dimension ref="A1:S43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S32" sqref="S32"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -14019,7 +14137,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="41" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="25"/>
@@ -14031,7 +14149,7 @@
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
       <c r="J5" s="23"/>
-      <c r="K5" s="24">
+      <c r="K5" s="21">
         <v>1</v>
       </c>
       <c r="L5" s="23"/>
@@ -14105,7 +14223,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="41" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="25"/>
@@ -14219,7 +14337,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="41" t="s">
         <v>92</v>
       </c>
       <c r="B12" s="25"/>
@@ -14277,7 +14395,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="41" t="s">
         <v>38</v>
       </c>
       <c r="B14" s="25"/>
@@ -14305,7 +14423,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="41" t="s">
         <v>41</v>
       </c>
       <c r="B15" s="25"/>
@@ -14391,7 +14509,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="41" t="s">
         <v>93</v>
       </c>
       <c r="B18" s="25"/>
@@ -15155,7 +15273,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="74" orientation="landscape" r:id="rId2"/>
+  <pageSetup scale="57" orientation="landscape" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -15221,11 +15339,11 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="34"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
@@ -15275,10 +15393,10 @@
       <c r="A10" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="37" t="s">
         <v>407</v>
       </c>
     </row>
@@ -15286,8 +15404,8 @@
       <c r="A11" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="40"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="38"/>
     </row>
     <row r="12" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
@@ -15301,11 +15419,11 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="36"/>
+      <c r="C13" s="34"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
@@ -15352,11 +15470,11 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="36"/>
+      <c r="C18" s="34"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
@@ -15381,22 +15499,22 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="35" t="s">
         <v>131</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="39" t="s">
+      <c r="C21" s="37" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
+      <c r="A22" s="36"/>
       <c r="B22" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="40"/>
+      <c r="C22" s="38"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
@@ -15479,33 +15597,33 @@
       <c r="A30" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="32"/>
-      <c r="C30" s="34"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="40"/>
     </row>
     <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="35"/>
-      <c r="C31" s="36"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="34"/>
     </row>
     <row r="32" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="35" t="s">
         <v>65</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="39" t="s">
+      <c r="C32" s="37" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="38"/>
+      <c r="A33" s="36"/>
       <c r="B33" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="40"/>
+      <c r="C33" s="38"/>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
@@ -15585,22 +15703,22 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="37" t="s">
+      <c r="A41" s="35" t="s">
         <v>166</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="39" t="s">
+      <c r="C41" s="37" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="38"/>
+      <c r="A42" s="36"/>
       <c r="B42" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="40"/>
+      <c r="C42" s="38"/>
     </row>
     <row r="43" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
@@ -15636,21 +15754,27 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="32"/>
+      <c r="A46" s="39"/>
       <c r="B46" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="34"/>
+      <c r="C46" s="40"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="32"/>
+      <c r="A47" s="39"/>
       <c r="B47" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="34"/>
+      <c r="C47" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="C32:C33"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B10:B11"/>
@@ -15663,12 +15787,6 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="C32:C33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://cpicpgx.org/guidelines/guideline-for-abacavir-and-hla-b/"/>

</xml_diff>

<commit_message>
Create allopurinol recommendation KO and test; Updated druglist KO. Updated cpicPairs.xlsx
</commit_message>
<xml_diff>
--- a/cpicPairs.xlsx
+++ b/cpicPairs.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KgridObjRepo\cpic-objects\"/>
@@ -20,13 +20,13 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1759" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1780" uniqueCount="429">
   <si>
     <t>Gene</t>
   </si>
@@ -1283,6 +1283,36 @@
   </si>
   <si>
     <t>G6PD WHO Class</t>
+  </si>
+  <si>
+    <t>/99999/fk45m7fn9t/v0.0.1</t>
+  </si>
+  <si>
+    <t>/99999/fk4d79nq4z/v0.0.5</t>
+  </si>
+  <si>
+    <t>/99999/fk4d22836k/v0.0.5</t>
+  </si>
+  <si>
+    <t>/99999/fk4bz6hp15/v0.0.5</t>
+  </si>
+  <si>
+    <t>/99999/fk4mc97w6m/v0.0.5</t>
+  </si>
+  <si>
+    <t>/99999/fk4d22836l/v0.0.5</t>
+  </si>
+  <si>
+    <t>/99999/fk4t167482/v0.0.1</t>
+  </si>
+  <si>
+    <t>P&amp;P</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>TCA</t>
   </si>
 </sst>
 </file>
@@ -1920,13 +1950,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1943,15 +1982,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1999,7 +2029,21 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="65">
+  <dxfs count="67">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -6063,7 +6107,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -6186,7 +6230,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -6426,7 +6470,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:Q43" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField axis="axisCol" showAll="0">
@@ -7003,8 +7047,8 @@
   <dataFields count="1">
     <dataField name="Count of Guideline" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="65">
-    <format dxfId="64">
+  <formats count="67">
+    <format dxfId="66">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14" selected="0">
@@ -7026,13 +7070,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="63">
+    <format dxfId="65">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="62">
+    <format dxfId="64">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="61">
+    <format dxfId="63">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14">
@@ -7054,10 +7098,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="60">
+    <format dxfId="62">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="59">
+    <format dxfId="61">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14" selected="0">
@@ -7079,13 +7123,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="58">
+    <format dxfId="60">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="57">
+    <format dxfId="59">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="56">
+    <format dxfId="58">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14">
@@ -7107,10 +7151,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="55">
+    <format dxfId="57">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="54">
+    <format dxfId="56">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7119,17 +7163,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="53">
+    <format dxfId="55">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="52">
+    <format dxfId="54">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="51">
+    <format dxfId="53">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7138,7 +7182,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="50">
+    <format dxfId="52">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7147,17 +7191,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="49">
+    <format dxfId="51">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="48">
+    <format dxfId="50">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="49">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7166,7 +7210,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="46">
+    <format dxfId="48">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7175,17 +7219,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="45">
+    <format dxfId="47">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="44">
+    <format dxfId="46">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="45">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7194,16 +7238,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="42">
+    <format dxfId="44">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="43">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="40">
+    <format dxfId="42">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="39">
+    <format dxfId="41">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="38">
@@ -7249,10 +7293,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="40">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="37">
+    <format dxfId="39">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7264,7 +7308,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="36">
+    <format dxfId="38">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7276,7 +7320,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="35">
+    <format dxfId="37">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7288,7 +7332,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="34">
+    <format dxfId="36">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7300,7 +7344,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="33">
+    <format dxfId="35">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7312,7 +7356,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="34">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7324,7 +7368,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="33">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7336,7 +7380,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="32">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7364,7 +7408,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="31">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7395,7 +7439,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="30">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7443,7 +7487,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="29">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7457,7 +7501,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
+    <format dxfId="28">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7502,7 +7546,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="27">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="12" selected="0">
@@ -7562,7 +7606,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="24">
+    <format dxfId="26">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7574,7 +7618,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="23">
+    <format dxfId="25">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7586,7 +7630,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="24">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7598,7 +7642,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="23">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7610,7 +7654,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="22">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7622,7 +7666,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7631,7 +7675,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7640,7 +7684,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7649,11 +7693,35 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
             <x v="221"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="17">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="43"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="25"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="16">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="43"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="80"/>
           </reference>
         </references>
       </pivotArea>
@@ -7665,36 +7733,12 @@
             <x v="43"/>
           </reference>
           <reference field="1" count="1">
-            <x v="25"/>
+            <x v="201"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="14">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="43"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="80"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="13">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="43"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="201"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="12">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7706,7 +7750,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="13">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7718,7 +7762,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="12">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7730,7 +7774,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7739,7 +7783,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7748,7 +7792,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7757,7 +7801,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7766,7 +7810,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7775,7 +7819,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7784,7 +7828,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="5">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7793,7 +7837,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7802,7 +7846,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7811,7 +7855,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="2">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7819,6 +7863,27 @@
           </reference>
           <reference field="1" count="1">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="0">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="44"/>
           </reference>
         </references>
       </pivotArea>
@@ -13956,10 +14021,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -13968,10 +14033,10 @@
     <col min="2" max="3" width="9.125" style="4" customWidth="1"/>
     <col min="4" max="16" width="9.125" style="5" customWidth="1"/>
     <col min="17" max="17" width="11.375" style="6" customWidth="1"/>
-    <col min="18" max="18" width="3" customWidth="1"/>
-    <col min="19" max="19" width="46.375" customWidth="1"/>
-    <col min="20" max="20" width="6" customWidth="1"/>
-    <col min="21" max="21" width="8.75" customWidth="1"/>
+    <col min="18" max="18" width="1.25" customWidth="1"/>
+    <col min="19" max="19" width="27.375" customWidth="1"/>
+    <col min="20" max="20" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5.75" customWidth="1"/>
     <col min="23" max="24" width="6" customWidth="1"/>
     <col min="25" max="25" width="8.5" customWidth="1"/>
@@ -14067,7 +14132,7 @@
     <col min="130" max="130" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
@@ -14075,7 +14140,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>405</v>
       </c>
@@ -14083,7 +14148,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>401</v>
       </c>
@@ -14136,8 +14201,8 @@
         <v>403</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="41" t="s">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" s="31" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="25"/>
@@ -14163,8 +14228,14 @@
       <c r="S5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T5" t="s">
+        <v>419</v>
+      </c>
+      <c r="U5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>14</v>
       </c>
@@ -14192,8 +14263,8 @@
         <v>408</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" s="31" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="25"/>
@@ -14221,9 +14292,18 @@
       <c r="S7" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="41" t="s">
+      <c r="T7" t="s">
+        <v>425</v>
+      </c>
+      <c r="U7" t="s">
+        <v>426</v>
+      </c>
+      <c r="V7" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" s="31" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="25"/>
@@ -14249,8 +14329,14 @@
       <c r="S8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T8" t="s">
+        <v>420</v>
+      </c>
+      <c r="U8" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>27</v>
       </c>
@@ -14278,7 +14364,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
         <v>32</v>
       </c>
@@ -14305,8 +14391,9 @@
       <c r="S10" s="30" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T10" s="30"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>36</v>
       </c>
@@ -14336,8 +14423,8 @@
         <v>410</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="41" t="s">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A12" s="31" t="s">
         <v>92</v>
       </c>
       <c r="B12" s="25"/>
@@ -14363,13 +14450,19 @@
       <c r="S12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T12" t="s">
+        <v>421</v>
+      </c>
+      <c r="U12" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>115</v>
       </c>
       <c r="B13" s="25"/>
-      <c r="C13" s="25">
+      <c r="C13" s="26">
         <v>1</v>
       </c>
       <c r="D13" s="23"/>
@@ -14393,9 +14486,12 @@
       <c r="S13" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="41" t="s">
+      <c r="V13" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14" s="31" t="s">
         <v>38</v>
       </c>
       <c r="B14" s="25"/>
@@ -14421,9 +14517,15 @@
       <c r="S14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="41" t="s">
+      <c r="T14" t="s">
+        <v>422</v>
+      </c>
+      <c r="U14" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15" s="31" t="s">
         <v>41</v>
       </c>
       <c r="B15" s="25"/>
@@ -14449,8 +14551,14 @@
       <c r="S15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T15" t="s">
+        <v>423</v>
+      </c>
+      <c r="U15" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>117</v>
       </c>
@@ -14477,8 +14585,11 @@
       <c r="S16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="V16" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>122</v>
       </c>
@@ -14507,9 +14618,12 @@
       <c r="S17" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A18" s="41" t="s">
+      <c r="V17" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A18" s="31" t="s">
         <v>93</v>
       </c>
       <c r="B18" s="25"/>
@@ -14535,8 +14649,14 @@
       <c r="S18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T18" t="s">
+        <v>424</v>
+      </c>
+      <c r="U18" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="s">
         <v>47</v>
       </c>
@@ -14563,8 +14683,9 @@
       <c r="S19" s="30" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T19" s="30"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>48</v>
       </c>
@@ -14592,7 +14713,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>131</v>
       </c>
@@ -14621,8 +14742,11 @@
       <c r="S21" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="V21" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>54</v>
       </c>
@@ -14650,7 +14774,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>56</v>
       </c>
@@ -14678,7 +14802,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>57</v>
       </c>
@@ -14705,8 +14829,11 @@
       <c r="S24" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="V24" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>58</v>
       </c>
@@ -14734,7 +14861,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>61</v>
       </c>
@@ -14762,7 +14889,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>63</v>
       </c>
@@ -14790,7 +14917,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>95</v>
       </c>
@@ -14818,7 +14945,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>97</v>
       </c>
@@ -14846,7 +14973,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>65</v>
       </c>
@@ -14876,7 +15003,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>68</v>
       </c>
@@ -14904,7 +15031,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>98</v>
       </c>
@@ -14932,7 +15059,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>160</v>
       </c>
@@ -14960,7 +15087,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>72</v>
       </c>
@@ -14988,7 +15115,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>77</v>
       </c>
@@ -15016,7 +15143,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>79</v>
       </c>
@@ -15044,7 +15171,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" s="27" t="s">
         <v>255</v>
       </c>
@@ -15071,8 +15198,9 @@
       <c r="S37" s="30" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T37" s="30"/>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>81</v>
       </c>
@@ -15100,7 +15228,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>166</v>
       </c>
@@ -15129,8 +15257,11 @@
       <c r="S39" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="V39" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>84</v>
       </c>
@@ -15158,7 +15289,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>85</v>
       </c>
@@ -15186,7 +15317,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" s="27" t="s">
         <v>87</v>
       </c>
@@ -15217,8 +15348,9 @@
       <c r="S42" s="30" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T42" s="30"/>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>403</v>
       </c>
@@ -15328,22 +15460,22 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="32" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="34" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="34"/>
+      <c r="C5" s="37"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
@@ -15393,10 +15525,10 @@
       <c r="A10" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="40" t="s">
         <v>407</v>
       </c>
     </row>
@@ -15404,26 +15536,26 @@
       <c r="A11" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="38"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="41"/>
     </row>
     <row r="12" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="32" t="s">
         <v>115</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="34" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="34"/>
+      <c r="C13" s="37"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
@@ -15459,22 +15591,22 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="32" t="s">
         <v>122</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="34" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="34"/>
+      <c r="C18" s="37"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
@@ -15499,22 +15631,22 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="38" t="s">
         <v>131</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="40" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="36"/>
+      <c r="A22" s="39"/>
       <c r="B22" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="38"/>
+      <c r="C22" s="41"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
@@ -15586,10 +15718,10 @@
       <c r="A29" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="33" t="s">
+      <c r="C29" s="34" t="s">
         <v>407</v>
       </c>
     </row>
@@ -15597,33 +15729,33 @@
       <c r="A30" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="35"/>
     </row>
     <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="32"/>
-      <c r="C31" s="34"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="37"/>
     </row>
     <row r="32" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="38" t="s">
         <v>65</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="40" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="36"/>
+      <c r="A33" s="39"/>
       <c r="B33" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="38"/>
+      <c r="C33" s="41"/>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
@@ -15703,22 +15835,22 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="38" t="s">
         <v>166</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="37" t="s">
+      <c r="C41" s="40" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="36"/>
+      <c r="A42" s="39"/>
       <c r="B42" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="38"/>
+      <c r="C42" s="41"/>
     </row>
     <row r="43" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
@@ -15743,38 +15875,32 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="31" t="s">
+      <c r="A45" s="32" t="s">
         <v>87</v>
       </c>
       <c r="B45" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C45" s="33" t="s">
+      <c r="C45" s="34" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="39"/>
+      <c r="A46" s="33"/>
       <c r="B46" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="40"/>
+      <c r="C46" s="35"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="39"/>
+      <c r="A47" s="33"/>
       <c r="B47" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="40"/>
+      <c r="C47" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="C32:C33"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B10:B11"/>
@@ -15787,6 +15913,12 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="C21:C22"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="C32:C33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://cpicpgx.org/guidelines/guideline-for-abacavir-and-hla-b/"/>

</xml_diff>

<commit_message>
Created oxcarbazepine recommendation KO and test; Updated other diplotype-based rec KOs; Updated cpicPairs.xlsx; Updated druglist;
</commit_message>
<xml_diff>
--- a/cpicPairs.xlsx
+++ b/cpicPairs.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1780" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1786" uniqueCount="433">
   <si>
     <t>Gene</t>
   </si>
@@ -1313,13 +1313,25 @@
   </si>
   <si>
     <t>TCA</t>
+  </si>
+  <si>
+    <t>Implications</t>
+  </si>
+  <si>
+    <t>naïve or not</t>
+  </si>
+  <si>
+    <t>/99999/fk4qc17m5z/v0.0.1</t>
+  </si>
+  <si>
+    <t>/99999/fk4058s74p/v0.0.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1444,8 +1456,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="39">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1661,6 +1679,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -1870,7 +1894,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1956,16 +1980,10 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1982,6 +2000,30 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2029,7 +2071,147 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="67">
+  <dxfs count="87">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -7047,8 +7229,8 @@
   <dataFields count="1">
     <dataField name="Count of Guideline" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="67">
-    <format dxfId="66">
+  <formats count="87">
+    <format dxfId="86">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14" selected="0">
@@ -7070,13 +7252,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="65">
+    <format dxfId="85">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="64">
+    <format dxfId="84">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="63">
+    <format dxfId="83">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14">
@@ -7098,10 +7280,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="62">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="61">
+    <format dxfId="81">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14" selected="0">
@@ -7123,13 +7305,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="60">
+    <format dxfId="80">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="59">
+    <format dxfId="79">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="58">
+    <format dxfId="78">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14">
@@ -7151,10 +7333,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="57">
+    <format dxfId="77">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="56">
+    <format dxfId="76">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7163,17 +7345,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="55">
+    <format dxfId="75">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="54">
+    <format dxfId="74">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="53">
+    <format dxfId="73">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7182,7 +7364,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="52">
+    <format dxfId="72">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7191,17 +7373,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="51">
+    <format dxfId="71">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="50">
+    <format dxfId="70">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="49">
+    <format dxfId="69">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7210,7 +7392,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="48">
+    <format dxfId="68">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7219,17 +7401,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="47">
+    <format dxfId="67">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="46">
+    <format dxfId="66">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="45">
+    <format dxfId="65">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7238,16 +7420,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="44">
+    <format dxfId="64">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="63">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="62">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="61">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="38">
@@ -7293,10 +7475,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="40">
+    <format dxfId="60">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="39">
+    <format dxfId="59">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7308,7 +7490,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="58">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7320,7 +7502,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="37">
+    <format dxfId="57">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7332,7 +7514,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="36">
+    <format dxfId="56">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7344,7 +7526,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="35">
+    <format dxfId="55">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7356,7 +7538,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="34">
+    <format dxfId="54">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7368,7 +7550,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="33">
+    <format dxfId="53">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7380,7 +7562,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="52">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7408,7 +7590,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="51">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7439,7 +7621,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="50">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7487,7 +7669,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="49">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7501,7 +7683,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="48">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7546,7 +7728,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="47">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="12" selected="0">
@@ -7606,7 +7788,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
+    <format dxfId="46">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7618,7 +7800,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="45">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7630,7 +7812,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="24">
+    <format dxfId="44">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7642,7 +7824,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="23">
+    <format dxfId="43">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7654,7 +7836,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="42">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7666,7 +7848,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="41">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7675,7 +7857,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="40">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7684,7 +7866,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
+    <format dxfId="39">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7693,7 +7875,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="38">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7702,7 +7884,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="37">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7714,7 +7896,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="36">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7726,7 +7908,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="35">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7738,7 +7920,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="34">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7750,7 +7932,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="33">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7762,7 +7944,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="32">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7774,7 +7956,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7783,7 +7965,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7792,7 +7974,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="29">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7801,7 +7983,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="28">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7810,7 +7992,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="27">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7819,7 +8001,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="26">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7828,7 +8010,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="25">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7837,7 +8019,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="24">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7846,7 +8028,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="23">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7855,7 +8037,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="22">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7867,11 +8049,212 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
             <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="20">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="44"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="19">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="18">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="39"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="17">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="16">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="15">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="14">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="42"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="13">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="45"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="12">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="47"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="11">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="72"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="10">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="64"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="39"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="64"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="147"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="147"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="147"/>
           </reference>
         </references>
       </pivotArea>
@@ -7883,7 +8266,7 @@
             <x v="36"/>
           </reference>
           <reference field="1" count="1">
-            <x v="44"/>
+            <x v="65"/>
           </reference>
         </references>
       </pivotArea>
@@ -14021,10 +14404,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V43"/>
+  <dimension ref="A1:W43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -14038,7 +14421,8 @@
     <col min="20" max="20" width="23.625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="4.625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5.75" customWidth="1"/>
-    <col min="23" max="24" width="6" customWidth="1"/>
+    <col min="23" max="23" width="28.125" customWidth="1"/>
+    <col min="24" max="24" width="6" customWidth="1"/>
     <col min="25" max="25" width="8.5" customWidth="1"/>
     <col min="26" max="26" width="9" customWidth="1"/>
     <col min="27" max="27" width="6.625" customWidth="1"/>
@@ -14132,7 +14516,7 @@
     <col min="130" max="130" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
@@ -14140,7 +14524,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>405</v>
       </c>
@@ -14148,7 +14532,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>401</v>
       </c>
@@ -14201,7 +14585,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
         <v>8</v>
       </c>
@@ -14222,21 +14606,23 @@
       <c r="N5" s="23"/>
       <c r="O5" s="23"/>
       <c r="P5" s="23"/>
-      <c r="Q5" s="9">
+      <c r="Q5" s="42">
         <v>1</v>
       </c>
-      <c r="S5" t="s">
+      <c r="S5" s="44" t="s">
         <v>409</v>
       </c>
-      <c r="T5" t="s">
+      <c r="T5" s="44" t="s">
         <v>419</v>
       </c>
-      <c r="U5" t="s">
+      <c r="U5" s="44" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="V5" s="44"/>
+      <c r="W5" s="44"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" s="31" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="25"/>
@@ -14248,7 +14634,7 @@
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
-      <c r="K6" s="24">
+      <c r="K6" s="21">
         <v>1</v>
       </c>
       <c r="L6" s="23"/>
@@ -14256,23 +14642,31 @@
       <c r="N6" s="23"/>
       <c r="O6" s="23"/>
       <c r="P6" s="23"/>
-      <c r="Q6" s="9">
+      <c r="Q6" s="42">
         <v>1</v>
       </c>
-      <c r="S6" t="s">
+      <c r="S6" s="44" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
+      <c r="T6" s="44" t="s">
+        <v>432</v>
+      </c>
+      <c r="U6" s="44" t="s">
+        <v>293</v>
+      </c>
+      <c r="V6" s="44"/>
+      <c r="W6" s="44"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" s="46" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="25"/>
-      <c r="C7" s="26">
+      <c r="C7" s="49">
         <v>1</v>
       </c>
       <c r="D7" s="23"/>
-      <c r="E7" s="24">
+      <c r="E7" s="48">
         <v>1</v>
       </c>
       <c r="F7" s="23"/>
@@ -14286,23 +14680,26 @@
       <c r="N7" s="23"/>
       <c r="O7" s="23"/>
       <c r="P7" s="23"/>
-      <c r="Q7" s="9">
+      <c r="Q7" s="47">
         <v>2</v>
       </c>
-      <c r="S7" t="s">
+      <c r="S7" s="43" t="s">
         <v>413</v>
       </c>
-      <c r="T7" t="s">
+      <c r="T7" s="43" t="s">
         <v>425</v>
       </c>
-      <c r="U7" t="s">
+      <c r="U7" s="43" t="s">
         <v>426</v>
       </c>
-      <c r="V7" t="s">
+      <c r="V7" s="43" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W7" s="43" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="s">
         <v>24</v>
       </c>
@@ -14323,20 +14720,22 @@
         <v>1</v>
       </c>
       <c r="P8" s="23"/>
-      <c r="Q8" s="9">
+      <c r="Q8" s="42">
         <v>1</v>
       </c>
-      <c r="S8" t="s">
+      <c r="S8" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="T8" t="s">
+      <c r="T8" s="44" t="s">
         <v>420</v>
       </c>
-      <c r="U8" t="s">
+      <c r="U8" s="44" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="V8" s="44"/>
+      <c r="W8" s="44"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>27</v>
       </c>
@@ -14364,7 +14763,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
         <v>32</v>
       </c>
@@ -14388,12 +14787,15 @@
       <c r="Q10" s="9">
         <v>1</v>
       </c>
-      <c r="S10" s="30" t="s">
+      <c r="S10" s="45" t="s">
         <v>415</v>
       </c>
       <c r="T10" s="30"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="U10" s="30"/>
+      <c r="V10" s="30"/>
+      <c r="W10" s="30"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>36</v>
       </c>
@@ -14423,7 +14825,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
         <v>92</v>
       </c>
@@ -14444,20 +14846,22 @@
       <c r="N12" s="23"/>
       <c r="O12" s="23"/>
       <c r="P12" s="23"/>
-      <c r="Q12" s="9">
+      <c r="Q12" s="42">
         <v>1</v>
       </c>
-      <c r="S12" t="s">
+      <c r="S12" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="T12" t="s">
+      <c r="T12" s="44" t="s">
         <v>421</v>
       </c>
-      <c r="U12" t="s">
+      <c r="U12" s="44" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="V12" s="44"/>
+      <c r="W12" s="44"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>115</v>
       </c>
@@ -14490,7 +14894,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
         <v>38</v>
       </c>
@@ -14511,20 +14915,22 @@
       <c r="N14" s="23"/>
       <c r="O14" s="23"/>
       <c r="P14" s="23"/>
-      <c r="Q14" s="9">
+      <c r="Q14" s="42">
         <v>1</v>
       </c>
-      <c r="S14" t="s">
+      <c r="S14" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="T14" t="s">
+      <c r="T14" s="44" t="s">
         <v>422</v>
       </c>
-      <c r="U14" t="s">
+      <c r="U14" s="44" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="V14" s="44"/>
+      <c r="W14" s="44"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="31" t="s">
         <v>41</v>
       </c>
@@ -14545,20 +14951,22 @@
       <c r="N15" s="23"/>
       <c r="O15" s="23"/>
       <c r="P15" s="23"/>
-      <c r="Q15" s="9">
+      <c r="Q15" s="42">
         <v>1</v>
       </c>
-      <c r="S15" t="s">
+      <c r="S15" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="T15" t="s">
+      <c r="T15" s="44" t="s">
         <v>423</v>
       </c>
-      <c r="U15" t="s">
+      <c r="U15" s="44" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="V15" s="44"/>
+      <c r="W15" s="44"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>117</v>
       </c>
@@ -14589,12 +14997,12 @@
         <v>428</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>122</v>
       </c>
       <c r="B17" s="25"/>
-      <c r="C17" s="25">
+      <c r="C17" s="26">
         <v>1</v>
       </c>
       <c r="D17" s="23"/>
@@ -14622,7 +15030,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="31" t="s">
         <v>93</v>
       </c>
@@ -14643,20 +15051,22 @@
       <c r="N18" s="23"/>
       <c r="O18" s="23"/>
       <c r="P18" s="23"/>
-      <c r="Q18" s="9">
+      <c r="Q18" s="42">
         <v>1</v>
       </c>
-      <c r="S18" t="s">
+      <c r="S18" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="T18" t="s">
+      <c r="T18" s="44" t="s">
         <v>424</v>
       </c>
-      <c r="U18" t="s">
+      <c r="U18" s="44" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="V18" s="44"/>
+      <c r="W18" s="44"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="s">
         <v>47</v>
       </c>
@@ -14680,12 +15090,15 @@
       <c r="Q19" s="9">
         <v>1</v>
       </c>
-      <c r="S19" s="30" t="s">
+      <c r="S19" s="45" t="s">
         <v>415</v>
       </c>
       <c r="T19" s="30"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="U19" s="30"/>
+      <c r="V19" s="30"/>
+      <c r="W19" s="30"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>48</v>
       </c>
@@ -14713,7 +15126,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>131</v>
       </c>
@@ -14746,7 +15159,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>54</v>
       </c>
@@ -14774,7 +15187,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>56</v>
       </c>
@@ -14802,7 +15215,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>57</v>
       </c>
@@ -14833,7 +15246,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>58</v>
       </c>
@@ -14861,8 +15274,8 @@
         <v>417</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A26" s="12" t="s">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A26" s="46" t="s">
         <v>61</v>
       </c>
       <c r="B26" s="25"/>
@@ -14874,7 +15287,7 @@
       <c r="H26" s="23"/>
       <c r="I26" s="23"/>
       <c r="J26" s="23"/>
-      <c r="K26" s="24">
+      <c r="K26" s="48">
         <v>1</v>
       </c>
       <c r="L26" s="23"/>
@@ -14882,14 +15295,24 @@
       <c r="N26" s="23"/>
       <c r="O26" s="23"/>
       <c r="P26" s="23"/>
-      <c r="Q26" s="9">
+      <c r="Q26" s="47">
         <v>1</v>
       </c>
-      <c r="S26" t="s">
+      <c r="S26" s="43" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="T26" s="43" t="s">
+        <v>431</v>
+      </c>
+      <c r="U26" s="43" t="s">
+        <v>293</v>
+      </c>
+      <c r="V26" s="43"/>
+      <c r="W26" s="43" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>63</v>
       </c>
@@ -14917,7 +15340,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>95</v>
       </c>
@@ -14945,7 +15368,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>97</v>
       </c>
@@ -14973,7 +15396,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>65</v>
       </c>
@@ -15003,7 +15426,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>68</v>
       </c>
@@ -15031,7 +15454,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>98</v>
       </c>
@@ -15059,7 +15482,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>160</v>
       </c>
@@ -15087,7 +15510,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>72</v>
       </c>
@@ -15115,7 +15538,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>77</v>
       </c>
@@ -15143,7 +15566,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>79</v>
       </c>
@@ -15171,7 +15594,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" s="27" t="s">
         <v>255</v>
       </c>
@@ -15195,12 +15618,15 @@
       <c r="Q37" s="9">
         <v>1</v>
       </c>
-      <c r="S37" s="30" t="s">
+      <c r="S37" s="45" t="s">
         <v>415</v>
       </c>
       <c r="T37" s="30"/>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="U37" s="30"/>
+      <c r="V37" s="30"/>
+      <c r="W37" s="30"/>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>81</v>
       </c>
@@ -15228,7 +15654,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>166</v>
       </c>
@@ -15261,7 +15687,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>84</v>
       </c>
@@ -15289,7 +15715,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>85</v>
       </c>
@@ -15317,7 +15743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42" s="27" t="s">
         <v>87</v>
       </c>
@@ -15345,12 +15771,15 @@
       <c r="Q42" s="9">
         <v>3</v>
       </c>
-      <c r="S42" s="30" t="s">
+      <c r="S42" s="45" t="s">
         <v>416</v>
       </c>
       <c r="T42" s="30"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="U42" s="30"/>
+      <c r="V42" s="30"/>
+      <c r="W42" s="30"/>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>403</v>
       </c>
@@ -15471,11 +15900,11 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="37"/>
+      <c r="C5" s="35"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
@@ -15525,10 +15954,10 @@
       <c r="A10" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="38" t="s">
         <v>407</v>
       </c>
     </row>
@@ -15536,8 +15965,8 @@
       <c r="A11" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="41"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="39"/>
     </row>
     <row r="12" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
@@ -15551,11 +15980,11 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="37"/>
+      <c r="C13" s="35"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
@@ -15602,11 +16031,11 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="36"/>
+      <c r="A18" s="33"/>
       <c r="B18" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="37"/>
+      <c r="C18" s="35"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
@@ -15631,22 +16060,22 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="36" t="s">
         <v>131</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="40" t="s">
+      <c r="C21" s="38" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="39"/>
+      <c r="A22" s="37"/>
       <c r="B22" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="41"/>
+      <c r="C22" s="39"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
@@ -15729,33 +16158,33 @@
       <c r="A30" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="35"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="41"/>
     </row>
     <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="37"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="35"/>
     </row>
     <row r="32" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="36" t="s">
         <v>65</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="38" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="39"/>
+      <c r="A33" s="37"/>
       <c r="B33" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="41"/>
+      <c r="C33" s="39"/>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
@@ -15835,22 +16264,22 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="38" t="s">
+      <c r="A41" s="36" t="s">
         <v>166</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="40" t="s">
+      <c r="C41" s="38" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="39"/>
+      <c r="A42" s="37"/>
       <c r="B42" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="41"/>
+      <c r="C42" s="39"/>
     </row>
     <row r="43" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
@@ -15886,21 +16315,27 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="33"/>
+      <c r="A46" s="40"/>
       <c r="B46" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="35"/>
+      <c r="C46" s="41"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="33"/>
+      <c r="A47" s="40"/>
       <c r="B47" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="35"/>
+      <c r="C47" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="C32:C33"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B10:B11"/>
@@ -15913,12 +16348,6 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="C32:C33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://cpicpgx.org/guidelines/guideline-for-abacavir-and-hla-b/"/>

</xml_diff>

<commit_message>
Create ondansetron and tropisetron recommendation KOs and tests; Updated druglist
</commit_message>
<xml_diff>
--- a/cpicPairs.xlsx
+++ b/cpicPairs.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1786" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="452">
   <si>
     <t>Gene</t>
   </si>
@@ -1325,6 +1325,63 @@
   </si>
   <si>
     <t>/99999/fk4058s74p/v0.0.1</t>
+  </si>
+  <si>
+    <t>Genotype</t>
+  </si>
+  <si>
+    <t>Mapping</t>
+  </si>
+  <si>
+    <t>Phenotype</t>
+  </si>
+  <si>
+    <t>functional</t>
+  </si>
+  <si>
+    <t>*allele</t>
+  </si>
+  <si>
+    <t>metabolizer</t>
+  </si>
+  <si>
+    <t>pos/neg</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>xlsx</t>
+  </si>
+  <si>
+    <t>WHO class</t>
+  </si>
+  <si>
+    <t>nonstar allele</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>marker</t>
+  </si>
+  <si>
+    <t>phenotype</t>
+  </si>
+  <si>
+    <t>simple table</t>
+  </si>
+  <si>
+    <t>need activity score and specific allele</t>
+  </si>
+  <si>
+    <t>/99999/fk4c83hw23/v0.0.1</t>
+  </si>
+  <si>
+    <t>/99999/fk4fn2d721/v0.0.1</t>
   </si>
 </sst>
 </file>
@@ -1463,7 +1520,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1685,6 +1742,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -1894,7 +1957,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2011,6 +2074,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2023,6 +2087,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2071,7 +2149,81 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="87">
+  <dxfs count="99">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.249977111117893"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.249977111117893"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.249977111117893"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.249977111117893"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.249977111117893"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -6642,6 +6794,53 @@
   <dataFields count="1">
     <dataField name="Count of Guideline" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
+  <formats count="5">
+    <format dxfId="11">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="42"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="10">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="42"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="123"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="123"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea dataOnly="0" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="43"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -7229,8 +7428,8 @@
   <dataFields count="1">
     <dataField name="Count of Guideline" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="87">
-    <format dxfId="86">
+  <formats count="94">
+    <format dxfId="98">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14" selected="0">
@@ -7252,13 +7451,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="85">
+    <format dxfId="97">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="84">
+    <format dxfId="96">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="83">
+    <format dxfId="95">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14">
@@ -7280,10 +7479,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="94">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="81">
+    <format dxfId="93">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14" selected="0">
@@ -7305,13 +7504,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
+    <format dxfId="92">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="79">
+    <format dxfId="91">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="78">
+    <format dxfId="90">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14">
@@ -7333,10 +7532,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="89">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="76">
+    <format dxfId="88">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7345,17 +7544,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="87">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="86">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="73">
+    <format dxfId="85">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7364,7 +7563,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="72">
+    <format dxfId="84">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7373,17 +7572,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="83">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
+    <format dxfId="82">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="69">
+    <format dxfId="81">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7392,7 +7591,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="80">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7401,17 +7600,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="67">
+    <format dxfId="79">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="66">
+    <format dxfId="78">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="65">
+    <format dxfId="77">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7420,16 +7619,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="64">
+    <format dxfId="76">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="63">
+    <format dxfId="75">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="62">
+    <format dxfId="74">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="61">
+    <format dxfId="73">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="38">
@@ -7475,10 +7674,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="60">
+    <format dxfId="72">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="59">
+    <format dxfId="71">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7490,7 +7689,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="58">
+    <format dxfId="70">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7502,7 +7701,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="57">
+    <format dxfId="69">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7514,7 +7713,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="56">
+    <format dxfId="68">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7526,7 +7725,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="55">
+    <format dxfId="67">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7538,7 +7737,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="54">
+    <format dxfId="66">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7550,7 +7749,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="53">
+    <format dxfId="65">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7562,7 +7761,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="52">
+    <format dxfId="64">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7590,7 +7789,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="51">
+    <format dxfId="63">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7621,7 +7820,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="50">
+    <format dxfId="62">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7669,7 +7868,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="49">
+    <format dxfId="61">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7683,7 +7882,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="48">
+    <format dxfId="60">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7728,7 +7927,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="47">
+    <format dxfId="59">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="12" selected="0">
@@ -7788,7 +7987,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="46">
+    <format dxfId="58">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7800,7 +7999,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="45">
+    <format dxfId="57">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7812,7 +8011,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="44">
+    <format dxfId="56">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7824,7 +8023,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="43">
+    <format dxfId="55">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7836,7 +8035,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="42">
+    <format dxfId="54">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7848,7 +8047,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="41">
+    <format dxfId="53">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7857,7 +8056,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="40">
+    <format dxfId="52">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7866,7 +8065,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="39">
+    <format dxfId="51">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7875,7 +8074,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="50">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7884,7 +8083,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="37">
+    <format dxfId="49">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7896,7 +8095,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="36">
+    <format dxfId="48">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7908,7 +8107,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="35">
+    <format dxfId="47">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7920,7 +8119,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="34">
+    <format dxfId="46">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7932,7 +8131,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="33">
+    <format dxfId="45">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7944,7 +8143,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="44">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7956,7 +8155,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="43">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7965,7 +8164,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="42">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7974,7 +8173,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="41">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7983,7 +8182,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="40">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -7992,7 +8191,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="39">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8001,7 +8200,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
+    <format dxfId="38">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8010,7 +8209,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="37">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8019,7 +8218,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="24">
+    <format dxfId="36">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8028,11 +8227,131 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="23">
+    <format dxfId="35">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="34">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="64"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="33">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="32">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="44"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="31">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="30">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="39"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="29">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="28">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="27">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="26">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="42"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="25">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="45"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="24">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="47"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="23">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="72"/>
           </reference>
         </references>
       </pivotArea>
@@ -8044,7 +8363,7 @@
             <x v="64"/>
           </reference>
           <reference field="1" count="1">
-            <x v="0"/>
+            <x v="5"/>
           </reference>
         </references>
       </pivotArea>
@@ -8053,24 +8372,51 @@
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="20">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="19">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
             <x v="7"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="36"/>
-          </reference>
+    <format dxfId="18">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
           <reference field="1" count="1">
-            <x v="44"/>
+            <x v="7"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
+    <format dxfId="17">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="39"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="16">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8082,50 +8428,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="15">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
-            <x v="39"/>
+            <x v="64"/>
           </reference>
           <reference field="1" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="17">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="16">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="15">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="14"/>
+            <x v="147"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="14">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="42"/>
+            <x v="147"/>
           </reference>
         </references>
       </pivotArea>
@@ -8134,73 +8453,28 @@
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="45"/>
+            <x v="147"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="12">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="47"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="11">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="72"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="10">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
-            <x v="64"/>
+            <x v="36"/>
           </reference>
           <reference field="1" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="9">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="8">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="7">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="7"/>
+            <x v="65"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="6">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="7"/>
+            <x v="144"/>
           </reference>
         </references>
       </pivotArea>
@@ -8212,40 +8486,37 @@
             <x v="39"/>
           </reference>
           <reference field="1" count="1">
-            <x v="7"/>
+            <x v="144"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="4">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="36"/>
-          </reference>
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
           <reference field="1" count="1">
-            <x v="7"/>
+            <x v="144"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="3">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="64"/>
-          </reference>
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
           <reference field="1" count="1">
-            <x v="147"/>
+            <x v="213"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="2">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="39"/>
+          </reference>
           <reference field="1" count="1">
-            <x v="147"/>
+            <x v="213"/>
           </reference>
         </references>
       </pivotArea>
@@ -8254,19 +8525,16 @@
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="147"/>
+            <x v="213"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="0">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="36"/>
-          </reference>
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
           <reference field="1" count="1">
-            <x v="65"/>
+            <x v="199"/>
           </reference>
         </references>
       </pivotArea>
@@ -14236,21 +14504,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="D3" sqref="D3:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.625" customWidth="1"/>
     <col min="2" max="2" width="28.125" customWidth="1"/>
-    <col min="3" max="21" width="99.625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.75" customWidth="1"/>
+    <col min="4" max="4" width="28.25" customWidth="1"/>
+    <col min="5" max="5" width="23.875" customWidth="1"/>
+    <col min="6" max="6" width="22.875" customWidth="1"/>
+    <col min="7" max="7" width="21.625" customWidth="1"/>
+    <col min="8" max="8" width="19.75" customWidth="1"/>
+    <col min="9" max="49" width="8.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -14258,135 +14531,263 @@
         <v>406</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>401</v>
       </c>
       <c r="B3" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>433</v>
+      </c>
+      <c r="E3" t="s">
+        <v>434</v>
+      </c>
+      <c r="F3" t="s">
+        <v>436</v>
+      </c>
+      <c r="G3" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>443</v>
+      </c>
+      <c r="E4" t="s">
+        <v>445</v>
+      </c>
+      <c r="F4" s="44"/>
+      <c r="G4" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>437</v>
+      </c>
+      <c r="E5" t="s">
+        <v>441</v>
+      </c>
+      <c r="F5" s="44"/>
+      <c r="G5" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>437</v>
+      </c>
+      <c r="E6" t="s">
+        <v>441</v>
+      </c>
+      <c r="F6" t="s">
+        <v>436</v>
+      </c>
+      <c r="G6" s="44"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>437</v>
+      </c>
+      <c r="E7" t="s">
+        <v>441</v>
+      </c>
+      <c r="F7" s="44"/>
+      <c r="G7" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="D8" t="s">
+        <v>437</v>
+      </c>
+      <c r="E8" t="s">
+        <v>441</v>
+      </c>
+      <c r="F8" t="s">
+        <v>436</v>
+      </c>
+      <c r="G8" s="44"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="52">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="52">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>440</v>
+      </c>
+      <c r="E11" t="s">
+        <v>441</v>
+      </c>
+      <c r="F11" s="44"/>
+      <c r="G11" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>437</v>
+      </c>
+      <c r="E12" t="s">
+        <v>439</v>
+      </c>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>437</v>
+      </c>
+      <c r="E13" t="s">
+        <v>439</v>
+      </c>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B14" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>446</v>
+      </c>
+      <c r="E14" t="s">
+        <v>448</v>
+      </c>
+      <c r="F14" s="44"/>
+      <c r="G14" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>437</v>
+      </c>
+      <c r="E15" t="s">
+        <v>441</v>
+      </c>
+      <c r="F15" t="s">
+        <v>436</v>
+      </c>
+      <c r="G15" s="44"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>437</v>
+      </c>
+      <c r="E16" t="s">
+        <v>441</v>
+      </c>
+      <c r="F16" t="s">
+        <v>436</v>
+      </c>
+      <c r="G16" s="44"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="D17" t="s">
+        <v>437</v>
+      </c>
+      <c r="E17" t="s">
+        <v>441</v>
+      </c>
+      <c r="F17" s="44"/>
+      <c r="G17" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="52">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>403</v>
       </c>
@@ -14396,6 +14797,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -14404,24 +14806,33 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W43"/>
+  <dimension ref="A1:W49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="T40" sqref="T40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.875" style="13" customWidth="1"/>
-    <col min="2" max="3" width="9.125" style="4" customWidth="1"/>
-    <col min="4" max="16" width="9.125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="12.375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="10.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="10.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.125" style="5" customWidth="1"/>
+    <col min="15" max="15" width="10.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.125" style="5" customWidth="1"/>
     <col min="17" max="17" width="11.375" style="6" customWidth="1"/>
     <col min="18" max="18" width="1.25" customWidth="1"/>
     <col min="19" max="19" width="27.375" customWidth="1"/>
     <col min="20" max="20" width="23.625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="4.625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5.75" customWidth="1"/>
-    <col min="23" max="23" width="28.125" customWidth="1"/>
+    <col min="23" max="23" width="32.625" customWidth="1"/>
     <col min="24" max="24" width="6" customWidth="1"/>
     <col min="25" max="25" width="8.5" customWidth="1"/>
     <col min="26" max="26" width="9" customWidth="1"/>
@@ -14609,17 +15020,17 @@
       <c r="Q5" s="42">
         <v>1</v>
       </c>
-      <c r="S5" s="44" t="s">
+      <c r="S5" s="45" t="s">
         <v>409</v>
       </c>
-      <c r="T5" s="44" t="s">
+      <c r="T5" s="45" t="s">
         <v>419</v>
       </c>
-      <c r="U5" s="44" t="s">
+      <c r="U5" s="45" t="s">
         <v>293</v>
       </c>
-      <c r="V5" s="44"/>
-      <c r="W5" s="44"/>
+      <c r="V5" s="45"/>
+      <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
@@ -14645,28 +15056,28 @@
       <c r="Q6" s="42">
         <v>1</v>
       </c>
-      <c r="S6" s="44" t="s">
+      <c r="S6" s="45" t="s">
         <v>408</v>
       </c>
-      <c r="T6" s="44" t="s">
+      <c r="T6" s="45" t="s">
         <v>432</v>
       </c>
-      <c r="U6" s="44" t="s">
+      <c r="U6" s="45" t="s">
         <v>293</v>
       </c>
-      <c r="V6" s="44"/>
-      <c r="W6" s="44"/>
+      <c r="V6" s="45"/>
+      <c r="W6" s="45"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="47" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="25"/>
-      <c r="C7" s="49">
+      <c r="C7" s="50">
         <v>1</v>
       </c>
       <c r="D7" s="23"/>
-      <c r="E7" s="48">
+      <c r="E7" s="49">
         <v>1</v>
       </c>
       <c r="F7" s="23"/>
@@ -14680,7 +15091,7 @@
       <c r="N7" s="23"/>
       <c r="O7" s="23"/>
       <c r="P7" s="23"/>
-      <c r="Q7" s="47">
+      <c r="Q7" s="48">
         <v>2</v>
       </c>
       <c r="S7" s="43" t="s">
@@ -14723,17 +15134,17 @@
       <c r="Q8" s="42">
         <v>1</v>
       </c>
-      <c r="S8" s="44" t="s">
+      <c r="S8" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="T8" s="44" t="s">
+      <c r="T8" s="45" t="s">
         <v>420</v>
       </c>
-      <c r="U8" s="44" t="s">
+      <c r="U8" s="45" t="s">
         <v>427</v>
       </c>
-      <c r="V8" s="44"/>
-      <c r="W8" s="44"/>
+      <c r="V8" s="45"/>
+      <c r="W8" s="45"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
@@ -14787,7 +15198,7 @@
       <c r="Q10" s="9">
         <v>1</v>
       </c>
-      <c r="S10" s="45" t="s">
+      <c r="S10" s="46" t="s">
         <v>415</v>
       </c>
       <c r="T10" s="30"/>
@@ -14849,17 +15260,17 @@
       <c r="Q12" s="42">
         <v>1</v>
       </c>
-      <c r="S12" s="44" t="s">
+      <c r="S12" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="T12" s="44" t="s">
+      <c r="T12" s="45" t="s">
         <v>421</v>
       </c>
-      <c r="U12" s="44" t="s">
+      <c r="U12" s="45" t="s">
         <v>427</v>
       </c>
-      <c r="V12" s="44"/>
-      <c r="W12" s="44"/>
+      <c r="V12" s="45"/>
+      <c r="W12" s="45"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
@@ -14918,17 +15329,17 @@
       <c r="Q14" s="42">
         <v>1</v>
       </c>
-      <c r="S14" s="44" t="s">
+      <c r="S14" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="T14" s="44" t="s">
+      <c r="T14" s="45" t="s">
         <v>422</v>
       </c>
-      <c r="U14" s="44" t="s">
+      <c r="U14" s="45" t="s">
         <v>427</v>
       </c>
-      <c r="V14" s="44"/>
-      <c r="W14" s="44"/>
+      <c r="V14" s="45"/>
+      <c r="W14" s="45"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="31" t="s">
@@ -14954,17 +15365,17 @@
       <c r="Q15" s="42">
         <v>1</v>
       </c>
-      <c r="S15" s="44" t="s">
+      <c r="S15" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="T15" s="44" t="s">
+      <c r="T15" s="45" t="s">
         <v>423</v>
       </c>
-      <c r="U15" s="44" t="s">
+      <c r="U15" s="45" t="s">
         <v>427</v>
       </c>
-      <c r="V15" s="44"/>
-      <c r="W15" s="44"/>
+      <c r="V15" s="45"/>
+      <c r="W15" s="45"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
@@ -15054,17 +15465,17 @@
       <c r="Q18" s="42">
         <v>1</v>
       </c>
-      <c r="S18" s="44" t="s">
+      <c r="S18" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="T18" s="44" t="s">
+      <c r="T18" s="45" t="s">
         <v>424</v>
       </c>
-      <c r="U18" s="44" t="s">
+      <c r="U18" s="45" t="s">
         <v>427</v>
       </c>
-      <c r="V18" s="44"/>
-      <c r="W18" s="44"/>
+      <c r="V18" s="45"/>
+      <c r="W18" s="45"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="s">
@@ -15090,7 +15501,7 @@
       <c r="Q19" s="9">
         <v>1</v>
       </c>
-      <c r="S19" s="45" t="s">
+      <c r="S19" s="46" t="s">
         <v>415</v>
       </c>
       <c r="T19" s="30"/>
@@ -15247,13 +15658,13 @@
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="31" t="s">
         <v>58</v>
       </c>
       <c r="B25" s="25"/>
       <c r="C25" s="25"/>
       <c r="D25" s="23"/>
-      <c r="E25" s="24">
+      <c r="E25" s="21">
         <v>1</v>
       </c>
       <c r="F25" s="23"/>
@@ -15267,15 +15678,23 @@
       <c r="N25" s="23"/>
       <c r="O25" s="23"/>
       <c r="P25" s="23"/>
-      <c r="Q25" s="9">
+      <c r="Q25" s="42">
         <v>1</v>
       </c>
-      <c r="S25" t="s">
+      <c r="S25" s="45" t="s">
         <v>417</v>
       </c>
+      <c r="T25" s="45" t="s">
+        <v>450</v>
+      </c>
+      <c r="U25" s="45" t="s">
+        <v>427</v>
+      </c>
+      <c r="V25" s="45"/>
+      <c r="W25" s="45"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A26" s="46" t="s">
+      <c r="A26" s="47" t="s">
         <v>61</v>
       </c>
       <c r="B26" s="25"/>
@@ -15287,7 +15706,7 @@
       <c r="H26" s="23"/>
       <c r="I26" s="23"/>
       <c r="J26" s="23"/>
-      <c r="K26" s="48">
+      <c r="K26" s="49">
         <v>1</v>
       </c>
       <c r="L26" s="23"/>
@@ -15295,7 +15714,7 @@
       <c r="N26" s="23"/>
       <c r="O26" s="23"/>
       <c r="P26" s="23"/>
-      <c r="Q26" s="47">
+      <c r="Q26" s="48">
         <v>1</v>
       </c>
       <c r="S26" s="43" t="s">
@@ -15567,7 +15986,7 @@
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="55" t="s">
         <v>79</v>
       </c>
       <c r="B36" s="25"/>
@@ -15590,8 +16009,14 @@
       <c r="Q36" s="9">
         <v>1</v>
       </c>
-      <c r="S36" t="s">
+      <c r="S36" s="54" t="s">
         <v>417</v>
+      </c>
+      <c r="T36" s="54"/>
+      <c r="U36" s="54"/>
+      <c r="V36" s="54"/>
+      <c r="W36" s="54" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.2">
@@ -15618,7 +16043,7 @@
       <c r="Q37" s="9">
         <v>1</v>
       </c>
-      <c r="S37" s="45" t="s">
+      <c r="S37" s="46" t="s">
         <v>415</v>
       </c>
       <c r="T37" s="30"/>
@@ -15688,13 +16113,13 @@
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="31" t="s">
         <v>84</v>
       </c>
       <c r="B40" s="25"/>
       <c r="C40" s="25"/>
       <c r="D40" s="23"/>
-      <c r="E40" s="24">
+      <c r="E40" s="21">
         <v>1</v>
       </c>
       <c r="F40" s="23"/>
@@ -15708,12 +16133,20 @@
       <c r="N40" s="23"/>
       <c r="O40" s="23"/>
       <c r="P40" s="23"/>
-      <c r="Q40" s="9">
+      <c r="Q40" s="42">
         <v>1</v>
       </c>
-      <c r="S40" t="s">
+      <c r="S40" s="45" t="s">
         <v>417</v>
       </c>
+      <c r="T40" s="45" t="s">
+        <v>451</v>
+      </c>
+      <c r="U40" s="45" t="s">
+        <v>427</v>
+      </c>
+      <c r="V40" s="45"/>
+      <c r="W40" s="45"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
@@ -15771,7 +16204,7 @@
       <c r="Q42" s="9">
         <v>3</v>
       </c>
-      <c r="S42" s="45" t="s">
+      <c r="S42" s="46" t="s">
         <v>416</v>
       </c>
       <c r="T42" s="30"/>
@@ -15831,6 +16264,154 @@
       <c r="Q43" s="9">
         <v>47</v>
       </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A46" s="13" t="s">
+        <v>433</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="G46" s="29"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="L46" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="M46" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="N46" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="O46" s="56" t="s">
+        <v>437</v>
+      </c>
+      <c r="P46" s="29"/>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A47" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="K47" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="L47" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="M47" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="N47" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="O47" s="56" t="s">
+        <v>441</v>
+      </c>
+      <c r="P47" s="29"/>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A48" s="13" t="s">
+        <v>436</v>
+      </c>
+      <c r="B48" s="53"/>
+      <c r="C48" s="53"/>
+      <c r="D48" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="E48" s="29"/>
+      <c r="F48" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="G48" s="29"/>
+      <c r="H48" s="29"/>
+      <c r="I48" s="29"/>
+      <c r="J48" s="29"/>
+      <c r="K48" s="29"/>
+      <c r="L48" s="29"/>
+      <c r="M48" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="N48" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="O48" s="29"/>
+      <c r="P48" s="29"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A49" s="13" t="s">
+        <v>435</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="D49" s="29"/>
+      <c r="E49" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="F49" s="29"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="J49" s="29"/>
+      <c r="K49" s="29"/>
+      <c r="L49" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="M49" s="29"/>
+      <c r="N49" s="29"/>
+      <c r="O49" s="56" t="s">
+        <v>438</v>
+      </c>
+      <c r="P49" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Refactored recommendation KOs to handle combination of dipltotype/phenotype to determine recommendations.
</commit_message>
<xml_diff>
--- a/cpicPairs.xlsx
+++ b/cpicPairs.xlsx
@@ -2040,36 +2040,6 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="14" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2102,6 +2072,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="14" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2198,31 +2198,6 @@
           <bgColor theme="9"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.249977111117893"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.249977111117893"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.249977111117893"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.249977111117893"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.249977111117893"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -2797,6 +2772,31 @@
     <dxf>
       <alignment horizontal="center" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.249977111117893"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.249977111117893"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.249977111117893"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.249977111117893"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.249977111117893"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -6795,7 +6795,7 @@
     <dataField name="Count of Guideline" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="11">
+    <format dxfId="98">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6804,7 +6804,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="97">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6813,7 +6813,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="96">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6822,7 +6822,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="95">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6831,7 +6831,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="94">
       <pivotArea dataOnly="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7429,59 +7429,6 @@
     <dataField name="Count of Guideline" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="94">
-    <format dxfId="98">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="14" selected="0">
-            <x v="36"/>
-            <x v="38"/>
-            <x v="39"/>
-            <x v="41"/>
-            <x v="42"/>
-            <x v="43"/>
-            <x v="54"/>
-            <x v="63"/>
-            <x v="64"/>
-            <x v="74"/>
-            <x v="108"/>
-            <x v="115"/>
-            <x v="118"/>
-            <x v="123"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="97">
-      <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="96">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="95">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="14">
-            <x v="36"/>
-            <x v="38"/>
-            <x v="39"/>
-            <x v="41"/>
-            <x v="42"/>
-            <x v="43"/>
-            <x v="54"/>
-            <x v="63"/>
-            <x v="64"/>
-            <x v="74"/>
-            <x v="108"/>
-            <x v="115"/>
-            <x v="118"/>
-            <x v="123"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="94">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
-    </format>
     <format dxfId="93">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
@@ -7538,23 +7485,76 @@
     <format dxfId="88">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
+          <reference field="0" count="14" selected="0">
+            <x v="36"/>
+            <x v="38"/>
+            <x v="39"/>
+            <x v="41"/>
+            <x v="42"/>
+            <x v="43"/>
+            <x v="54"/>
+            <x v="63"/>
+            <x v="64"/>
+            <x v="74"/>
+            <x v="108"/>
+            <x v="115"/>
+            <x v="118"/>
+            <x v="123"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="87">
+      <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="86">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="85">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="14">
+            <x v="36"/>
+            <x v="38"/>
+            <x v="39"/>
+            <x v="41"/>
+            <x v="42"/>
+            <x v="43"/>
+            <x v="54"/>
+            <x v="63"/>
+            <x v="64"/>
+            <x v="74"/>
+            <x v="108"/>
+            <x v="115"/>
+            <x v="118"/>
+            <x v="123"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="84">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="83">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
           <reference field="0" count="1" selected="0">
             <x v="22"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="81">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="85">
+    <format dxfId="80">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7563,7 +7563,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="84">
+    <format dxfId="79">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7572,17 +7572,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="78">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="77">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="81">
+    <format dxfId="76">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7591,7 +7591,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
+    <format dxfId="75">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7600,17 +7600,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="74">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="73">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="77">
+    <format dxfId="72">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7619,16 +7619,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="76">
+    <format dxfId="71">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="75">
+    <format dxfId="70">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="74">
+    <format dxfId="69">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="73">
+    <format dxfId="68">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="38">
@@ -7674,68 +7674,8 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="72">
+    <format dxfId="67">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="71">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="64"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="70">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="36"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="42"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="69">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="36"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="45"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="68">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="36"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="72"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="67">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="39"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="47"/>
-          </reference>
-        </references>
-      </pivotArea>
     </format>
     <format dxfId="66">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
@@ -7753,6 +7693,66 @@
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="42"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="64">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="45"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="63">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="72"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="62">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="39"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="47"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="61">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="64"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="60">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
             <x v="118"/>
           </reference>
           <reference field="1" count="1">
@@ -7761,7 +7761,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="64">
+    <format dxfId="59">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7789,7 +7789,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="63">
+    <format dxfId="58">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7820,7 +7820,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="62">
+    <format dxfId="57">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7868,7 +7868,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="61">
+    <format dxfId="56">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7882,7 +7882,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="60">
+    <format dxfId="55">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7927,7 +7927,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="59">
+    <format dxfId="54">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="12" selected="0">
@@ -7987,7 +7987,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="58">
+    <format dxfId="53">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7999,7 +7999,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="57">
+    <format dxfId="52">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8011,7 +8011,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="56">
+    <format dxfId="51">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8023,7 +8023,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="55">
+    <format dxfId="50">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8035,7 +8035,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="54">
+    <format dxfId="49">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8047,7 +8047,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="53">
+    <format dxfId="48">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8056,7 +8056,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="52">
+    <format dxfId="47">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8065,7 +8065,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="51">
+    <format dxfId="46">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8074,7 +8074,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="50">
+    <format dxfId="45">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8083,7 +8083,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="49">
+    <format dxfId="44">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8095,7 +8095,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="48">
+    <format dxfId="43">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8107,7 +8107,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="47">
+    <format dxfId="42">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8119,7 +8119,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="46">
+    <format dxfId="41">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8131,7 +8131,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="45">
+    <format dxfId="40">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8143,7 +8143,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="44">
+    <format dxfId="39">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8155,7 +8155,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="43">
+    <format dxfId="38">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -8164,7 +8164,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="42">
+    <format dxfId="37">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -8173,7 +8173,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="41">
+    <format dxfId="36">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -8182,7 +8182,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="40">
+    <format dxfId="35">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8191,7 +8191,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="39">
+    <format dxfId="34">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8200,7 +8200,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="33">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8209,7 +8209,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="37">
+    <format dxfId="32">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8218,7 +8218,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="36">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8227,7 +8227,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="35">
+    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8236,7 +8236,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="34">
+    <format dxfId="29">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8248,7 +8248,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="33">
+    <format dxfId="28">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8257,7 +8257,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="27">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8269,7 +8269,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="26">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8281,7 +8281,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="25">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8293,7 +8293,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="24">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8302,7 +8302,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="23">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8311,7 +8311,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="22">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8320,7 +8320,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
+    <format dxfId="21">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8329,7 +8329,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="20">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8338,7 +8338,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="24">
+    <format dxfId="19">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8347,7 +8347,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="23">
+    <format dxfId="18">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8356,7 +8356,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="17">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8368,7 +8368,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="16">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8377,7 +8377,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="15">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8386,7 +8386,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8395,7 +8395,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="13">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8404,7 +8404,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="12">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8416,7 +8416,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="11">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8428,7 +8428,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="10">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8440,7 +8440,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8449,7 +8449,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="8">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8458,7 +8458,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="7">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -14564,7 +14564,7 @@
       <c r="E4" t="s">
         <v>445</v>
       </c>
-      <c r="F4" s="44"/>
+      <c r="F4" s="34"/>
       <c r="G4" t="s">
         <v>444</v>
       </c>
@@ -14582,7 +14582,7 @@
       <c r="E5" t="s">
         <v>441</v>
       </c>
-      <c r="F5" s="44"/>
+      <c r="F5" s="34"/>
       <c r="G5" t="s">
         <v>438</v>
       </c>
@@ -14603,7 +14603,7 @@
       <c r="F6" t="s">
         <v>436</v>
       </c>
-      <c r="G6" s="44"/>
+      <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -14618,7 +14618,7 @@
       <c r="E7" t="s">
         <v>441</v>
       </c>
-      <c r="F7" s="44"/>
+      <c r="F7" s="34"/>
       <c r="G7" t="s">
         <v>438</v>
       </c>
@@ -14639,21 +14639,21 @@
       <c r="F8" t="s">
         <v>436</v>
       </c>
-      <c r="G8" s="44"/>
+      <c r="G8" s="34"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="52">
+      <c r="B9" s="42">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="52">
+      <c r="B10" s="42">
         <v>3</v>
       </c>
     </row>
@@ -14670,7 +14670,7 @@
       <c r="E11" t="s">
         <v>441</v>
       </c>
-      <c r="F11" s="44"/>
+      <c r="F11" s="34"/>
       <c r="G11" t="s">
         <v>442</v>
       </c>
@@ -14688,8 +14688,8 @@
       <c r="E12" t="s">
         <v>439</v>
       </c>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -14704,8 +14704,8 @@
       <c r="E13" t="s">
         <v>439</v>
       </c>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -14720,7 +14720,7 @@
       <c r="E14" t="s">
         <v>448</v>
       </c>
-      <c r="F14" s="44"/>
+      <c r="F14" s="34"/>
       <c r="G14" t="s">
         <v>447</v>
       </c>
@@ -14741,7 +14741,7 @@
       <c r="F15" t="s">
         <v>436</v>
       </c>
-      <c r="G15" s="44"/>
+      <c r="G15" s="34"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -14759,7 +14759,7 @@
       <c r="F16" t="s">
         <v>436</v>
       </c>
-      <c r="G16" s="44"/>
+      <c r="G16" s="34"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -14774,16 +14774,16 @@
       <c r="E17" t="s">
         <v>441</v>
       </c>
-      <c r="F17" s="44"/>
+      <c r="F17" s="34"/>
       <c r="G17" t="s">
         <v>438</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="51" t="s">
+      <c r="A18" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="52">
+      <c r="B18" s="42">
         <v>1</v>
       </c>
     </row>
@@ -14808,8 +14808,8 @@
   </sheetPr>
   <dimension ref="A1:W49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="T40" sqref="T40"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -15017,20 +15017,20 @@
       <c r="N5" s="23"/>
       <c r="O5" s="23"/>
       <c r="P5" s="23"/>
-      <c r="Q5" s="42">
+      <c r="Q5" s="32">
         <v>1</v>
       </c>
-      <c r="S5" s="45" t="s">
+      <c r="S5" s="35" t="s">
         <v>409</v>
       </c>
-      <c r="T5" s="45" t="s">
+      <c r="T5" s="35" t="s">
         <v>419</v>
       </c>
-      <c r="U5" s="45" t="s">
-        <v>293</v>
-      </c>
-      <c r="V5" s="45"/>
-      <c r="W5" s="45"/>
+      <c r="U5" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="V5" s="35"/>
+      <c r="W5" s="35"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
@@ -15053,31 +15053,31 @@
       <c r="N6" s="23"/>
       <c r="O6" s="23"/>
       <c r="P6" s="23"/>
-      <c r="Q6" s="42">
+      <c r="Q6" s="32">
         <v>1</v>
       </c>
-      <c r="S6" s="45" t="s">
+      <c r="S6" s="35" t="s">
         <v>408</v>
       </c>
-      <c r="T6" s="45" t="s">
+      <c r="T6" s="35" t="s">
         <v>432</v>
       </c>
-      <c r="U6" s="45" t="s">
-        <v>293</v>
-      </c>
-      <c r="V6" s="45"/>
-      <c r="W6" s="45"/>
+      <c r="U6" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="V6" s="35"/>
+      <c r="W6" s="35"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="37" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="25"/>
-      <c r="C7" s="50">
+      <c r="C7" s="40">
         <v>1</v>
       </c>
       <c r="D7" s="23"/>
-      <c r="E7" s="49">
+      <c r="E7" s="39">
         <v>1</v>
       </c>
       <c r="F7" s="23"/>
@@ -15091,22 +15091,22 @@
       <c r="N7" s="23"/>
       <c r="O7" s="23"/>
       <c r="P7" s="23"/>
-      <c r="Q7" s="48">
+      <c r="Q7" s="38">
         <v>2</v>
       </c>
-      <c r="S7" s="43" t="s">
+      <c r="S7" s="33" t="s">
         <v>413</v>
       </c>
-      <c r="T7" s="43" t="s">
+      <c r="T7" s="33" t="s">
         <v>425</v>
       </c>
-      <c r="U7" s="43" t="s">
+      <c r="U7" s="33" t="s">
         <v>426</v>
       </c>
-      <c r="V7" s="43" t="s">
+      <c r="V7" s="33" t="s">
         <v>428</v>
       </c>
-      <c r="W7" s="43" t="s">
+      <c r="W7" s="33" t="s">
         <v>429</v>
       </c>
     </row>
@@ -15131,20 +15131,20 @@
         <v>1</v>
       </c>
       <c r="P8" s="23"/>
-      <c r="Q8" s="42">
+      <c r="Q8" s="32">
         <v>1</v>
       </c>
-      <c r="S8" s="45" t="s">
+      <c r="S8" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="T8" s="45" t="s">
+      <c r="T8" s="35" t="s">
         <v>420</v>
       </c>
-      <c r="U8" s="45" t="s">
+      <c r="U8" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="V8" s="45"/>
-      <c r="W8" s="45"/>
+      <c r="V8" s="35"/>
+      <c r="W8" s="35"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
@@ -15198,7 +15198,7 @@
       <c r="Q10" s="9">
         <v>1</v>
       </c>
-      <c r="S10" s="46" t="s">
+      <c r="S10" s="36" t="s">
         <v>415</v>
       </c>
       <c r="T10" s="30"/>
@@ -15257,20 +15257,20 @@
       <c r="N12" s="23"/>
       <c r="O12" s="23"/>
       <c r="P12" s="23"/>
-      <c r="Q12" s="42">
+      <c r="Q12" s="32">
         <v>1</v>
       </c>
-      <c r="S12" s="45" t="s">
+      <c r="S12" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="T12" s="45" t="s">
+      <c r="T12" s="35" t="s">
         <v>421</v>
       </c>
-      <c r="U12" s="45" t="s">
+      <c r="U12" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="V12" s="45"/>
-      <c r="W12" s="45"/>
+      <c r="V12" s="35"/>
+      <c r="W12" s="35"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
@@ -15326,20 +15326,20 @@
       <c r="N14" s="23"/>
       <c r="O14" s="23"/>
       <c r="P14" s="23"/>
-      <c r="Q14" s="42">
+      <c r="Q14" s="32">
         <v>1</v>
       </c>
-      <c r="S14" s="45" t="s">
+      <c r="S14" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="T14" s="45" t="s">
+      <c r="T14" s="35" t="s">
         <v>422</v>
       </c>
-      <c r="U14" s="45" t="s">
+      <c r="U14" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="V14" s="45"/>
-      <c r="W14" s="45"/>
+      <c r="V14" s="35"/>
+      <c r="W14" s="35"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="31" t="s">
@@ -15362,20 +15362,20 @@
       <c r="N15" s="23"/>
       <c r="O15" s="23"/>
       <c r="P15" s="23"/>
-      <c r="Q15" s="42">
+      <c r="Q15" s="32">
         <v>1</v>
       </c>
-      <c r="S15" s="45" t="s">
+      <c r="S15" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="T15" s="45" t="s">
+      <c r="T15" s="35" t="s">
         <v>423</v>
       </c>
-      <c r="U15" s="45" t="s">
+      <c r="U15" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="V15" s="45"/>
-      <c r="W15" s="45"/>
+      <c r="V15" s="35"/>
+      <c r="W15" s="35"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
@@ -15462,20 +15462,20 @@
       <c r="N18" s="23"/>
       <c r="O18" s="23"/>
       <c r="P18" s="23"/>
-      <c r="Q18" s="42">
+      <c r="Q18" s="32">
         <v>1</v>
       </c>
-      <c r="S18" s="45" t="s">
+      <c r="S18" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="T18" s="45" t="s">
+      <c r="T18" s="35" t="s">
         <v>424</v>
       </c>
-      <c r="U18" s="45" t="s">
+      <c r="U18" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="V18" s="45"/>
-      <c r="W18" s="45"/>
+      <c r="V18" s="35"/>
+      <c r="W18" s="35"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="s">
@@ -15501,7 +15501,7 @@
       <c r="Q19" s="9">
         <v>1</v>
       </c>
-      <c r="S19" s="46" t="s">
+      <c r="S19" s="36" t="s">
         <v>415</v>
       </c>
       <c r="T19" s="30"/>
@@ -15678,23 +15678,23 @@
       <c r="N25" s="23"/>
       <c r="O25" s="23"/>
       <c r="P25" s="23"/>
-      <c r="Q25" s="42">
+      <c r="Q25" s="32">
         <v>1</v>
       </c>
-      <c r="S25" s="45" t="s">
+      <c r="S25" s="35" t="s">
         <v>417</v>
       </c>
-      <c r="T25" s="45" t="s">
+      <c r="T25" s="35" t="s">
         <v>450</v>
       </c>
-      <c r="U25" s="45" t="s">
+      <c r="U25" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="V25" s="45"/>
-      <c r="W25" s="45"/>
+      <c r="V25" s="35"/>
+      <c r="W25" s="35"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A26" s="47" t="s">
+      <c r="A26" s="37" t="s">
         <v>61</v>
       </c>
       <c r="B26" s="25"/>
@@ -15706,7 +15706,7 @@
       <c r="H26" s="23"/>
       <c r="I26" s="23"/>
       <c r="J26" s="23"/>
-      <c r="K26" s="49">
+      <c r="K26" s="39">
         <v>1</v>
       </c>
       <c r="L26" s="23"/>
@@ -15714,20 +15714,20 @@
       <c r="N26" s="23"/>
       <c r="O26" s="23"/>
       <c r="P26" s="23"/>
-      <c r="Q26" s="48">
+      <c r="Q26" s="38">
         <v>1</v>
       </c>
-      <c r="S26" s="43" t="s">
+      <c r="S26" s="33" t="s">
         <v>411</v>
       </c>
-      <c r="T26" s="43" t="s">
+      <c r="T26" s="33" t="s">
         <v>431</v>
       </c>
-      <c r="U26" s="43" t="s">
-        <v>293</v>
-      </c>
-      <c r="V26" s="43"/>
-      <c r="W26" s="43" t="s">
+      <c r="U26" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="V26" s="33"/>
+      <c r="W26" s="33" t="s">
         <v>430</v>
       </c>
     </row>
@@ -15986,7 +15986,7 @@
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A36" s="55" t="s">
+      <c r="A36" s="45" t="s">
         <v>79</v>
       </c>
       <c r="B36" s="25"/>
@@ -16009,13 +16009,13 @@
       <c r="Q36" s="9">
         <v>1</v>
       </c>
-      <c r="S36" s="54" t="s">
+      <c r="S36" s="44" t="s">
         <v>417</v>
       </c>
-      <c r="T36" s="54"/>
-      <c r="U36" s="54"/>
-      <c r="V36" s="54"/>
-      <c r="W36" s="54" t="s">
+      <c r="T36" s="44"/>
+      <c r="U36" s="44"/>
+      <c r="V36" s="44"/>
+      <c r="W36" s="44" t="s">
         <v>449</v>
       </c>
     </row>
@@ -16043,7 +16043,7 @@
       <c r="Q37" s="9">
         <v>1</v>
       </c>
-      <c r="S37" s="46" t="s">
+      <c r="S37" s="36" t="s">
         <v>415</v>
       </c>
       <c r="T37" s="30"/>
@@ -16133,20 +16133,20 @@
       <c r="N40" s="23"/>
       <c r="O40" s="23"/>
       <c r="P40" s="23"/>
-      <c r="Q40" s="42">
+      <c r="Q40" s="32">
         <v>1</v>
       </c>
-      <c r="S40" s="45" t="s">
+      <c r="S40" s="35" t="s">
         <v>417</v>
       </c>
-      <c r="T40" s="45" t="s">
+      <c r="T40" s="35" t="s">
         <v>451</v>
       </c>
-      <c r="U40" s="45" t="s">
+      <c r="U40" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="V40" s="45"/>
-      <c r="W40" s="45"/>
+      <c r="V40" s="35"/>
+      <c r="W40" s="35"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
@@ -16204,7 +16204,7 @@
       <c r="Q42" s="9">
         <v>3</v>
       </c>
-      <c r="S42" s="46" t="s">
+      <c r="S42" s="36" t="s">
         <v>416</v>
       </c>
       <c r="T42" s="30"/>
@@ -16304,7 +16304,7 @@
       <c r="N46" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="O46" s="56" t="s">
+      <c r="O46" s="46" t="s">
         <v>437</v>
       </c>
       <c r="P46" s="29"/>
@@ -16348,7 +16348,7 @@
       <c r="N47" s="5" t="s">
         <v>441</v>
       </c>
-      <c r="O47" s="56" t="s">
+      <c r="O47" s="46" t="s">
         <v>441</v>
       </c>
       <c r="P47" s="29"/>
@@ -16357,8 +16357,8 @@
       <c r="A48" s="13" t="s">
         <v>436</v>
       </c>
-      <c r="B48" s="53"/>
-      <c r="C48" s="53"/>
+      <c r="B48" s="43"/>
+      <c r="C48" s="43"/>
       <c r="D48" s="5" t="s">
         <v>436</v>
       </c>
@@ -16408,7 +16408,7 @@
       </c>
       <c r="M49" s="29"/>
       <c r="N49" s="29"/>
-      <c r="O49" s="56" t="s">
+      <c r="O49" s="46" t="s">
         <v>438</v>
       </c>
       <c r="P49" s="29"/>
@@ -16470,22 +16470,22 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="47" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="49" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="35"/>
+      <c r="C5" s="52"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
@@ -16535,10 +16535,10 @@
       <c r="A10" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="55" t="s">
         <v>407</v>
       </c>
     </row>
@@ -16546,26 +16546,26 @@
       <c r="A11" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="39"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="56"/>
     </row>
     <row r="12" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="47" t="s">
         <v>115</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="49" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="35"/>
+      <c r="C13" s="52"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
@@ -16601,22 +16601,22 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="47" t="s">
         <v>122</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="49" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
+      <c r="A18" s="51"/>
       <c r="B18" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="35"/>
+      <c r="C18" s="52"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
@@ -16641,22 +16641,22 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="53" t="s">
         <v>131</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="55" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="39"/>
+      <c r="C22" s="56"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
@@ -16728,10 +16728,10 @@
       <c r="A29" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="49" t="s">
         <v>407</v>
       </c>
     </row>
@@ -16739,33 +16739,33 @@
       <c r="A30" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="41"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="50"/>
     </row>
     <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="35"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="52"/>
     </row>
     <row r="32" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="53" t="s">
         <v>65</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="55" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
+      <c r="A33" s="54"/>
       <c r="B33" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="39"/>
+      <c r="C33" s="56"/>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
@@ -16845,22 +16845,22 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="36" t="s">
+      <c r="A41" s="53" t="s">
         <v>166</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="38" t="s">
+      <c r="C41" s="55" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="37"/>
+      <c r="A42" s="54"/>
       <c r="B42" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="39"/>
+      <c r="C42" s="56"/>
     </row>
     <row r="43" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
@@ -16885,38 +16885,32 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="32" t="s">
+      <c r="A45" s="47" t="s">
         <v>87</v>
       </c>
       <c r="B45" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C45" s="34" t="s">
+      <c r="C45" s="49" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="40"/>
+      <c r="A46" s="48"/>
       <c r="B46" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="41"/>
+      <c r="C46" s="50"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="40"/>
+      <c r="A47" s="48"/>
       <c r="B47" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="41"/>
+      <c r="C47" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="C32:C33"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B10:B11"/>
@@ -16929,6 +16923,12 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="C21:C22"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="C32:C33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://cpicpgx.org/guidelines/guideline-for-abacavir-and-hla-b/"/>

</xml_diff>

<commit_message>
Created carbamazepine recommendation (HLA-A & HLA-B) KO; Updated cpicPairs.xlsx
</commit_message>
<xml_diff>
--- a/cpicPairs.xlsx
+++ b/cpicPairs.xlsx
@@ -18,7 +18,7 @@
     <sheet name="Gene-Drug" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1928" uniqueCount="460">
   <si>
     <t>Gene</t>
   </si>
@@ -1382,6 +1382,30 @@
   </si>
   <si>
     <t>/99999/fk4fn2d721/v0.0.1</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>A&amp;P</t>
+  </si>
+  <si>
+    <t>A&amp;F</t>
+  </si>
+  <si>
+    <t>A&amp;A</t>
+  </si>
+  <si>
+    <t>Genes</t>
+  </si>
+  <si>
+    <t>KO arkid</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
@@ -1957,7 +1981,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2076,16 +2100,10 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2102,6 +2120,16 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -14806,10 +14834,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W49"/>
+  <dimension ref="A1:X49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -14827,107 +14855,108 @@
     <col min="15" max="15" width="10.375" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.125" style="5" customWidth="1"/>
     <col min="17" max="17" width="11.375" style="6" customWidth="1"/>
-    <col min="18" max="18" width="1.25" customWidth="1"/>
+    <col min="18" max="18" width="15.625" customWidth="1"/>
     <col min="19" max="19" width="27.375" customWidth="1"/>
     <col min="20" max="20" width="23.625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.75" customWidth="1"/>
-    <col min="23" max="23" width="32.625" customWidth="1"/>
-    <col min="24" max="24" width="6" customWidth="1"/>
-    <col min="25" max="25" width="8.5" customWidth="1"/>
-    <col min="26" max="26" width="9" customWidth="1"/>
-    <col min="27" max="27" width="6.625" customWidth="1"/>
-    <col min="28" max="28" width="6.25" customWidth="1"/>
-    <col min="29" max="29" width="5.75" customWidth="1"/>
-    <col min="30" max="31" width="7.375" customWidth="1"/>
-    <col min="32" max="35" width="8.25" customWidth="1"/>
-    <col min="36" max="36" width="10.125" customWidth="1"/>
-    <col min="37" max="37" width="8.125" customWidth="1"/>
-    <col min="38" max="38" width="9.125" customWidth="1"/>
-    <col min="39" max="41" width="8.125" customWidth="1"/>
-    <col min="42" max="44" width="7.875" customWidth="1"/>
-    <col min="45" max="45" width="6.125" customWidth="1"/>
-    <col min="46" max="46" width="6" customWidth="1"/>
-    <col min="47" max="47" width="9.625" customWidth="1"/>
-    <col min="48" max="48" width="4.75" customWidth="1"/>
-    <col min="49" max="49" width="7" customWidth="1"/>
-    <col min="50" max="50" width="7.25" customWidth="1"/>
-    <col min="51" max="51" width="3" customWidth="1"/>
-    <col min="52" max="52" width="8.375" customWidth="1"/>
-    <col min="53" max="53" width="5.875" customWidth="1"/>
-    <col min="54" max="54" width="7" customWidth="1"/>
-    <col min="55" max="55" width="6.875" customWidth="1"/>
-    <col min="56" max="56" width="6" customWidth="1"/>
-    <col min="57" max="57" width="4.875" customWidth="1"/>
-    <col min="58" max="58" width="6.5" customWidth="1"/>
-    <col min="59" max="59" width="6.125" customWidth="1"/>
-    <col min="60" max="60" width="7.125" customWidth="1"/>
-    <col min="61" max="61" width="6.625" customWidth="1"/>
-    <col min="62" max="62" width="7.5" customWidth="1"/>
-    <col min="63" max="63" width="7.125" customWidth="1"/>
-    <col min="64" max="64" width="5.625" customWidth="1"/>
-    <col min="65" max="65" width="6.25" customWidth="1"/>
-    <col min="66" max="67" width="6.5" customWidth="1"/>
-    <col min="68" max="69" width="10.125" customWidth="1"/>
-    <col min="70" max="70" width="10.25" customWidth="1"/>
-    <col min="71" max="71" width="8.125" customWidth="1"/>
-    <col min="72" max="72" width="7.125" customWidth="1"/>
-    <col min="73" max="74" width="7" customWidth="1"/>
-    <col min="75" max="75" width="7.25" customWidth="1"/>
-    <col min="76" max="77" width="6" customWidth="1"/>
-    <col min="78" max="78" width="5" customWidth="1"/>
-    <col min="79" max="79" width="7.75" customWidth="1"/>
-    <col min="80" max="80" width="4.875" customWidth="1"/>
-    <col min="81" max="81" width="5.875" customWidth="1"/>
-    <col min="82" max="82" width="4.375" customWidth="1"/>
-    <col min="83" max="83" width="6.875" customWidth="1"/>
-    <col min="84" max="84" width="6.25" customWidth="1"/>
-    <col min="85" max="85" width="7.625" customWidth="1"/>
-    <col min="86" max="86" width="9.5" customWidth="1"/>
-    <col min="87" max="87" width="6.5" customWidth="1"/>
-    <col min="88" max="88" width="6.125" customWidth="1"/>
-    <col min="89" max="90" width="5.625" customWidth="1"/>
-    <col min="91" max="91" width="8.375" customWidth="1"/>
-    <col min="92" max="92" width="6.25" customWidth="1"/>
-    <col min="93" max="93" width="6.875" customWidth="1"/>
-    <col min="94" max="94" width="8.25" customWidth="1"/>
-    <col min="95" max="95" width="7.625" customWidth="1"/>
-    <col min="96" max="96" width="5" customWidth="1"/>
-    <col min="97" max="97" width="6.25" customWidth="1"/>
-    <col min="98" max="98" width="7.375" customWidth="1"/>
-    <col min="99" max="99" width="6.375" customWidth="1"/>
-    <col min="100" max="100" width="7.25" customWidth="1"/>
-    <col min="101" max="101" width="7.375" customWidth="1"/>
-    <col min="102" max="102" width="7.125" customWidth="1"/>
-    <col min="103" max="103" width="5.875" customWidth="1"/>
-    <col min="104" max="104" width="7" customWidth="1"/>
-    <col min="105" max="105" width="8.5" customWidth="1"/>
-    <col min="106" max="106" width="10.25" customWidth="1"/>
-    <col min="107" max="108" width="8.75" customWidth="1"/>
-    <col min="109" max="109" width="7.75" customWidth="1"/>
-    <col min="110" max="110" width="9.5" customWidth="1"/>
-    <col min="111" max="111" width="6" customWidth="1"/>
-    <col min="112" max="112" width="7" customWidth="1"/>
-    <col min="113" max="113" width="7.75" customWidth="1"/>
-    <col min="114" max="114" width="8.625" customWidth="1"/>
-    <col min="115" max="115" width="4.625" customWidth="1"/>
-    <col min="116" max="116" width="5.375" customWidth="1"/>
-    <col min="117" max="117" width="6.25" customWidth="1"/>
-    <col min="118" max="118" width="8.5" customWidth="1"/>
-    <col min="119" max="119" width="6.25" customWidth="1"/>
-    <col min="120" max="121" width="8.125" customWidth="1"/>
-    <col min="122" max="122" width="9.375" customWidth="1"/>
-    <col min="123" max="123" width="6.375" customWidth="1"/>
-    <col min="124" max="124" width="4.75" customWidth="1"/>
-    <col min="125" max="125" width="8.625" customWidth="1"/>
-    <col min="126" max="126" width="4.75" customWidth="1"/>
-    <col min="127" max="127" width="7.25" customWidth="1"/>
-    <col min="128" max="128" width="8" customWidth="1"/>
-    <col min="129" max="129" width="6.875" customWidth="1"/>
-    <col min="130" max="130" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.125" customWidth="1"/>
+    <col min="22" max="22" width="5.5" customWidth="1"/>
+    <col min="23" max="23" width="5.75" customWidth="1"/>
+    <col min="24" max="24" width="32.625" customWidth="1"/>
+    <col min="25" max="25" width="6" customWidth="1"/>
+    <col min="26" max="26" width="8.5" customWidth="1"/>
+    <col min="27" max="27" width="9" customWidth="1"/>
+    <col min="28" max="28" width="6.625" customWidth="1"/>
+    <col min="29" max="29" width="6.25" customWidth="1"/>
+    <col min="30" max="30" width="5.75" customWidth="1"/>
+    <col min="31" max="32" width="7.375" customWidth="1"/>
+    <col min="33" max="36" width="8.25" customWidth="1"/>
+    <col min="37" max="37" width="10.125" customWidth="1"/>
+    <col min="38" max="38" width="8.125" customWidth="1"/>
+    <col min="39" max="39" width="9.125" customWidth="1"/>
+    <col min="40" max="42" width="8.125" customWidth="1"/>
+    <col min="43" max="45" width="7.875" customWidth="1"/>
+    <col min="46" max="46" width="6.125" customWidth="1"/>
+    <col min="47" max="47" width="6" customWidth="1"/>
+    <col min="48" max="48" width="9.625" customWidth="1"/>
+    <col min="49" max="49" width="4.75" customWidth="1"/>
+    <col min="50" max="50" width="7" customWidth="1"/>
+    <col min="51" max="51" width="7.25" customWidth="1"/>
+    <col min="52" max="52" width="3" customWidth="1"/>
+    <col min="53" max="53" width="8.375" customWidth="1"/>
+    <col min="54" max="54" width="5.875" customWidth="1"/>
+    <col min="55" max="55" width="7" customWidth="1"/>
+    <col min="56" max="56" width="6.875" customWidth="1"/>
+    <col min="57" max="57" width="6" customWidth="1"/>
+    <col min="58" max="58" width="4.875" customWidth="1"/>
+    <col min="59" max="59" width="6.5" customWidth="1"/>
+    <col min="60" max="60" width="6.125" customWidth="1"/>
+    <col min="61" max="61" width="7.125" customWidth="1"/>
+    <col min="62" max="62" width="6.625" customWidth="1"/>
+    <col min="63" max="63" width="7.5" customWidth="1"/>
+    <col min="64" max="64" width="7.125" customWidth="1"/>
+    <col min="65" max="65" width="5.625" customWidth="1"/>
+    <col min="66" max="66" width="6.25" customWidth="1"/>
+    <col min="67" max="68" width="6.5" customWidth="1"/>
+    <col min="69" max="70" width="10.125" customWidth="1"/>
+    <col min="71" max="71" width="10.25" customWidth="1"/>
+    <col min="72" max="72" width="8.125" customWidth="1"/>
+    <col min="73" max="73" width="7.125" customWidth="1"/>
+    <col min="74" max="75" width="7" customWidth="1"/>
+    <col min="76" max="76" width="7.25" customWidth="1"/>
+    <col min="77" max="78" width="6" customWidth="1"/>
+    <col min="79" max="79" width="5" customWidth="1"/>
+    <col min="80" max="80" width="7.75" customWidth="1"/>
+    <col min="81" max="81" width="4.875" customWidth="1"/>
+    <col min="82" max="82" width="5.875" customWidth="1"/>
+    <col min="83" max="83" width="4.375" customWidth="1"/>
+    <col min="84" max="84" width="6.875" customWidth="1"/>
+    <col min="85" max="85" width="6.25" customWidth="1"/>
+    <col min="86" max="86" width="7.625" customWidth="1"/>
+    <col min="87" max="87" width="9.5" customWidth="1"/>
+    <col min="88" max="88" width="6.5" customWidth="1"/>
+    <col min="89" max="89" width="6.125" customWidth="1"/>
+    <col min="90" max="91" width="5.625" customWidth="1"/>
+    <col min="92" max="92" width="8.375" customWidth="1"/>
+    <col min="93" max="93" width="6.25" customWidth="1"/>
+    <col min="94" max="94" width="6.875" customWidth="1"/>
+    <col min="95" max="95" width="8.25" customWidth="1"/>
+    <col min="96" max="96" width="7.625" customWidth="1"/>
+    <col min="97" max="97" width="5" customWidth="1"/>
+    <col min="98" max="98" width="6.25" customWidth="1"/>
+    <col min="99" max="99" width="7.375" customWidth="1"/>
+    <col min="100" max="100" width="6.375" customWidth="1"/>
+    <col min="101" max="101" width="7.25" customWidth="1"/>
+    <col min="102" max="102" width="7.375" customWidth="1"/>
+    <col min="103" max="103" width="7.125" customWidth="1"/>
+    <col min="104" max="104" width="5.875" customWidth="1"/>
+    <col min="105" max="105" width="7" customWidth="1"/>
+    <col min="106" max="106" width="8.5" customWidth="1"/>
+    <col min="107" max="107" width="10.25" customWidth="1"/>
+    <col min="108" max="109" width="8.75" customWidth="1"/>
+    <col min="110" max="110" width="7.75" customWidth="1"/>
+    <col min="111" max="111" width="9.5" customWidth="1"/>
+    <col min="112" max="112" width="6" customWidth="1"/>
+    <col min="113" max="113" width="7" customWidth="1"/>
+    <col min="114" max="114" width="7.75" customWidth="1"/>
+    <col min="115" max="115" width="8.625" customWidth="1"/>
+    <col min="116" max="116" width="4.625" customWidth="1"/>
+    <col min="117" max="117" width="5.375" customWidth="1"/>
+    <col min="118" max="118" width="6.25" customWidth="1"/>
+    <col min="119" max="119" width="8.5" customWidth="1"/>
+    <col min="120" max="120" width="6.25" customWidth="1"/>
+    <col min="121" max="122" width="8.125" customWidth="1"/>
+    <col min="123" max="123" width="9.375" customWidth="1"/>
+    <col min="124" max="124" width="6.375" customWidth="1"/>
+    <col min="125" max="125" width="4.75" customWidth="1"/>
+    <col min="126" max="126" width="8.625" customWidth="1"/>
+    <col min="127" max="127" width="4.75" customWidth="1"/>
+    <col min="128" max="128" width="7.25" customWidth="1"/>
+    <col min="129" max="129" width="8" customWidth="1"/>
+    <col min="130" max="130" width="6.875" customWidth="1"/>
+    <col min="131" max="131" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
@@ -14935,7 +14964,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>405</v>
       </c>
@@ -14943,7 +14972,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>401</v>
       </c>
@@ -14995,8 +15024,23 @@
       <c r="Q4" s="6" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="R4" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="S4" s="58" t="s">
+        <v>456</v>
+      </c>
+      <c r="T4" s="58" t="s">
+        <v>457</v>
+      </c>
+      <c r="U4" s="58" t="s">
+        <v>458</v>
+      </c>
+      <c r="V4" s="58" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
         <v>8</v>
       </c>
@@ -15020,6 +15064,10 @@
       <c r="Q5" s="32">
         <v>1</v>
       </c>
+      <c r="R5" s="35" t="str">
+        <f>A5</f>
+        <v>abacavir</v>
+      </c>
       <c r="S5" s="35" t="s">
         <v>409</v>
       </c>
@@ -15029,10 +15077,13 @@
       <c r="U5" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="V5" s="35"/>
+      <c r="V5" s="35" t="s">
+        <v>10</v>
+      </c>
       <c r="W5" s="35"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X5" s="35"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
         <v>14</v>
       </c>
@@ -15056,6 +15107,10 @@
       <c r="Q6" s="32">
         <v>1</v>
       </c>
+      <c r="R6" s="35" t="str">
+        <f t="shared" ref="R6:R42" si="0">A6</f>
+        <v>allopurinol</v>
+      </c>
       <c r="S6" s="35" t="s">
         <v>408</v>
       </c>
@@ -15065,10 +15120,13 @@
       <c r="U6" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="V6" s="35"/>
+      <c r="V6" s="35" t="s">
+        <v>10</v>
+      </c>
       <c r="W6" s="35"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X6" s="35"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="37" t="s">
         <v>18</v>
       </c>
@@ -15094,6 +15152,10 @@
       <c r="Q7" s="38">
         <v>2</v>
       </c>
+      <c r="R7" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>amitriptyline</v>
+      </c>
       <c r="S7" s="33" t="s">
         <v>413</v>
       </c>
@@ -15104,13 +15166,16 @@
         <v>426</v>
       </c>
       <c r="V7" s="33" t="s">
+        <v>427</v>
+      </c>
+      <c r="W7" s="33" t="s">
         <v>428</v>
       </c>
-      <c r="W7" s="33" t="s">
+      <c r="X7" s="33" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="s">
         <v>24</v>
       </c>
@@ -15134,6 +15199,10 @@
       <c r="Q8" s="32">
         <v>1</v>
       </c>
+      <c r="R8" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>atazanavir</v>
+      </c>
       <c r="S8" s="35" t="s">
         <v>23</v>
       </c>
@@ -15143,10 +15212,13 @@
       <c r="U8" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="V8" s="35"/>
+      <c r="V8" s="35" t="s">
+        <v>427</v>
+      </c>
       <c r="W8" s="35"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X8" s="35"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>27</v>
       </c>
@@ -15170,11 +15242,21 @@
       <c r="Q9" s="9">
         <v>1</v>
       </c>
+      <c r="R9" t="str">
+        <f t="shared" si="0"/>
+        <v>azathioprine</v>
+      </c>
       <c r="S9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U9" s="57" t="s">
+        <v>427</v>
+      </c>
+      <c r="V9" s="57" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
         <v>32</v>
       </c>
@@ -15198,6 +15280,10 @@
       <c r="Q10" s="9">
         <v>1</v>
       </c>
+      <c r="R10" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>capecitabine</v>
+      </c>
       <c r="S10" s="36" t="s">
         <v>415</v>
       </c>
@@ -15205,8 +15291,9 @@
       <c r="U10" s="30"/>
       <c r="V10" s="30"/>
       <c r="W10" s="30"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X10" s="30"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>36</v>
       </c>
@@ -15232,11 +15319,21 @@
       <c r="Q11" s="9">
         <v>2</v>
       </c>
+      <c r="R11" t="str">
+        <f t="shared" si="0"/>
+        <v>carbamazepine</v>
+      </c>
       <c r="S11" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U11" s="57" t="s">
+        <v>455</v>
+      </c>
+      <c r="V11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
         <v>92</v>
       </c>
@@ -15260,6 +15357,10 @@
       <c r="Q12" s="32">
         <v>1</v>
       </c>
+      <c r="R12" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>citalopram</v>
+      </c>
       <c r="S12" s="35" t="s">
         <v>17</v>
       </c>
@@ -15269,10 +15370,13 @@
       <c r="U12" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="V12" s="35"/>
+      <c r="V12" s="35" t="s">
+        <v>427</v>
+      </c>
       <c r="W12" s="35"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X12" s="35"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>115</v>
       </c>
@@ -15298,14 +15402,24 @@
       <c r="Q13" s="9">
         <v>2</v>
       </c>
+      <c r="R13" t="str">
+        <f t="shared" si="0"/>
+        <v>clomipramine</v>
+      </c>
       <c r="S13" t="s">
         <v>413</v>
       </c>
+      <c r="U13" s="57" t="s">
+        <v>427</v>
+      </c>
       <c r="V13" t="s">
+        <v>427</v>
+      </c>
+      <c r="W13" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
         <v>38</v>
       </c>
@@ -15329,6 +15443,10 @@
       <c r="Q14" s="32">
         <v>1</v>
       </c>
+      <c r="R14" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>clopidogrel</v>
+      </c>
       <c r="S14" s="35" t="s">
         <v>17</v>
       </c>
@@ -15338,10 +15456,13 @@
       <c r="U14" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="V14" s="35"/>
+      <c r="V14" s="35" t="s">
+        <v>427</v>
+      </c>
       <c r="W14" s="35"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X14" s="35"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="31" t="s">
         <v>41</v>
       </c>
@@ -15365,6 +15486,10 @@
       <c r="Q15" s="32">
         <v>1</v>
       </c>
+      <c r="R15" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>codeine</v>
+      </c>
       <c r="S15" s="35" t="s">
         <v>21</v>
       </c>
@@ -15374,10 +15499,13 @@
       <c r="U15" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="V15" s="35"/>
+      <c r="V15" s="35" t="s">
+        <v>427</v>
+      </c>
       <c r="W15" s="35"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X15" s="35"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>117</v>
       </c>
@@ -15401,14 +15529,24 @@
       <c r="Q16" s="9">
         <v>1</v>
       </c>
+      <c r="R16" t="str">
+        <f t="shared" si="0"/>
+        <v>desipramine</v>
+      </c>
       <c r="S16" t="s">
         <v>21</v>
       </c>
-      <c r="V16" t="s">
+      <c r="U16" s="57" t="s">
+        <v>427</v>
+      </c>
+      <c r="V16" s="57" t="s">
+        <v>427</v>
+      </c>
+      <c r="W16" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>122</v>
       </c>
@@ -15434,14 +15572,24 @@
       <c r="Q17" s="9">
         <v>2</v>
       </c>
+      <c r="R17" t="str">
+        <f t="shared" si="0"/>
+        <v>doxepin</v>
+      </c>
       <c r="S17" t="s">
         <v>413</v>
       </c>
-      <c r="V17" t="s">
+      <c r="U17" s="57" t="s">
+        <v>426</v>
+      </c>
+      <c r="V17" s="57" t="s">
+        <v>427</v>
+      </c>
+      <c r="W17" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="31" t="s">
         <v>93</v>
       </c>
@@ -15465,6 +15613,10 @@
       <c r="Q18" s="32">
         <v>1</v>
       </c>
+      <c r="R18" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>escitalopram</v>
+      </c>
       <c r="S18" s="35" t="s">
         <v>17</v>
       </c>
@@ -15474,10 +15626,13 @@
       <c r="U18" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="V18" s="35"/>
+      <c r="V18" s="35" t="s">
+        <v>427</v>
+      </c>
       <c r="W18" s="35"/>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X18" s="35"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="s">
         <v>47</v>
       </c>
@@ -15501,6 +15656,10 @@
       <c r="Q19" s="9">
         <v>1</v>
       </c>
+      <c r="R19" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>fluorouracil</v>
+      </c>
       <c r="S19" s="36" t="s">
         <v>415</v>
       </c>
@@ -15508,8 +15667,9 @@
       <c r="U19" s="30"/>
       <c r="V19" s="30"/>
       <c r="W19" s="30"/>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X19" s="30"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>48</v>
       </c>
@@ -15533,11 +15693,21 @@
       <c r="Q20" s="9">
         <v>1</v>
       </c>
+      <c r="R20" t="str">
+        <f t="shared" si="0"/>
+        <v>fluvoxamine</v>
+      </c>
       <c r="S20" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U20" t="s">
+        <v>427</v>
+      </c>
+      <c r="V20" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>131</v>
       </c>
@@ -15563,14 +15733,24 @@
       <c r="Q21" s="9">
         <v>2</v>
       </c>
+      <c r="R21" t="str">
+        <f t="shared" si="0"/>
+        <v>imipramine</v>
+      </c>
       <c r="S21" t="s">
         <v>413</v>
       </c>
+      <c r="U21" t="s">
+        <v>426</v>
+      </c>
       <c r="V21" t="s">
+        <v>427</v>
+      </c>
+      <c r="W21" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>54</v>
       </c>
@@ -15594,11 +15774,21 @@
       <c r="Q22" s="9">
         <v>1</v>
       </c>
+      <c r="R22" t="str">
+        <f t="shared" si="0"/>
+        <v>ivacaftor</v>
+      </c>
       <c r="S22" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U22" t="s">
+        <v>427</v>
+      </c>
+      <c r="V22" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>56</v>
       </c>
@@ -15622,11 +15812,21 @@
       <c r="Q23" s="9">
         <v>1</v>
       </c>
+      <c r="R23" t="str">
+        <f t="shared" si="0"/>
+        <v>mercaptopurine</v>
+      </c>
       <c r="S23" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U23" t="s">
+        <v>427</v>
+      </c>
+      <c r="V23" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>57</v>
       </c>
@@ -15650,14 +15850,24 @@
       <c r="Q24" s="9">
         <v>1</v>
       </c>
+      <c r="R24" t="str">
+        <f t="shared" si="0"/>
+        <v>nortriptyline</v>
+      </c>
       <c r="S24" t="s">
         <v>417</v>
       </c>
+      <c r="U24" t="s">
+        <v>427</v>
+      </c>
       <c r="V24" t="s">
+        <v>427</v>
+      </c>
+      <c r="W24" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="31" t="s">
         <v>58</v>
       </c>
@@ -15681,6 +15891,10 @@
       <c r="Q25" s="32">
         <v>1</v>
       </c>
+      <c r="R25" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>ondansetron</v>
+      </c>
       <c r="S25" s="35" t="s">
         <v>417</v>
       </c>
@@ -15690,10 +15904,13 @@
       <c r="U25" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="V25" s="35"/>
+      <c r="V25" s="35" t="s">
+        <v>427</v>
+      </c>
       <c r="W25" s="35"/>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X25" s="35"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" s="37" t="s">
         <v>61</v>
       </c>
@@ -15717,6 +15934,10 @@
       <c r="Q26" s="38">
         <v>1</v>
       </c>
+      <c r="R26" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>oxcarbazepine</v>
+      </c>
       <c r="S26" s="33" t="s">
         <v>411</v>
       </c>
@@ -15726,12 +15947,15 @@
       <c r="U26" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="V26" s="33"/>
-      <c r="W26" s="33" t="s">
+      <c r="V26" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="W26" s="33"/>
+      <c r="X26" s="33" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>63</v>
       </c>
@@ -15755,11 +15979,21 @@
       <c r="Q27" s="9">
         <v>1</v>
       </c>
+      <c r="R27" t="str">
+        <f t="shared" si="0"/>
+        <v>paroxetine</v>
+      </c>
       <c r="S27" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U27" t="s">
+        <v>427</v>
+      </c>
+      <c r="V27" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>95</v>
       </c>
@@ -15783,11 +16017,21 @@
       <c r="Q28" s="9">
         <v>1</v>
       </c>
+      <c r="R28" t="str">
+        <f t="shared" si="0"/>
+        <v>peginterferon alfa-2a</v>
+      </c>
       <c r="S28" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U28" t="s">
+        <v>427</v>
+      </c>
+      <c r="V28" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>97</v>
       </c>
@@ -15811,11 +16055,21 @@
       <c r="Q29" s="9">
         <v>1</v>
       </c>
+      <c r="R29" t="str">
+        <f t="shared" si="0"/>
+        <v>peginterferon alfa-2b</v>
+      </c>
       <c r="S29" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U29" t="s">
+        <v>427</v>
+      </c>
+      <c r="V29" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>65</v>
       </c>
@@ -15841,11 +16095,21 @@
       <c r="Q30" s="9">
         <v>2</v>
       </c>
+      <c r="R30" t="str">
+        <f t="shared" si="0"/>
+        <v>phenytoin</v>
+      </c>
       <c r="S30" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U30" t="s">
+        <v>453</v>
+      </c>
+      <c r="V30" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>68</v>
       </c>
@@ -15869,11 +16133,21 @@
       <c r="Q31" s="9">
         <v>1</v>
       </c>
+      <c r="R31" t="str">
+        <f t="shared" si="0"/>
+        <v>rasburicase</v>
+      </c>
       <c r="S31" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U31" t="s">
+        <v>427</v>
+      </c>
+      <c r="V31" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>98</v>
       </c>
@@ -15897,11 +16171,21 @@
       <c r="Q32" s="9">
         <v>1</v>
       </c>
+      <c r="R32" t="str">
+        <f t="shared" si="0"/>
+        <v>ribavirin</v>
+      </c>
       <c r="S32" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U32" t="s">
+        <v>427</v>
+      </c>
+      <c r="V32" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>160</v>
       </c>
@@ -15925,11 +16209,21 @@
       <c r="Q33" s="9">
         <v>1</v>
       </c>
+      <c r="R33" t="str">
+        <f t="shared" si="0"/>
+        <v>sertraline</v>
+      </c>
       <c r="S33" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U33" t="s">
+        <v>427</v>
+      </c>
+      <c r="V33" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>72</v>
       </c>
@@ -15953,11 +16247,21 @@
       <c r="Q34" s="9">
         <v>1</v>
       </c>
+      <c r="R34" t="str">
+        <f t="shared" si="0"/>
+        <v>simvastatin</v>
+      </c>
       <c r="S34" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U34" t="s">
+        <v>427</v>
+      </c>
+      <c r="V34" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>77</v>
       </c>
@@ -15981,11 +16285,21 @@
       <c r="Q35" s="9">
         <v>1</v>
       </c>
+      <c r="R35" t="str">
+        <f t="shared" si="0"/>
+        <v>tacrolimus</v>
+      </c>
       <c r="S35" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U35" t="s">
+        <v>427</v>
+      </c>
+      <c r="V35" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="45" t="s">
         <v>79</v>
       </c>
@@ -16009,17 +16323,26 @@
       <c r="Q36" s="9">
         <v>1</v>
       </c>
+      <c r="R36" s="44" t="str">
+        <f t="shared" si="0"/>
+        <v>tamoxifen</v>
+      </c>
       <c r="S36" s="44" t="s">
         <v>417</v>
       </c>
       <c r="T36" s="44"/>
-      <c r="U36" s="44"/>
-      <c r="V36" s="44"/>
-      <c r="W36" s="44" t="s">
+      <c r="U36" s="44" t="s">
+        <v>427</v>
+      </c>
+      <c r="V36" s="44" t="s">
+        <v>427</v>
+      </c>
+      <c r="W36" s="44"/>
+      <c r="X36" s="44" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="27" t="s">
         <v>255</v>
       </c>
@@ -16043,6 +16366,10 @@
       <c r="Q37" s="9">
         <v>1</v>
       </c>
+      <c r="R37" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>tegafur</v>
+      </c>
       <c r="S37" s="36" t="s">
         <v>415</v>
       </c>
@@ -16050,8 +16377,9 @@
       <c r="U37" s="30"/>
       <c r="V37" s="30"/>
       <c r="W37" s="30"/>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X37" s="30"/>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>81</v>
       </c>
@@ -16075,11 +16403,21 @@
       <c r="Q38" s="9">
         <v>1</v>
       </c>
+      <c r="R38" t="str">
+        <f t="shared" si="0"/>
+        <v>thioguanine</v>
+      </c>
       <c r="S38" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U38" t="s">
+        <v>427</v>
+      </c>
+      <c r="V38" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>166</v>
       </c>
@@ -16105,14 +16443,24 @@
       <c r="Q39" s="9">
         <v>2</v>
       </c>
+      <c r="R39" t="str">
+        <f t="shared" si="0"/>
+        <v>trimipramine</v>
+      </c>
       <c r="S39" t="s">
         <v>413</v>
       </c>
+      <c r="U39" t="s">
+        <v>426</v>
+      </c>
       <c r="V39" t="s">
+        <v>427</v>
+      </c>
+      <c r="W39" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="31" t="s">
         <v>84</v>
       </c>
@@ -16136,6 +16484,10 @@
       <c r="Q40" s="32">
         <v>1</v>
       </c>
+      <c r="R40" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>tropisetron</v>
+      </c>
       <c r="S40" s="35" t="s">
         <v>417</v>
       </c>
@@ -16147,8 +16499,9 @@
       </c>
       <c r="V40" s="35"/>
       <c r="W40" s="35"/>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X40" s="35"/>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>85</v>
       </c>
@@ -16172,11 +16525,21 @@
       <c r="Q41" s="9">
         <v>1</v>
       </c>
+      <c r="R41" t="str">
+        <f t="shared" si="0"/>
+        <v>voriconazole</v>
+      </c>
       <c r="S41" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U41" t="s">
+        <v>427</v>
+      </c>
+      <c r="V41" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="27" t="s">
         <v>87</v>
       </c>
@@ -16204,6 +16567,10 @@
       <c r="Q42" s="9">
         <v>3</v>
       </c>
+      <c r="R42" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>warfarin</v>
+      </c>
       <c r="S42" s="36" t="s">
         <v>416</v>
       </c>
@@ -16211,8 +16578,9 @@
       <c r="U42" s="30"/>
       <c r="V42" s="30"/>
       <c r="W42" s="30"/>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X42" s="30"/>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>403</v>
       </c>
@@ -16265,7 +16633,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" s="13" t="s">
         <v>433</v>
       </c>
@@ -16309,12 +16677,12 @@
       </c>
       <c r="P46" s="29"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
         <v>434</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>441</v>
@@ -16353,7 +16721,7 @@
       </c>
       <c r="P47" s="29"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
         <v>436</v>
       </c>
@@ -16481,11 +16849,11 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="51"/>
+      <c r="A5" s="48"/>
       <c r="B5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="52"/>
+      <c r="C5" s="50"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
@@ -16535,10 +16903,10 @@
       <c r="A10" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="55" t="s">
+      <c r="C10" s="53" t="s">
         <v>407</v>
       </c>
     </row>
@@ -16546,8 +16914,8 @@
       <c r="A11" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="54"/>
-      <c r="C11" s="56"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="54"/>
     </row>
     <row r="12" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A12" s="47" t="s">
@@ -16561,11 +16929,11 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
+      <c r="A13" s="48"/>
       <c r="B13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="52"/>
+      <c r="C13" s="50"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
@@ -16612,11 +16980,11 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="51"/>
+      <c r="A18" s="48"/>
       <c r="B18" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="52"/>
+      <c r="C18" s="50"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
@@ -16641,22 +17009,22 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="53" t="s">
+      <c r="A21" s="51" t="s">
         <v>131</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="55" t="s">
+      <c r="C21" s="53" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="54"/>
+      <c r="A22" s="52"/>
       <c r="B22" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="56"/>
+      <c r="C22" s="54"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
@@ -16739,33 +17107,33 @@
       <c r="A30" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="48"/>
-      <c r="C30" s="50"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="56"/>
     </row>
     <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="51"/>
-      <c r="C31" s="52"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="50"/>
     </row>
     <row r="32" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="53" t="s">
+      <c r="A32" s="51" t="s">
         <v>65</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="55" t="s">
+      <c r="C32" s="53" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="54"/>
+      <c r="A33" s="52"/>
       <c r="B33" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="56"/>
+      <c r="C33" s="54"/>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
@@ -16845,22 +17213,22 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="53" t="s">
+      <c r="A41" s="51" t="s">
         <v>166</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="55" t="s">
+      <c r="C41" s="53" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="54"/>
+      <c r="A42" s="52"/>
       <c r="B42" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="56"/>
+      <c r="C42" s="54"/>
     </row>
     <row r="43" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
@@ -16896,21 +17264,27 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="48"/>
+      <c r="A46" s="55"/>
       <c r="B46" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="50"/>
+      <c r="C46" s="56"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="48"/>
+      <c r="A47" s="55"/>
       <c r="B47" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="50"/>
+      <c r="C47" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="C32:C33"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B10:B11"/>
@@ -16923,12 +17297,6 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="C32:C33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://cpicpgx.org/guidelines/guideline-for-abacavir-and-hla-b/"/>

</xml_diff>

<commit_message>
Created geno-pheno for CYP3A5
</commit_message>
<xml_diff>
--- a/cpicPairs.xlsx
+++ b/cpicPairs.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1930" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1931" uniqueCount="462">
   <si>
     <t>Gene</t>
   </si>
@@ -1409,6 +1409,9 @@
   </si>
   <si>
     <t>/99999/fk4mw3nw5p/v0.0.1</t>
+  </si>
+  <si>
+    <t>need patient race as input</t>
   </si>
 </sst>
 </file>
@@ -1984,7 +1987,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2133,6 +2136,12 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -14910,7 +14919,7 @@
   <dimension ref="A1:X49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="R46" sqref="R46"/>
+      <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -14929,7 +14938,7 @@
     <col min="16" max="16" width="9.125" style="5" customWidth="1"/>
     <col min="17" max="17" width="11.375" style="6" customWidth="1"/>
     <col min="18" max="18" width="15.625" customWidth="1"/>
-    <col min="19" max="19" width="27.375" customWidth="1"/>
+    <col min="19" max="19" width="22.875" customWidth="1"/>
     <col min="20" max="20" width="23.625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="6.125" customWidth="1"/>
     <col min="22" max="22" width="5.5" customWidth="1"/>
@@ -16658,7 +16667,9 @@
       <c r="U42" s="30"/>
       <c r="V42" s="30"/>
       <c r="W42" s="30"/>
-      <c r="X42" s="30"/>
+      <c r="X42" s="30" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
@@ -16717,7 +16728,7 @@
       <c r="A46" s="13" t="s">
         <v>433</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="59" t="s">
         <v>443</v>
       </c>
       <c r="C46" s="4" t="s">
@@ -16734,7 +16745,7 @@
       </c>
       <c r="G46" s="29"/>
       <c r="H46" s="29"/>
-      <c r="I46" s="5" t="s">
+      <c r="I46" s="60" t="s">
         <v>440</v>
       </c>
       <c r="J46" s="5" t="s">
@@ -16743,7 +16754,7 @@
       <c r="K46" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="L46" s="5" t="s">
+      <c r="L46" s="60" t="s">
         <v>446</v>
       </c>
       <c r="M46" s="5" t="s">

</xml_diff>

<commit_message>
Created g2p for SLCO1B1 and tests;
</commit_message>
<xml_diff>
--- a/cpicPairs.xlsx
+++ b/cpicPairs.xlsx
@@ -20,13 +20,13 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1931" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1940" uniqueCount="463">
   <si>
     <t>Gene</t>
   </si>
@@ -1412,6 +1412,9 @@
   </si>
   <si>
     <t>need patient race as input</t>
+  </si>
+  <si>
+    <t>Variant</t>
   </si>
 </sst>
 </file>
@@ -1987,7 +1990,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2107,19 +2110,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2137,10 +2140,16 @@
     <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2189,7 +2198,42 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="103">
+  <dxfs count="108">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -6509,7 +6553,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -6632,7 +6676,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -6863,7 +6907,7 @@
     <dataField name="Count of Guideline" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="102">
+    <format dxfId="107">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6872,7 +6916,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="101">
+    <format dxfId="106">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6881,7 +6925,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="100">
+    <format dxfId="105">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6890,7 +6934,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="99">
+    <format dxfId="104">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6899,7 +6943,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="98">
+    <format dxfId="103">
       <pivotArea dataOnly="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6919,7 +6963,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:Q43" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField axis="axisCol" showAll="0">
@@ -7496,7 +7540,60 @@
   <dataFields count="1">
     <dataField name="Count of Guideline" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="98">
+  <formats count="103">
+    <format dxfId="102">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="14" selected="0">
+            <x v="36"/>
+            <x v="38"/>
+            <x v="39"/>
+            <x v="41"/>
+            <x v="42"/>
+            <x v="43"/>
+            <x v="54"/>
+            <x v="63"/>
+            <x v="64"/>
+            <x v="74"/>
+            <x v="108"/>
+            <x v="115"/>
+            <x v="118"/>
+            <x v="123"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="101">
+      <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="100">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="99">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="14">
+            <x v="36"/>
+            <x v="38"/>
+            <x v="39"/>
+            <x v="41"/>
+            <x v="42"/>
+            <x v="43"/>
+            <x v="54"/>
+            <x v="63"/>
+            <x v="64"/>
+            <x v="74"/>
+            <x v="108"/>
+            <x v="115"/>
+            <x v="118"/>
+            <x v="123"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="98">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
     <format dxfId="97">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
@@ -7553,57 +7650,32 @@
     <format dxfId="92">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
-          <reference field="0" count="14" selected="0">
-            <x v="36"/>
-            <x v="38"/>
-            <x v="39"/>
-            <x v="41"/>
-            <x v="42"/>
-            <x v="43"/>
-            <x v="54"/>
-            <x v="63"/>
-            <x v="64"/>
-            <x v="74"/>
-            <x v="108"/>
-            <x v="115"/>
-            <x v="118"/>
-            <x v="123"/>
+          <reference field="0" count="1" selected="0">
+            <x v="22"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="91">
-      <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
     </format>
     <format dxfId="90">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
     <format dxfId="89">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
-          <reference field="0" count="14">
-            <x v="36"/>
-            <x v="38"/>
-            <x v="39"/>
-            <x v="41"/>
-            <x v="42"/>
-            <x v="43"/>
-            <x v="54"/>
-            <x v="63"/>
-            <x v="64"/>
-            <x v="74"/>
-            <x v="108"/>
-            <x v="115"/>
-            <x v="118"/>
-            <x v="123"/>
+          <reference field="0" count="1">
+            <x v="22"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="88">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="87">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7612,17 +7684,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="87">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="85">
+    <format dxfId="86">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="84">
+    <format dxfId="85">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7631,7 +7703,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="84">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7640,17 +7712,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="83">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="81">
+    <format dxfId="82">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="80">
+    <format dxfId="81">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7659,44 +7731,16 @@
         </references>
       </pivotArea>
     </format>
+    <format dxfId="80">
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
+    </format>
     <format dxfId="79">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1" selected="0">
-            <x v="22"/>
-          </reference>
-        </references>
-      </pivotArea>
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
     <format dxfId="78">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="2" count="0"/>
-        </references>
-      </pivotArea>
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
     <format dxfId="77">
-      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
-    </format>
-    <format dxfId="76">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
-            <x v="22"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="75">
-      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
-    </format>
-    <format dxfId="74">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="73">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="72">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="38">
@@ -7742,8 +7786,68 @@
         </references>
       </pivotArea>
     </format>
+    <format dxfId="76">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="75">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="64"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="74">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="42"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="73">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="45"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="72">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="72"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="71">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="39"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="47"/>
+          </reference>
+        </references>
+      </pivotArea>
     </format>
     <format dxfId="70">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
@@ -7761,66 +7865,6 @@
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
-            <x v="36"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="42"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="68">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="36"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="45"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="67">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="36"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="72"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="66">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="39"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="47"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="65">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="64"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="64">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
             <x v="118"/>
           </reference>
           <reference field="1" count="1">
@@ -7829,7 +7873,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="63">
+    <format dxfId="68">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7857,7 +7901,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="62">
+    <format dxfId="67">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7888,7 +7932,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="61">
+    <format dxfId="66">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7936,7 +7980,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="60">
+    <format dxfId="65">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7950,7 +7994,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="59">
+    <format dxfId="64">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7995,7 +8039,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="58">
+    <format dxfId="63">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="12" selected="0">
@@ -8055,7 +8099,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="57">
+    <format dxfId="62">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8067,7 +8111,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="56">
+    <format dxfId="61">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8079,7 +8123,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="55">
+    <format dxfId="60">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8091,7 +8135,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="54">
+    <format dxfId="59">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8103,7 +8147,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="53">
+    <format dxfId="58">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8115,7 +8159,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="52">
+    <format dxfId="57">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8124,7 +8168,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="51">
+    <format dxfId="56">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8133,7 +8177,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="50">
+    <format dxfId="55">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8142,7 +8186,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="49">
+    <format dxfId="54">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8151,7 +8195,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="48">
+    <format dxfId="53">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8163,7 +8207,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="47">
+    <format dxfId="52">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8175,7 +8219,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="46">
+    <format dxfId="51">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8187,7 +8231,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="45">
+    <format dxfId="50">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8199,7 +8243,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="44">
+    <format dxfId="49">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8211,7 +8255,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="43">
+    <format dxfId="48">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8223,7 +8267,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="42">
+    <format dxfId="47">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -8232,7 +8276,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="41">
+    <format dxfId="46">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -8241,7 +8285,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="40">
+    <format dxfId="45">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -8250,7 +8294,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="39">
+    <format dxfId="44">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8259,7 +8303,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="43">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8268,7 +8312,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="37">
+    <format dxfId="42">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8277,7 +8321,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="36">
+    <format dxfId="41">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8286,7 +8330,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="35">
+    <format dxfId="40">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8295,7 +8339,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="34">
+    <format dxfId="39">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8304,7 +8348,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="33">
+    <format dxfId="38">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8316,7 +8360,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="37">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8325,7 +8369,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="36">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8337,7 +8381,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="35">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8349,7 +8393,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="34">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8361,7 +8405,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="33">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8370,7 +8414,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="32">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8379,7 +8423,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
+    <format dxfId="31">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8388,7 +8432,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="30">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8397,7 +8441,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="24">
+    <format dxfId="29">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8406,7 +8450,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="23">
+    <format dxfId="28">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8415,7 +8459,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="27">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8424,7 +8468,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="26">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8436,7 +8480,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="25">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8445,7 +8489,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
+    <format dxfId="24">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8454,7 +8498,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="23">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8463,7 +8507,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="22">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8472,7 +8516,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="21">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8484,7 +8528,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="20">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8496,7 +8540,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="19">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8508,7 +8552,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8517,7 +8561,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="17">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8526,7 +8570,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="16">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8538,7 +8582,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8547,7 +8591,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="14">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8559,7 +8603,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="13">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8568,7 +8612,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8577,7 +8621,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="11">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8589,7 +8633,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="10">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8598,7 +8642,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8607,7 +8651,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="8">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8616,7 +8660,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="7">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8628,7 +8672,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8637,7 +8681,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="5">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8645,6 +8689,52 @@
           </reference>
           <reference field="1" count="1">
             <x v="27"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="199"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="2">
+            <x v="153"/>
+            <x v="154"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="105"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="175"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="0">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="174"/>
           </reference>
         </references>
       </pivotArea>
@@ -8924,7 +9014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G356"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -14918,8 +15008,8 @@
   </sheetPr>
   <dimension ref="A1:X49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="S29" sqref="S29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -14929,8 +15019,8 @@
     <col min="3" max="3" width="10.375" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.125" style="5" customWidth="1"/>
     <col min="5" max="5" width="10.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="10.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.125" style="5" customWidth="1"/>
+    <col min="8" max="9" width="10.375" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="9.125" style="5" customWidth="1"/>
     <col min="12" max="12" width="10.625" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="9.125" style="5" customWidth="1"/>
@@ -15860,22 +15950,25 @@
       <c r="N22" s="23"/>
       <c r="O22" s="23"/>
       <c r="P22" s="23"/>
-      <c r="Q22" s="9">
+      <c r="Q22" s="62">
         <v>1</v>
       </c>
-      <c r="R22" t="str">
+      <c r="R22" s="44" t="str">
         <f t="shared" si="0"/>
         <v>ivacaftor</v>
       </c>
-      <c r="S22" t="s">
+      <c r="S22" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="U22" t="s">
+      <c r="T22" s="44"/>
+      <c r="U22" s="44" t="s">
         <v>427</v>
       </c>
-      <c r="V22" t="s">
+      <c r="V22" s="44" t="s">
         <v>427</v>
       </c>
+      <c r="W22" s="44"/>
+      <c r="X22" s="44"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
@@ -16103,22 +16196,25 @@
       <c r="N28" s="23"/>
       <c r="O28" s="23"/>
       <c r="P28" s="23"/>
-      <c r="Q28" s="9">
+      <c r="Q28" s="62">
         <v>1</v>
       </c>
-      <c r="R28" t="str">
+      <c r="R28" s="44" t="str">
         <f t="shared" si="0"/>
         <v>peginterferon alfa-2a</v>
       </c>
-      <c r="S28" t="s">
+      <c r="S28" s="44" t="s">
         <v>414</v>
       </c>
-      <c r="U28" t="s">
+      <c r="T28" s="44"/>
+      <c r="U28" s="44" t="s">
         <v>427</v>
       </c>
-      <c r="V28" t="s">
+      <c r="V28" s="44" t="s">
         <v>427</v>
       </c>
+      <c r="W28" s="44"/>
+      <c r="X28" s="44"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
@@ -16141,22 +16237,25 @@
       <c r="N29" s="23"/>
       <c r="O29" s="23"/>
       <c r="P29" s="23"/>
-      <c r="Q29" s="9">
+      <c r="Q29" s="62">
         <v>1</v>
       </c>
-      <c r="R29" t="str">
+      <c r="R29" s="44" t="str">
         <f t="shared" si="0"/>
         <v>peginterferon alfa-2b</v>
       </c>
-      <c r="S29" t="s">
+      <c r="S29" s="44" t="s">
         <v>414</v>
       </c>
-      <c r="U29" t="s">
+      <c r="T29" s="44"/>
+      <c r="U29" s="44" t="s">
         <v>427</v>
       </c>
-      <c r="V29" t="s">
+      <c r="V29" s="44" t="s">
         <v>427</v>
       </c>
+      <c r="W29" s="44"/>
+      <c r="X29" s="44"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
@@ -16219,22 +16318,25 @@
       <c r="N31" s="23"/>
       <c r="O31" s="23"/>
       <c r="P31" s="23"/>
-      <c r="Q31" s="9">
+      <c r="Q31" s="62">
         <v>1</v>
       </c>
-      <c r="R31" t="str">
+      <c r="R31" s="44" t="str">
         <f t="shared" si="0"/>
         <v>rasburicase</v>
       </c>
-      <c r="S31" t="s">
+      <c r="S31" s="44" t="s">
         <v>418</v>
       </c>
-      <c r="U31" t="s">
+      <c r="T31" s="44"/>
+      <c r="U31" s="44" t="s">
         <v>427</v>
       </c>
-      <c r="V31" t="s">
+      <c r="V31" s="44" t="s">
         <v>427</v>
       </c>
+      <c r="W31" s="44"/>
+      <c r="X31" s="44"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
@@ -16257,22 +16359,25 @@
       <c r="N32" s="23"/>
       <c r="O32" s="23"/>
       <c r="P32" s="23"/>
-      <c r="Q32" s="9">
+      <c r="Q32" s="62">
         <v>1</v>
       </c>
-      <c r="R32" t="str">
+      <c r="R32" s="44" t="str">
         <f t="shared" si="0"/>
         <v>ribavirin</v>
       </c>
-      <c r="S32" t="s">
+      <c r="S32" s="44" t="s">
         <v>414</v>
       </c>
-      <c r="U32" t="s">
+      <c r="T32" s="44"/>
+      <c r="U32" s="44" t="s">
         <v>427</v>
       </c>
-      <c r="V32" t="s">
+      <c r="V32" s="44" t="s">
         <v>427</v>
       </c>
+      <c r="W32" s="44"/>
+      <c r="X32" s="44"/>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
@@ -16409,7 +16514,7 @@
       <c r="N36" s="23"/>
       <c r="O36" s="23"/>
       <c r="P36" s="23"/>
-      <c r="Q36" s="9">
+      <c r="Q36" s="62">
         <v>1</v>
       </c>
       <c r="R36" s="44" t="str">
@@ -16728,7 +16833,7 @@
       <c r="A46" s="13" t="s">
         <v>433</v>
       </c>
-      <c r="B46" s="59" t="s">
+      <c r="B46" s="49" t="s">
         <v>443</v>
       </c>
       <c r="C46" s="4" t="s">
@@ -16743,9 +16848,13 @@
       <c r="F46" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="G46" s="29"/>
-      <c r="H46" s="29"/>
-      <c r="I46" s="60" t="s">
+      <c r="G46" s="61" t="s">
+        <v>437</v>
+      </c>
+      <c r="H46" s="61" t="s">
+        <v>462</v>
+      </c>
+      <c r="I46" s="50" t="s">
         <v>440</v>
       </c>
       <c r="J46" s="5" t="s">
@@ -16754,7 +16863,7 @@
       <c r="K46" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="L46" s="60" t="s">
+      <c r="L46" s="50" t="s">
         <v>446</v>
       </c>
       <c r="M46" s="5" t="s">
@@ -16766,7 +16875,9 @@
       <c r="O46" s="46" t="s">
         <v>437</v>
       </c>
-      <c r="P46" s="29"/>
+      <c r="P46" s="61" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
@@ -16787,8 +16898,12 @@
       <c r="F47" s="5" t="s">
         <v>441</v>
       </c>
-      <c r="G47" s="29"/>
-      <c r="H47" s="29"/>
+      <c r="G47" s="61" t="s">
+        <v>441</v>
+      </c>
+      <c r="H47" s="61" t="s">
+        <v>441</v>
+      </c>
       <c r="I47" s="5" t="s">
         <v>441</v>
       </c>
@@ -16810,7 +16925,9 @@
       <c r="O47" s="46" t="s">
         <v>441</v>
       </c>
-      <c r="P47" s="29"/>
+      <c r="P47" s="61" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
@@ -16825,8 +16942,10 @@
       <c r="F48" s="5" t="s">
         <v>436</v>
       </c>
-      <c r="G48" s="29"/>
-      <c r="H48" s="29"/>
+      <c r="G48" s="61" t="s">
+        <v>436</v>
+      </c>
+      <c r="H48" s="61"/>
       <c r="I48" s="29"/>
       <c r="J48" s="29"/>
       <c r="K48" s="29"/>
@@ -16838,7 +16957,9 @@
         <v>436</v>
       </c>
       <c r="O48" s="29"/>
-      <c r="P48" s="29"/>
+      <c r="P48" s="61" t="s">
+        <v>436</v>
+      </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="13" t="s">
@@ -16855,8 +16976,10 @@
         <v>438</v>
       </c>
       <c r="F49" s="29"/>
-      <c r="G49" s="29"/>
-      <c r="H49" s="29"/>
+      <c r="G49" s="61"/>
+      <c r="H49" s="61" t="s">
+        <v>438</v>
+      </c>
       <c r="I49" s="5" t="s">
         <v>442</v>
       </c>
@@ -16929,18 +17052,18 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="51" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="53" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
+      <c r="A5" s="52"/>
       <c r="B5" s="15" t="s">
         <v>21</v>
       </c>
@@ -17009,18 +17132,18 @@
       <c r="C11" s="58"/>
     </row>
     <row r="12" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="51" t="s">
         <v>115</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="53" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
+      <c r="A13" s="52"/>
       <c r="B13" s="15" t="s">
         <v>21</v>
       </c>
@@ -17060,18 +17183,18 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="51" t="s">
         <v>122</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="C17" s="53" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="53"/>
+      <c r="A18" s="52"/>
       <c r="B18" s="15" t="s">
         <v>21</v>
       </c>
@@ -17187,10 +17310,10 @@
       <c r="A29" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="B29" s="49" t="s">
+      <c r="B29" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="51" t="s">
+      <c r="C29" s="53" t="s">
         <v>407</v>
       </c>
     </row>
@@ -17198,14 +17321,14 @@
       <c r="A30" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="50"/>
-      <c r="C30" s="52"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="60"/>
     </row>
     <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="53"/>
+      <c r="B31" s="52"/>
       <c r="C31" s="54"/>
     </row>
     <row r="32" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
@@ -17344,32 +17467,38 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="49" t="s">
+      <c r="A45" s="51" t="s">
         <v>87</v>
       </c>
       <c r="B45" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C45" s="51" t="s">
+      <c r="C45" s="53" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="50"/>
+      <c r="A46" s="59"/>
       <c r="B46" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="52"/>
+      <c r="C46" s="60"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="50"/>
+      <c r="A47" s="59"/>
       <c r="B47" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="52"/>
+      <c r="C47" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="C32:C33"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B10:B11"/>
@@ -17382,12 +17511,6 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="C32:C33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://cpicpgx.org/guidelines/guideline-for-abacavir-and-hla-b/"/>

</xml_diff>

<commit_message>
Created recommendation for voriconazole (CYP2C19)
</commit_message>
<xml_diff>
--- a/cpicPairs.xlsx
+++ b/cpicPairs.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1940" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1950" uniqueCount="472">
   <si>
     <t>Gene</t>
   </si>
@@ -1415,6 +1415,33 @@
   </si>
   <si>
     <t>Variant</t>
+  </si>
+  <si>
+    <t>/99999/fk4mc97w0h/v0.0.4</t>
+  </si>
+  <si>
+    <t>/99999/fk49z9gr7p/v0.0.6</t>
+  </si>
+  <si>
+    <t>/99999/fk4md04x9z/v0.0.1</t>
+  </si>
+  <si>
+    <t>/99999/fk47380j09/v0.0.1</t>
+  </si>
+  <si>
+    <t>/99999-fk4vq45s09/v0.0.1</t>
+  </si>
+  <si>
+    <t>/99999/fk47h1x090/v0.0.4</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>/99999/fk4bv8qb3r/v0.0.1</t>
+  </si>
+  <si>
+    <t>/99999/fk4cz4fm8f/v0.0.1</t>
   </si>
 </sst>
 </file>
@@ -1990,7 +2017,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2152,6 +2179,21 @@
     <xf numFmtId="0" fontId="0" fillId="40" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="135"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2198,7 +2240,14 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="108">
+  <dxfs count="109">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -6907,7 +6956,7 @@
     <dataField name="Count of Guideline" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="107">
+    <format dxfId="108">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6916,7 +6965,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="106">
+    <format dxfId="107">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6925,7 +6974,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="105">
+    <format dxfId="106">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6934,7 +6983,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="104">
+    <format dxfId="105">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6943,7 +6992,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="103">
+    <format dxfId="104">
       <pivotArea dataOnly="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7540,8 +7589,8 @@
   <dataFields count="1">
     <dataField name="Count of Guideline" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="103">
-    <format dxfId="102">
+  <formats count="104">
+    <format dxfId="103">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14" selected="0">
@@ -7563,13 +7612,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="101">
+    <format dxfId="102">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="100">
+    <format dxfId="101">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="99">
+    <format dxfId="100">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14">
@@ -7591,10 +7640,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="98">
+    <format dxfId="99">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="97">
+    <format dxfId="98">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14" selected="0">
@@ -7616,13 +7665,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="96">
+    <format dxfId="97">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="95">
+    <format dxfId="96">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="94">
+    <format dxfId="95">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14">
@@ -7644,10 +7693,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="93">
+    <format dxfId="94">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="92">
+    <format dxfId="93">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7656,17 +7705,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="91">
+    <format dxfId="92">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="90">
+    <format dxfId="91">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="89">
+    <format dxfId="90">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7675,7 +7724,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="89">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7684,17 +7733,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="88">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="87">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="85">
+    <format dxfId="86">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7703,7 +7752,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="84">
+    <format dxfId="85">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7712,17 +7761,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="84">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="83">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="81">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7731,16 +7780,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
+    <format dxfId="81">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="79">
+    <format dxfId="80">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="78">
+    <format dxfId="79">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="77">
+    <format dxfId="78">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="38">
@@ -7786,10 +7835,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="76">
+    <format dxfId="77">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="75">
+    <format dxfId="76">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7801,7 +7850,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="75">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7813,7 +7862,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
+    <format dxfId="74">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7825,7 +7874,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="72">
+    <format dxfId="73">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7837,7 +7886,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="72">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7849,7 +7898,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
+    <format dxfId="71">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7861,7 +7910,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="69">
+    <format dxfId="70">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7873,7 +7922,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="69">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7901,7 +7950,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="67">
+    <format dxfId="68">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7932,7 +7981,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="66">
+    <format dxfId="67">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7980,7 +8029,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="65">
+    <format dxfId="66">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7994,7 +8043,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="64">
+    <format dxfId="65">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8039,7 +8088,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="63">
+    <format dxfId="64">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="12" selected="0">
@@ -8099,7 +8148,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="62">
+    <format dxfId="63">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8111,7 +8160,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="61">
+    <format dxfId="62">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8123,7 +8172,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="60">
+    <format dxfId="61">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8135,7 +8184,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="59">
+    <format dxfId="60">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8147,7 +8196,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="58">
+    <format dxfId="59">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8159,7 +8208,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="57">
+    <format dxfId="58">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8168,7 +8217,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="56">
+    <format dxfId="57">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8177,7 +8226,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="55">
+    <format dxfId="56">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8186,11 +8235,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="54">
+    <format dxfId="55">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
             <x v="221"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="54">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="43"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="25"/>
           </reference>
         </references>
       </pivotArea>
@@ -8202,7 +8263,7 @@
             <x v="43"/>
           </reference>
           <reference field="1" count="1">
-            <x v="25"/>
+            <x v="80"/>
           </reference>
         </references>
       </pivotArea>
@@ -8214,24 +8275,12 @@
             <x v="43"/>
           </reference>
           <reference field="1" count="1">
-            <x v="80"/>
+            <x v="201"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="51">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="43"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="201"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="50">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8243,7 +8292,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="49">
+    <format dxfId="50">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8255,7 +8304,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="48">
+    <format dxfId="49">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8267,7 +8316,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="47">
+    <format dxfId="48">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -8276,7 +8325,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="46">
+    <format dxfId="47">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -8285,7 +8334,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="45">
+    <format dxfId="46">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -8294,7 +8343,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="44">
+    <format dxfId="45">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8303,7 +8352,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="43">
+    <format dxfId="44">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8312,7 +8361,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="42">
+    <format dxfId="43">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8321,7 +8370,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="41">
+    <format dxfId="42">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8330,7 +8379,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="40">
+    <format dxfId="41">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8339,7 +8388,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="39">
+    <format dxfId="40">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8348,7 +8397,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="39">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8360,11 +8409,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="37">
+    <format dxfId="38">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
             <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="37">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="44"/>
           </reference>
         </references>
       </pivotArea>
@@ -8376,12 +8437,147 @@
             <x v="36"/>
           </reference>
           <reference field="1" count="1">
-            <x v="44"/>
+            <x v="7"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="35">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="39"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="34">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="33">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="32">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="31">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="42"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="30">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="45"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="29">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="47"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="28">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="72"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="27">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="64"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="26">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="25">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="24">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="23">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="22">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="39"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="21">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8393,154 +8589,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="34">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="39"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="33">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="32">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="31">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="14"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="30">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="42"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="29">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="45"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="28">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="47"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="27">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="72"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="26">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="64"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="25">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="24">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="23">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="22">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="21">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="39"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
     <format dxfId="20">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="36"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="19">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8552,7 +8601,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8561,7 +8610,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="18">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8570,7 +8619,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="17">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8582,7 +8631,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="16">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8591,7 +8640,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="15">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8603,7 +8652,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="14">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8612,7 +8661,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8621,7 +8670,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="12">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8633,7 +8682,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="11">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8642,7 +8691,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8651,7 +8700,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="9">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8660,7 +8709,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="8">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8672,7 +8721,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8681,7 +8730,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="6">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8693,7 +8742,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="5">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8702,7 +8751,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="4">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="2">
@@ -8712,7 +8761,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="3">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8721,7 +8770,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="2">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8730,11 +8779,20 @@
         </references>
       </pivotArea>
     </format>
+    <format dxfId="1">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="174"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="0">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="174"/>
+            <x v="219"/>
           </reference>
         </references>
       </pivotArea>
@@ -15006,10 +15064,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:X49"/>
+  <dimension ref="A1:X50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="S33" sqref="S33"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="T41" sqref="T41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -16716,22 +16774,27 @@
       <c r="N41" s="23"/>
       <c r="O41" s="23"/>
       <c r="P41" s="23"/>
-      <c r="Q41" s="9">
+      <c r="Q41" s="32">
         <v>1</v>
       </c>
-      <c r="R41" t="str">
+      <c r="R41" s="35" t="str">
         <f t="shared" si="0"/>
         <v>voriconazole</v>
       </c>
-      <c r="S41" t="s">
+      <c r="S41" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="U41" t="s">
+      <c r="T41" s="35" t="s">
+        <v>471</v>
+      </c>
+      <c r="U41" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="V41" t="s">
+      <c r="V41" s="35" t="s">
         <v>427</v>
       </c>
+      <c r="W41" s="35"/>
+      <c r="X41" s="35"/>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="27" t="s">
@@ -16994,6 +17057,42 @@
         <v>438</v>
       </c>
       <c r="P49" s="29"/>
+    </row>
+    <row r="50" spans="1:16" ht="159" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="63"/>
+      <c r="B50" s="63"/>
+      <c r="C50" s="63" t="s">
+        <v>463</v>
+      </c>
+      <c r="D50" s="64" t="s">
+        <v>470</v>
+      </c>
+      <c r="E50" s="64" t="s">
+        <v>464</v>
+      </c>
+      <c r="F50" s="64" t="s">
+        <v>465</v>
+      </c>
+      <c r="G50" s="66"/>
+      <c r="H50" s="66"/>
+      <c r="I50" s="64"/>
+      <c r="J50" s="65" t="s">
+        <v>469</v>
+      </c>
+      <c r="K50" s="65" t="s">
+        <v>469</v>
+      </c>
+      <c r="L50" s="64"/>
+      <c r="M50" s="64" t="s">
+        <v>466</v>
+      </c>
+      <c r="N50" s="64" t="s">
+        <v>467</v>
+      </c>
+      <c r="O50" s="64" t="s">
+        <v>468</v>
+      </c>
+      <c r="P50" s="67"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Created three recommendation KOs for TPMT; Updated druglist KO;
</commit_message>
<xml_diff>
--- a/cpicPairs.xlsx
+++ b/cpicPairs.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1951" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1954" uniqueCount="476">
   <si>
     <t>Gene</t>
   </si>
@@ -1445,6 +1445,15 @@
   </si>
   <si>
     <t>/99999/fk4qz3fz89/v0.0.1</t>
+  </si>
+  <si>
+    <t>/99999/fk4r225c4h/v0.0.1</t>
+  </si>
+  <si>
+    <t>/99999/fk4cx5fm8f/v0.0.1</t>
+  </si>
+  <si>
+    <t>/99999/fk4m91fj9z/v0.0.1</t>
   </si>
 </sst>
 </file>
@@ -2243,7 +2252,14 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="110">
+  <dxfs count="111">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -6966,7 +6982,7 @@
     <dataField name="Count of Guideline" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="109">
+    <format dxfId="110">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6975,7 +6991,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="108">
+    <format dxfId="109">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6984,7 +7000,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="107">
+    <format dxfId="108">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6993,7 +7009,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="106">
+    <format dxfId="107">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7002,7 +7018,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="105">
+    <format dxfId="106">
       <pivotArea dataOnly="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7599,8 +7615,8 @@
   <dataFields count="1">
     <dataField name="Count of Guideline" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="105">
-    <format dxfId="104">
+  <formats count="106">
+    <format dxfId="105">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14" selected="0">
@@ -7622,13 +7638,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="103">
+    <format dxfId="104">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="102">
+    <format dxfId="103">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="101">
+    <format dxfId="102">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14">
@@ -7650,10 +7666,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="100">
+    <format dxfId="101">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="99">
+    <format dxfId="100">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14" selected="0">
@@ -7675,13 +7691,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="98">
+    <format dxfId="99">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="97">
+    <format dxfId="98">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="96">
+    <format dxfId="97">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14">
@@ -7703,10 +7719,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="95">
+    <format dxfId="96">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="94">
+    <format dxfId="95">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7715,17 +7731,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="93">
+    <format dxfId="94">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="92">
+    <format dxfId="93">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="91">
+    <format dxfId="92">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7734,7 +7750,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="90">
+    <format dxfId="91">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7743,17 +7759,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="89">
+    <format dxfId="90">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="89">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="87">
+    <format dxfId="88">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7762,7 +7778,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="87">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7771,17 +7787,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="85">
+    <format dxfId="86">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="84">
+    <format dxfId="85">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="83">
+    <format dxfId="84">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7790,16 +7806,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="83">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="81">
+    <format dxfId="82">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="80">
+    <format dxfId="81">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="79">
+    <format dxfId="80">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="38">
@@ -7845,10 +7861,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="79">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="77">
+    <format dxfId="78">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7860,7 +7876,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="76">
+    <format dxfId="77">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7872,7 +7888,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="76">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7884,7 +7900,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="75">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7896,7 +7912,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
+    <format dxfId="74">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7908,7 +7924,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="72">
+    <format dxfId="73">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7920,7 +7936,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="72">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7932,7 +7948,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
+    <format dxfId="71">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7960,7 +7976,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="69">
+    <format dxfId="70">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7991,7 +8007,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="69">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8039,7 +8055,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="67">
+    <format dxfId="68">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8053,7 +8069,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="66">
+    <format dxfId="67">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8098,7 +8114,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="65">
+    <format dxfId="66">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="12" selected="0">
@@ -8158,7 +8174,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="64">
+    <format dxfId="65">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8170,7 +8186,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="63">
+    <format dxfId="64">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8182,7 +8198,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="62">
+    <format dxfId="63">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8194,7 +8210,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="61">
+    <format dxfId="62">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8206,7 +8222,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="60">
+    <format dxfId="61">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8218,7 +8234,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="59">
+    <format dxfId="60">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8227,7 +8243,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="58">
+    <format dxfId="59">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8236,7 +8252,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="57">
+    <format dxfId="58">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8245,11 +8261,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="56">
+    <format dxfId="57">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
             <x v="221"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="56">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="43"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="25"/>
           </reference>
         </references>
       </pivotArea>
@@ -8261,7 +8289,7 @@
             <x v="43"/>
           </reference>
           <reference field="1" count="1">
-            <x v="25"/>
+            <x v="80"/>
           </reference>
         </references>
       </pivotArea>
@@ -8273,24 +8301,12 @@
             <x v="43"/>
           </reference>
           <reference field="1" count="1">
-            <x v="80"/>
+            <x v="201"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="53">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="43"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="201"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="52">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8302,7 +8318,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="51">
+    <format dxfId="52">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8314,7 +8330,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="50">
+    <format dxfId="51">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8326,7 +8342,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="49">
+    <format dxfId="50">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -8335,7 +8351,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="48">
+    <format dxfId="49">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -8344,7 +8360,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="47">
+    <format dxfId="48">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -8353,7 +8369,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="46">
+    <format dxfId="47">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8362,7 +8378,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="45">
+    <format dxfId="46">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8371,7 +8387,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="44">
+    <format dxfId="45">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8380,7 +8396,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="43">
+    <format dxfId="44">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8389,7 +8405,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="42">
+    <format dxfId="43">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8398,7 +8414,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="41">
+    <format dxfId="42">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8407,7 +8423,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="40">
+    <format dxfId="41">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8419,11 +8435,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="39">
+    <format dxfId="40">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
             <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="39">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="44"/>
           </reference>
         </references>
       </pivotArea>
@@ -8435,12 +8463,147 @@
             <x v="36"/>
           </reference>
           <reference field="1" count="1">
-            <x v="44"/>
+            <x v="7"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="37">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="39"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="36">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="35">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="34">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="33">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="42"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="32">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="45"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="31">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="47"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="30">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="72"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="29">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="64"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="28">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="27">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="26">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="25">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="24">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="39"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="23">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8452,154 +8615,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="36">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="39"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="35">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="34">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="33">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="14"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="32">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="42"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="31">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="45"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="30">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="47"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="29">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="72"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="28">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="64"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="27">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="26">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="25">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="24">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="23">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="39"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
     <format dxfId="22">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="36"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="21">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8611,7 +8627,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8620,7 +8636,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
+    <format dxfId="20">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8629,7 +8645,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="19">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8641,7 +8657,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8650,7 +8666,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="17">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8662,7 +8678,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="16">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8671,7 +8687,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8680,7 +8696,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="14">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8692,7 +8708,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="13">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8701,7 +8717,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8710,7 +8726,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="11">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8719,7 +8735,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="10">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8731,7 +8747,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8740,7 +8756,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="8">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8752,7 +8768,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="7">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8761,7 +8777,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="6">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="2">
@@ -8771,7 +8787,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="5">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8780,7 +8796,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="4">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8789,7 +8805,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="3">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8798,7 +8814,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="2">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8807,11 +8823,20 @@
         </references>
       </pivotArea>
     </format>
+    <format dxfId="1">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="159"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="0">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="159"/>
+            <x v="205"/>
           </reference>
         </references>
       </pivotArea>
@@ -15085,8 +15110,8 @@
   </sheetPr>
   <dimension ref="A1:X50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T30" sqref="T30"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -15488,22 +15513,27 @@
       </c>
       <c r="O9" s="23"/>
       <c r="P9" s="23"/>
-      <c r="Q9" s="9">
+      <c r="Q9" s="32">
         <v>1</v>
       </c>
-      <c r="R9" t="str">
+      <c r="R9" s="35" t="str">
         <f t="shared" si="0"/>
         <v>azathioprine</v>
       </c>
-      <c r="S9" t="s">
+      <c r="S9" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="U9" s="47" t="s">
+      <c r="T9" s="35" t="s">
+        <v>473</v>
+      </c>
+      <c r="U9" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="V9" s="47" t="s">
+      <c r="V9" s="35" t="s">
         <v>452</v>
       </c>
+      <c r="W9" s="35"/>
+      <c r="X9" s="35"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
@@ -16068,22 +16098,27 @@
       </c>
       <c r="O23" s="23"/>
       <c r="P23" s="23"/>
-      <c r="Q23" s="9">
+      <c r="Q23" s="32">
         <v>1</v>
       </c>
-      <c r="R23" t="str">
+      <c r="R23" s="35" t="str">
         <f t="shared" si="0"/>
         <v>mercaptopurine</v>
       </c>
-      <c r="S23" t="s">
+      <c r="S23" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="U23" t="s">
+      <c r="T23" s="35" t="s">
+        <v>475</v>
+      </c>
+      <c r="U23" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="V23" t="s">
+      <c r="V23" s="35" t="s">
         <v>452</v>
       </c>
+      <c r="W23" s="35"/>
+      <c r="X23" s="35"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
@@ -16676,22 +16711,27 @@
       </c>
       <c r="O38" s="23"/>
       <c r="P38" s="23"/>
-      <c r="Q38" s="9">
+      <c r="Q38" s="32">
         <v>1</v>
       </c>
-      <c r="R38" t="str">
+      <c r="R38" s="35" t="str">
         <f t="shared" si="0"/>
         <v>thioguanine</v>
       </c>
-      <c r="S38" t="s">
+      <c r="S38" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="U38" t="s">
+      <c r="T38" s="35" t="s">
+        <v>474</v>
+      </c>
+      <c r="U38" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="V38" t="s">
+      <c r="V38" s="35" t="s">
         <v>452</v>
       </c>
+      <c r="W38" s="35"/>
+      <c r="X38" s="35"/>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">

</xml_diff>

<commit_message>
Created recommendation KOs for CYP3A5 and SLCO1B1; Updated druglist KO
</commit_message>
<xml_diff>
--- a/cpicPairs.xlsx
+++ b/cpicPairs.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1954" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1957" uniqueCount="479">
   <si>
     <t>Gene</t>
   </si>
@@ -1454,13 +1454,22 @@
   </si>
   <si>
     <t>/99999/fk4m91fj9z/v0.0.1</t>
+  </si>
+  <si>
+    <t>/99999/fk40k3kt35/v0.0.1</t>
+  </si>
+  <si>
+    <t>/99999/fk4m95ek9z/v0.0.1</t>
+  </si>
+  <si>
+    <t>/99999/fk4t85em9x/v0.0.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1588,6 +1597,12 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2029,7 +2044,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2206,6 +2221,7 @@
     <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2252,7 +2268,28 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="111">
+  <dxfs count="114">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -6982,7 +7019,7 @@
     <dataField name="Count of Guideline" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="110">
+    <format dxfId="113">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -6991,7 +7028,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="109">
+    <format dxfId="112">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7000,7 +7037,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="108">
+    <format dxfId="111">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7009,7 +7046,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="107">
+    <format dxfId="110">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7018,7 +7055,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="106">
+    <format dxfId="109">
       <pivotArea dataOnly="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7615,8 +7652,8 @@
   <dataFields count="1">
     <dataField name="Count of Guideline" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="106">
-    <format dxfId="105">
+  <formats count="109">
+    <format dxfId="108">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14" selected="0">
@@ -7638,13 +7675,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="104">
+    <format dxfId="107">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="103">
+    <format dxfId="106">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="102">
+    <format dxfId="105">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14">
@@ -7666,10 +7703,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="101">
+    <format dxfId="104">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="100">
+    <format dxfId="103">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14" selected="0">
@@ -7691,13 +7728,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="99">
+    <format dxfId="102">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="98">
+    <format dxfId="101">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="97">
+    <format dxfId="100">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14">
@@ -7719,10 +7756,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="96">
+    <format dxfId="99">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="95">
+    <format dxfId="98">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7731,17 +7768,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="94">
+    <format dxfId="97">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="93">
+    <format dxfId="96">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="92">
+    <format dxfId="95">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7750,7 +7787,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="91">
+    <format dxfId="94">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7759,17 +7796,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="90">
+    <format dxfId="93">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="89">
+    <format dxfId="92">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="88">
+    <format dxfId="91">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7778,7 +7815,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="90">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7787,17 +7824,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="89">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="85">
+    <format dxfId="88">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="84">
+    <format dxfId="87">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7806,16 +7843,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="86">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="82">
+    <format dxfId="85">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="81">
+    <format dxfId="84">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="80">
+    <format dxfId="83">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="38">
@@ -7861,10 +7898,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="78">
+    <format dxfId="81">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7876,7 +7913,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="80">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7888,7 +7925,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="76">
+    <format dxfId="79">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7900,7 +7937,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="78">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7912,7 +7949,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="77">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7924,7 +7961,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
+    <format dxfId="76">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7936,7 +7973,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="72">
+    <format dxfId="75">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7948,7 +7985,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="74">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7976,7 +8013,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
+    <format dxfId="73">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8007,7 +8044,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="69">
+    <format dxfId="72">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8055,7 +8092,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="71">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8069,7 +8106,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="67">
+    <format dxfId="70">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8114,7 +8151,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="66">
+    <format dxfId="69">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="12" selected="0">
@@ -8174,7 +8211,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="65">
+    <format dxfId="68">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8186,7 +8223,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="64">
+    <format dxfId="67">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8198,7 +8235,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="63">
+    <format dxfId="66">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8210,7 +8247,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="62">
+    <format dxfId="65">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8222,7 +8259,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="61">
+    <format dxfId="64">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8234,7 +8271,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="60">
+    <format dxfId="63">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8243,7 +8280,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="59">
+    <format dxfId="62">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8252,7 +8289,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="58">
+    <format dxfId="61">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8261,7 +8298,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="57">
+    <format dxfId="60">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8270,7 +8307,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="56">
+    <format dxfId="59">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8282,7 +8319,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="55">
+    <format dxfId="58">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8294,7 +8331,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="54">
+    <format dxfId="57">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8306,7 +8343,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="53">
+    <format dxfId="56">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8318,7 +8355,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="52">
+    <format dxfId="55">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8330,7 +8367,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="51">
+    <format dxfId="54">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8342,7 +8379,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="50">
+    <format dxfId="53">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -8351,7 +8388,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="49">
+    <format dxfId="52">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -8360,7 +8397,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="48">
+    <format dxfId="51">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -8369,7 +8406,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="47">
+    <format dxfId="50">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8378,7 +8415,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="46">
+    <format dxfId="49">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8387,7 +8424,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="45">
+    <format dxfId="48">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8396,7 +8433,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="44">
+    <format dxfId="47">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8405,7 +8442,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="43">
+    <format dxfId="46">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8414,7 +8451,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="42">
+    <format dxfId="45">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8423,7 +8460,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="41">
+    <format dxfId="44">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8435,7 +8472,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="40">
+    <format dxfId="43">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8444,7 +8481,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="39">
+    <format dxfId="42">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8456,7 +8493,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="41">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8468,7 +8505,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="37">
+    <format dxfId="40">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8480,7 +8517,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="36">
+    <format dxfId="39">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8489,7 +8526,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="35">
+    <format dxfId="38">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8498,7 +8535,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="34">
+    <format dxfId="37">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8507,7 +8544,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="33">
+    <format dxfId="36">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8516,7 +8553,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="35">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8525,7 +8562,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="34">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8534,7 +8571,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="33">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8543,7 +8580,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="32">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8555,7 +8592,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8564,7 +8601,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="30">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8573,7 +8610,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
+    <format dxfId="29">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8582,7 +8619,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="28">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8591,7 +8628,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="24">
+    <format dxfId="27">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8603,7 +8640,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="23">
+    <format dxfId="26">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8615,7 +8652,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="25">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8627,7 +8664,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="24">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8636,7 +8673,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="23">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8645,7 +8682,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
+    <format dxfId="22">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8657,11 +8694,41 @@
         </references>
       </pivotArea>
     </format>
+    <format dxfId="21">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="144"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="20">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="39"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="144"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="19">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="144"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="144"/>
+            <x v="213"/>
           </reference>
         </references>
       </pivotArea>
@@ -8673,7 +8740,7 @@
             <x v="39"/>
           </reference>
           <reference field="1" count="1">
-            <x v="144"/>
+            <x v="213"/>
           </reference>
         </references>
       </pivotArea>
@@ -8682,7 +8749,7 @@
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="144"/>
+            <x v="213"/>
           </reference>
         </references>
       </pivotArea>
@@ -8691,42 +8758,12 @@
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="213"/>
+            <x v="199"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="14">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="39"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="213"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="13">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="213"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="12">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="199"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="11">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8735,7 +8772,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="13">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8747,7 +8784,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8756,7 +8793,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="11">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8768,7 +8805,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="10">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8777,7 +8814,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="9">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="2">
@@ -8787,7 +8824,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="8">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8796,7 +8833,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="7">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8805,7 +8842,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="6">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8814,7 +8851,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="5">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8823,7 +8860,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="4">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -8832,11 +8869,38 @@
         </references>
       </pivotArea>
     </format>
+    <format dxfId="3">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="205"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="183"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="186"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="0">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="205"/>
+            <x v="198"/>
           </reference>
         </references>
       </pivotArea>
@@ -15110,8 +15174,8 @@
   </sheetPr>
   <dimension ref="A1:X50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="X28" sqref="X28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -16517,22 +16581,27 @@
       <c r="N33" s="23"/>
       <c r="O33" s="23"/>
       <c r="P33" s="23"/>
-      <c r="Q33" s="9">
+      <c r="Q33" s="32">
         <v>1</v>
       </c>
-      <c r="R33" t="str">
+      <c r="R33" s="35" t="str">
         <f t="shared" si="0"/>
         <v>sertraline</v>
       </c>
-      <c r="S33" t="s">
+      <c r="S33" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="U33" t="s">
+      <c r="T33" s="35" t="s">
+        <v>476</v>
+      </c>
+      <c r="U33" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="V33" t="s">
+      <c r="V33" s="35" t="s">
         <v>427</v>
       </c>
+      <c r="W33" s="35"/>
+      <c r="X33" s="35"/>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
@@ -16555,22 +16624,27 @@
       <c r="N34" s="23"/>
       <c r="O34" s="23"/>
       <c r="P34" s="23"/>
-      <c r="Q34" s="9">
+      <c r="Q34" s="32">
         <v>1</v>
       </c>
-      <c r="R34" t="str">
+      <c r="R34" s="35" t="str">
         <f t="shared" si="0"/>
         <v>simvastatin</v>
       </c>
-      <c r="S34" t="s">
+      <c r="S34" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="U34" t="s">
+      <c r="T34" s="35" t="s">
+        <v>477</v>
+      </c>
+      <c r="U34" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="V34" t="s">
+      <c r="V34" s="35" t="s">
         <v>452</v>
       </c>
+      <c r="W34" s="35"/>
+      <c r="X34" s="35"/>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
@@ -16593,22 +16667,27 @@
       <c r="N35" s="23"/>
       <c r="O35" s="23"/>
       <c r="P35" s="23"/>
-      <c r="Q35" s="9">
+      <c r="Q35" s="32">
         <v>1</v>
       </c>
-      <c r="R35" t="str">
+      <c r="R35" s="35" t="str">
         <f t="shared" si="0"/>
         <v>tacrolimus</v>
       </c>
-      <c r="S35" t="s">
+      <c r="S35" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="U35" t="s">
+      <c r="T35" s="35" t="s">
+        <v>478</v>
+      </c>
+      <c r="U35" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="V35" t="s">
+      <c r="V35" s="35" t="s">
         <v>452</v>
       </c>
+      <c r="W35" s="35"/>
+      <c r="X35" s="35"/>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="45" t="s">
@@ -16899,7 +16978,7 @@
       <c r="U42" s="30"/>
       <c r="V42" s="30"/>
       <c r="W42" s="30"/>
-      <c r="X42" s="30" t="s">
+      <c r="X42" s="68" t="s">
         <v>461</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified 99999-fk4t167482/v0.0.1/model/resource/recommendation.js to cover the scenarios where only one gene is present.
</commit_message>
<xml_diff>
--- a/cpicPairs.xlsx
+++ b/cpicPairs.xlsx
@@ -1613,7 +1613,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1835,14 +1835,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -2004,6 +1998,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2050,7 +2057,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2120,12 +2127,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2159,10 +2160,6 @@
     <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2170,16 +2167,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2197,19 +2185,20 @@
     <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="135"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2227,7 +2216,36 @@
     <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2274,7 +2292,487 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="114">
+  <dxfs count="190">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -7025,7 +7523,7 @@
     <dataField name="Count of Guideline" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="113">
+    <format dxfId="189">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7034,7 +7532,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="112">
+    <format dxfId="188">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7043,7 +7541,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="111">
+    <format dxfId="187">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7052,7 +7550,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="110">
+    <format dxfId="186">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7061,7 +7559,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="109">
+    <format dxfId="185">
       <pivotArea dataOnly="0" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7658,8 +8156,8 @@
   <dataFields count="1">
     <dataField name="Count of Guideline" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="109">
-    <format dxfId="108">
+  <formats count="185">
+    <format dxfId="184">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14" selected="0">
@@ -7681,13 +8179,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="107">
+    <format dxfId="183">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="106">
+    <format dxfId="182">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="105">
+    <format dxfId="181">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14">
@@ -7709,10 +8207,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="104">
+    <format dxfId="180">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="103">
+    <format dxfId="179">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14" selected="0">
@@ -7734,13 +8232,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="102">
+    <format dxfId="178">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="101">
+    <format dxfId="177">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="100">
+    <format dxfId="176">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="14">
@@ -7762,10 +8260,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="99">
+    <format dxfId="175">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="98">
+    <format dxfId="174">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7774,17 +8272,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="97">
+    <format dxfId="173">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="96">
+    <format dxfId="172">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="95">
+    <format dxfId="171">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7793,7 +8291,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="94">
+    <format dxfId="170">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7802,17 +8300,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="93">
+    <format dxfId="169">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="92">
+    <format dxfId="168">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="91">
+    <format dxfId="167">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7821,7 +8319,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="90">
+    <format dxfId="166">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1" selected="0">
@@ -7830,17 +8328,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="89">
+    <format dxfId="165">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="164">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="87">
+    <format dxfId="163">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -7849,16 +8347,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="162">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="85">
+    <format dxfId="161">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="84">
+    <format dxfId="160">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="83">
+    <format dxfId="159">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="38">
@@ -7904,10 +8402,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="158">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="81">
+    <format dxfId="157">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7919,7 +8417,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
+    <format dxfId="156">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7931,7 +8429,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="155">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7943,7 +8441,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="154">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7955,7 +8453,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="153">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7967,7 +8465,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="76">
+    <format dxfId="152">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7979,7 +8477,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="151">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -7991,7 +8489,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="150">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8019,7 +8517,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
+    <format dxfId="149">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8050,7 +8548,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="72">
+    <format dxfId="148">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8098,7 +8596,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="147">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8112,7 +8610,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
+    <format dxfId="146">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8157,7 +8655,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="69">
+    <format dxfId="145">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="12" selected="0">
@@ -8217,7 +8715,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="144">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8229,7 +8727,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="67">
+    <format dxfId="143">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8241,7 +8739,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="66">
+    <format dxfId="142">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8253,7 +8751,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="65">
+    <format dxfId="141">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8265,7 +8763,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="64">
+    <format dxfId="140">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -8273,6 +8771,749 @@
           </reference>
           <reference field="1" count="1">
             <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="139">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="25"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="138">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="80"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="137">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="201"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="136">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="221"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="135">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="43"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="25"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="134">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="43"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="80"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="133">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="43"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="201"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="132">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="38"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="221"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="131">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="42"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="221"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="130">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="123"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="221"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="129">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="43"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="128">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="42"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="127">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="123"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="126">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="42"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="125">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="45"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="124">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="47"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="123">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="72"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="122">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="121">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="120">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="64"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="119">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="118">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="44"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="117">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="116">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="39"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="115">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="114">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="113">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="112">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="42"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="111">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="45"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="110">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="47"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="109">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="72"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="108">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="64"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="107">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="106">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="105">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="104">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="103">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="39"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="102">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="101">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="64"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="147"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="100">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="147"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="99">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="147"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="98">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="65"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="97">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="144"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="96">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="39"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="144"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="95">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="144"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="94">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="213"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="93">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="39"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="213"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="92">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="213"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="91">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="199"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="90">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="27"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="89">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="64"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="27"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="88">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="27"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="87">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="63"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="27"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="86">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="199"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="85">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="2">
+            <x v="153"/>
+            <x v="154"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="84">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="105"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="83">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="175"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="82">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="174"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="81">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="219"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="80">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="159"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="79">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="205"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="78">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="183"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="77">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="186"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="76">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="198"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="75">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="151"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="74">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="85"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="73">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="25"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="72">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="201"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="71">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="80"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="70">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="221"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="69">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="221"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="68">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="201"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="67">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="80"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="66">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="25"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="65">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="105"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="64">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="2">
+            <x v="153"/>
+            <x v="154"/>
           </reference>
         </references>
       </pivotArea>
@@ -8280,8 +9521,9 @@
     <format dxfId="63">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
-          <reference field="1" count="1">
-            <x v="25"/>
+          <reference field="1" count="2">
+            <x v="174"/>
+            <x v="175"/>
           </reference>
         </references>
       </pivotArea>
@@ -8290,7 +9532,7 @@
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="80"/>
+            <x v="85"/>
           </reference>
         </references>
       </pivotArea>
@@ -8299,7 +9541,7 @@
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="201"/>
+            <x v="116"/>
           </reference>
         </references>
       </pivotArea>
@@ -8308,55 +9550,45 @@
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="221"/>
+            <x v="151"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="59">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="43"/>
-          </reference>
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
           <reference field="1" count="1">
-            <x v="25"/>
+            <x v="159"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="58">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="43"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="80"/>
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="3">
+            <x v="183"/>
+            <x v="186"/>
+            <x v="198"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="57">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="43"/>
-          </reference>
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
           <reference field="1" count="1">
-            <x v="201"/>
+            <x v="205"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="56">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="38"/>
-          </reference>
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
           <reference field="1" count="1">
-            <x v="221"/>
+            <x v="219"/>
           </reference>
         </references>
       </pivotArea>
@@ -8365,10 +9597,10 @@
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
-            <x v="42"/>
+            <x v="39"/>
           </reference>
           <reference field="1" count="1">
-            <x v="221"/>
+            <x v="151"/>
           </reference>
         </references>
       </pivotArea>
@@ -8377,148 +9609,164 @@
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
-            <x v="123"/>
+            <x v="38"/>
           </reference>
           <reference field="1" count="1">
-            <x v="221"/>
+            <x v="159"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="53">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
-            <x v="43"/>
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="64"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="159"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="52">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
-            <x v="42"/>
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="183"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="51">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
-            <x v="123"/>
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="41"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="198"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="50">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="108"/>
+          </reference>
           <reference field="1" count="1">
-            <x v="42"/>
+            <x v="186"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="49">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="115"/>
+          </reference>
           <reference field="1" count="1">
-            <x v="45"/>
+            <x v="205"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="48">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="115"/>
+          </reference>
           <reference field="1" count="1">
-            <x v="47"/>
+            <x v="17"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="47">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="115"/>
+          </reference>
           <reference field="1" count="1">
-            <x v="72"/>
+            <x v="116"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="46">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="36"/>
+          </reference>
           <reference field="1" count="1">
-            <x v="14"/>
+            <x v="219"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="45">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="39"/>
+          </reference>
           <reference field="1" count="1">
-            <x v="0"/>
+            <x v="85"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="44">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="64"/>
-          </reference>
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
           <reference field="1" count="1">
-            <x v="0"/>
+            <x v="105"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="43">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="7"/>
+            <x v="105"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="42">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="36"/>
-          </reference>
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
           <reference field="1" count="1">
-            <x v="44"/>
+            <x v="199"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="41">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="36"/>
-          </reference>
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
           <reference field="1" count="1">
-            <x v="7"/>
+            <x v="199"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="40">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="39"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="7"/>
+      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="2">
+            <x v="174"/>
+            <x v="175"/>
           </reference>
         </references>
       </pivotArea>
@@ -8526,8 +9774,9 @@
     <format dxfId="39">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
-          <reference field="1" count="1">
-            <x v="0"/>
+          <reference field="1" count="2">
+            <x v="174"/>
+            <x v="175"/>
           </reference>
         </references>
       </pivotArea>
@@ -8535,8 +9784,9 @@
     <format dxfId="38">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
-          <reference field="1" count="1">
-            <x v="7"/>
+          <reference field="1" count="2">
+            <x v="153"/>
+            <x v="154"/>
           </reference>
         </references>
       </pivotArea>
@@ -8544,8 +9794,9 @@
     <format dxfId="37">
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
-          <reference field="1" count="1">
-            <x v="14"/>
+          <reference field="1" count="2">
+            <x v="153"/>
+            <x v="154"/>
           </reference>
         </references>
       </pivotArea>
@@ -8554,7 +9805,7 @@
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="42"/>
+            <x v="201"/>
           </reference>
         </references>
       </pivotArea>
@@ -8563,25 +9814,28 @@
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="45"/>
+            <x v="201"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="34">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="22"/>
+          </reference>
           <reference field="1" count="1">
-            <x v="47"/>
+            <x v="105"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="33">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="72"/>
+            <x v="105"/>
           </reference>
         </references>
       </pivotArea>
@@ -8590,10 +9844,10 @@
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
-            <x v="64"/>
+            <x v="22"/>
           </reference>
           <reference field="1" count="1">
-            <x v="5"/>
+            <x v="105"/>
           </reference>
         </references>
       </pivotArea>
@@ -8602,16 +9856,17 @@
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="5"/>
+            <x v="105"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="30">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
-          <reference field="1" count="1">
-            <x v="5"/>
+          <reference field="1" count="2">
+            <x v="153"/>
+            <x v="154"/>
           </reference>
         </references>
       </pivotArea>
@@ -8619,17 +9874,22 @@
     <format dxfId="29">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
-          <reference field="1" count="1">
-            <x v="7"/>
+          <reference field="1" count="2">
+            <x v="153"/>
+            <x v="154"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="28">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="7"/>
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="74"/>
+          </reference>
+          <reference field="1" count="2">
+            <x v="153"/>
+            <x v="154"/>
           </reference>
         </references>
       </pivotArea>
@@ -8638,10 +9898,11 @@
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
-            <x v="39"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="7"/>
+            <x v="74"/>
+          </reference>
+          <reference field="1" count="2">
+            <x v="153"/>
+            <x v="154"/>
           </reference>
         </references>
       </pivotArea>
@@ -8650,10 +9911,10 @@
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
-            <x v="36"/>
+            <x v="74"/>
           </reference>
           <reference field="1" count="1">
-            <x v="7"/>
+            <x v="175"/>
           </reference>
         </references>
       </pivotArea>
@@ -8662,28 +9923,34 @@
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
-            <x v="64"/>
+            <x v="74"/>
           </reference>
           <reference field="1" count="1">
-            <x v="147"/>
+            <x v="175"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="24">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="38"/>
+          </reference>
           <reference field="1" count="1">
-            <x v="147"/>
+            <x v="221"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="23">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="38"/>
+          </reference>
           <reference field="1" count="1">
-            <x v="147"/>
+            <x v="221"/>
           </reference>
         </references>
       </pivotArea>
@@ -8692,19 +9959,22 @@
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
-            <x v="36"/>
+            <x v="42"/>
           </reference>
           <reference field="1" count="1">
-            <x v="65"/>
+            <x v="221"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="21">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="42"/>
+          </reference>
           <reference field="1" count="1">
-            <x v="144"/>
+            <x v="221"/>
           </reference>
         </references>
       </pivotArea>
@@ -8713,79 +9983,86 @@
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
-            <x v="39"/>
+            <x v="123"/>
           </reference>
           <reference field="1" count="1">
-            <x v="144"/>
+            <x v="221"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="19">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="123"/>
+          </reference>
           <reference field="1" count="1">
-            <x v="144"/>
+            <x v="221"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="18">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="123"/>
+          </reference>
           <reference field="1" count="1">
-            <x v="213"/>
+            <x v="221"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="17">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="199"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="16">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="199"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="15">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
             <x v="39"/>
           </reference>
           <reference field="1" count="1">
-            <x v="213"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="16">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="213"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="15">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
             <x v="199"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="14">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="39"/>
+          </reference>
           <reference field="1" count="1">
-            <x v="27"/>
+            <x v="199"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="13">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="64"/>
-          </reference>
-          <reference field="1" count="1">
-            <x v="27"/>
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="2">
+            <x v="174"/>
+            <x v="175"/>
           </reference>
         </references>
       </pivotArea>
@@ -8793,8 +10070,9 @@
     <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
-          <reference field="1" count="1">
-            <x v="27"/>
+          <reference field="1" count="2">
+            <x v="174"/>
+            <x v="175"/>
           </reference>
         </references>
       </pivotArea>
@@ -8803,74 +10081,94 @@
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
-            <x v="63"/>
+            <x v="54"/>
           </reference>
           <reference field="1" count="1">
-            <x v="27"/>
+            <x v="174"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="10">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="54"/>
+          </reference>
           <reference field="1" count="1">
-            <x v="199"/>
+            <x v="174"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="9">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="2">
-            <x v="153"/>
-            <x v="154"/>
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="43"/>
+          </reference>
+          <reference field="1" count="1">
+            <x v="25"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="8">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="43"/>
+          </reference>
           <reference field="1" count="1">
-            <x v="105"/>
+            <x v="25"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="7">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="43"/>
+          </reference>
           <reference field="1" count="1">
-            <x v="175"/>
+            <x v="80"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="6">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="43"/>
+          </reference>
           <reference field="1" count="1">
-            <x v="174"/>
+            <x v="80"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="5">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="43"/>
+          </reference>
           <reference field="1" count="1">
-            <x v="219"/>
+            <x v="201"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="4">
-      <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="43"/>
+          </reference>
           <reference field="1" count="1">
-            <x v="159"/>
+            <x v="201"/>
           </reference>
         </references>
       </pivotArea>
@@ -8879,7 +10177,7 @@
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="205"/>
+            <x v="221"/>
           </reference>
         </references>
       </pivotArea>
@@ -8888,7 +10186,7 @@
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="183"/>
+            <x v="221"/>
           </reference>
         </references>
       </pivotArea>
@@ -8897,7 +10195,7 @@
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="186"/>
+            <x v="25"/>
           </reference>
         </references>
       </pivotArea>
@@ -8906,7 +10204,7 @@
       <pivotArea field="1" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
-            <x v="198"/>
+            <x v="25"/>
           </reference>
         </references>
       </pivotArea>
@@ -14936,7 +16234,7 @@
       <c r="E4" t="s">
         <v>445</v>
       </c>
-      <c r="F4" s="34"/>
+      <c r="F4" s="32"/>
       <c r="G4" t="s">
         <v>444</v>
       </c>
@@ -14954,7 +16252,7 @@
       <c r="E5" t="s">
         <v>441</v>
       </c>
-      <c r="F5" s="34"/>
+      <c r="F5" s="32"/>
       <c r="G5" t="s">
         <v>438</v>
       </c>
@@ -14975,7 +16273,7 @@
       <c r="F6" t="s">
         <v>436</v>
       </c>
-      <c r="G6" s="34"/>
+      <c r="G6" s="32"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -14990,7 +16288,7 @@
       <c r="E7" t="s">
         <v>441</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="32"/>
       <c r="G7" t="s">
         <v>438</v>
       </c>
@@ -15011,21 +16309,21 @@
       <c r="F8" t="s">
         <v>436</v>
       </c>
-      <c r="G8" s="34"/>
+      <c r="G8" s="32"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="42">
+      <c r="B9" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="42">
+      <c r="B10" s="40">
         <v>3</v>
       </c>
     </row>
@@ -15042,7 +16340,7 @@
       <c r="E11" t="s">
         <v>441</v>
       </c>
-      <c r="F11" s="34"/>
+      <c r="F11" s="32"/>
       <c r="G11" t="s">
         <v>442</v>
       </c>
@@ -15060,8 +16358,8 @@
       <c r="E12" t="s">
         <v>439</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -15076,8 +16374,8 @@
       <c r="E13" t="s">
         <v>439</v>
       </c>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -15092,7 +16390,7 @@
       <c r="E14" t="s">
         <v>448</v>
       </c>
-      <c r="F14" s="34"/>
+      <c r="F14" s="32"/>
       <c r="G14" t="s">
         <v>447</v>
       </c>
@@ -15113,7 +16411,7 @@
       <c r="F15" t="s">
         <v>436</v>
       </c>
-      <c r="G15" s="34"/>
+      <c r="G15" s="32"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -15131,7 +16429,7 @@
       <c r="F16" t="s">
         <v>436</v>
       </c>
-      <c r="G16" s="34"/>
+      <c r="G16" s="32"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -15146,16 +16444,16 @@
       <c r="E17" t="s">
         <v>441</v>
       </c>
-      <c r="F17" s="34"/>
+      <c r="F17" s="32"/>
       <c r="G17" t="s">
         <v>438</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="42">
+      <c r="B18" s="40">
         <v>1</v>
       </c>
     </row>
@@ -15181,7 +16479,7 @@
   <dimension ref="A1:X50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+      <selection activeCell="R45" sqref="R45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -15199,7 +16497,7 @@
     <col min="15" max="15" width="10.375" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.125" style="5" customWidth="1"/>
     <col min="17" max="17" width="11.375" style="6" customWidth="1"/>
-    <col min="18" max="18" width="15.625" customWidth="1"/>
+    <col min="18" max="18" width="17.75" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="22.875" customWidth="1"/>
     <col min="20" max="20" width="23.625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="6.125" customWidth="1"/>
@@ -15335,10 +16633,10 @@
       <c r="F4" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="27" t="s">
         <v>31</v>
       </c>
       <c r="I4" s="5" t="s">
@@ -15362,30 +16660,30 @@
       <c r="O4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="29" t="s">
+      <c r="P4" s="27" t="s">
         <v>91</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>403</v>
       </c>
-      <c r="R4" s="48" t="s">
+      <c r="R4" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="S4" s="48" t="s">
+      <c r="S4" s="44" t="s">
         <v>456</v>
       </c>
-      <c r="T4" s="48" t="s">
+      <c r="T4" s="44" t="s">
         <v>457</v>
       </c>
-      <c r="U4" s="48" t="s">
+      <c r="U4" s="44" t="s">
         <v>458</v>
       </c>
-      <c r="V4" s="48" t="s">
+      <c r="V4" s="44" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="25"/>
@@ -15405,30 +16703,30 @@
       <c r="N5" s="23"/>
       <c r="O5" s="23"/>
       <c r="P5" s="23"/>
-      <c r="Q5" s="32">
+      <c r="Q5" s="30">
         <v>1</v>
       </c>
-      <c r="R5" s="35" t="str">
+      <c r="R5" s="33" t="str">
         <f>A5</f>
         <v>abacavir</v>
       </c>
-      <c r="S5" s="35" t="s">
+      <c r="S5" s="33" t="s">
         <v>409</v>
       </c>
-      <c r="T5" s="35" t="s">
+      <c r="T5" s="33" t="s">
         <v>419</v>
       </c>
-      <c r="U5" s="35" t="s">
+      <c r="U5" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="V5" s="35" t="s">
+      <c r="V5" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="W5" s="35"/>
-      <c r="X5" s="35"/>
+      <c r="W5" s="33"/>
+      <c r="X5" s="33"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="29" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="25"/>
@@ -15448,38 +16746,38 @@
       <c r="N6" s="23"/>
       <c r="O6" s="23"/>
       <c r="P6" s="23"/>
-      <c r="Q6" s="32">
+      <c r="Q6" s="30">
         <v>1</v>
       </c>
-      <c r="R6" s="35" t="str">
+      <c r="R6" s="33" t="str">
         <f t="shared" ref="R6:R42" si="0">A6</f>
         <v>allopurinol</v>
       </c>
-      <c r="S6" s="35" t="s">
+      <c r="S6" s="33" t="s">
         <v>408</v>
       </c>
-      <c r="T6" s="35" t="s">
+      <c r="T6" s="33" t="s">
         <v>432</v>
       </c>
-      <c r="U6" s="35" t="s">
+      <c r="U6" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="V6" s="35" t="s">
+      <c r="V6" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="W6" s="35"/>
-      <c r="X6" s="35"/>
+      <c r="W6" s="33"/>
+      <c r="X6" s="33"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="35" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="25"/>
-      <c r="C7" s="40">
+      <c r="C7" s="38">
         <v>1</v>
       </c>
       <c r="D7" s="23"/>
-      <c r="E7" s="39">
+      <c r="E7" s="37">
         <v>1</v>
       </c>
       <c r="F7" s="23"/>
@@ -15493,34 +16791,34 @@
       <c r="N7" s="23"/>
       <c r="O7" s="23"/>
       <c r="P7" s="23"/>
-      <c r="Q7" s="38">
+      <c r="Q7" s="36">
         <v>2</v>
       </c>
-      <c r="R7" s="33" t="str">
+      <c r="R7" s="31" t="str">
         <f t="shared" si="0"/>
         <v>amitriptyline</v>
       </c>
-      <c r="S7" s="33" t="s">
+      <c r="S7" s="31" t="s">
         <v>413</v>
       </c>
-      <c r="T7" s="33" t="s">
+      <c r="T7" s="31" t="s">
         <v>425</v>
       </c>
-      <c r="U7" s="33" t="s">
+      <c r="U7" s="31" t="s">
         <v>426</v>
       </c>
-      <c r="V7" s="33" t="s">
+      <c r="V7" s="31" t="s">
         <v>427</v>
       </c>
-      <c r="W7" s="33" t="s">
+      <c r="W7" s="31" t="s">
         <v>428</v>
       </c>
-      <c r="X7" s="33" t="s">
+      <c r="X7" s="31" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="29" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="25"/>
@@ -15540,27 +16838,27 @@
         <v>1</v>
       </c>
       <c r="P8" s="23"/>
-      <c r="Q8" s="32">
+      <c r="Q8" s="30">
         <v>1</v>
       </c>
-      <c r="R8" s="35" t="str">
+      <c r="R8" s="33" t="str">
         <f t="shared" si="0"/>
         <v>atazanavir</v>
       </c>
-      <c r="S8" s="35" t="s">
+      <c r="S8" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="T8" s="35" t="s">
+      <c r="T8" s="33" t="s">
         <v>420</v>
       </c>
-      <c r="U8" s="35" t="s">
+      <c r="U8" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="V8" s="35" t="s">
+      <c r="V8" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="W8" s="35"/>
-      <c r="X8" s="35"/>
+      <c r="W8" s="33"/>
+      <c r="X8" s="33"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
@@ -15578,35 +16876,35 @@
       <c r="K9" s="23"/>
       <c r="L9" s="23"/>
       <c r="M9" s="23"/>
-      <c r="N9" s="24">
+      <c r="N9" s="21">
         <v>1</v>
       </c>
       <c r="O9" s="23"/>
       <c r="P9" s="23"/>
-      <c r="Q9" s="32">
+      <c r="Q9" s="30">
         <v>1</v>
       </c>
-      <c r="R9" s="35" t="str">
+      <c r="R9" s="33" t="str">
         <f t="shared" si="0"/>
         <v>azathioprine</v>
       </c>
-      <c r="S9" s="35" t="s">
+      <c r="S9" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="T9" s="35" t="s">
+      <c r="T9" s="33" t="s">
         <v>473</v>
       </c>
-      <c r="U9" s="35" t="s">
+      <c r="U9" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="V9" s="35" t="s">
+      <c r="V9" s="33" t="s">
         <v>452</v>
       </c>
-      <c r="W9" s="35"/>
-      <c r="X9" s="35"/>
+      <c r="W9" s="33"/>
+      <c r="X9" s="33"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="53" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="25"/>
@@ -15615,7 +16913,7 @@
       <c r="E10" s="23"/>
       <c r="F10" s="23"/>
       <c r="G10" s="23"/>
-      <c r="H10" s="28">
+      <c r="H10" s="70">
         <v>1</v>
       </c>
       <c r="I10" s="23"/>
@@ -15626,24 +16924,24 @@
       <c r="N10" s="23"/>
       <c r="O10" s="23"/>
       <c r="P10" s="23"/>
-      <c r="Q10" s="9">
+      <c r="Q10" s="64">
         <v>1</v>
       </c>
-      <c r="R10" s="36" t="str">
+      <c r="R10" s="34" t="str">
         <f t="shared" si="0"/>
         <v>capecitabine</v>
       </c>
-      <c r="S10" s="36" t="s">
+      <c r="S10" s="34" t="s">
         <v>415</v>
       </c>
-      <c r="T10" s="30"/>
-      <c r="U10" s="30"/>
-      <c r="V10" s="30"/>
-      <c r="W10" s="30"/>
-      <c r="X10" s="30"/>
+      <c r="T10" s="28"/>
+      <c r="U10" s="28"/>
+      <c r="V10" s="28"/>
+      <c r="W10" s="28"/>
+      <c r="X10" s="28"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="35" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="25"/>
@@ -15654,10 +16952,10 @@
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
       <c r="I11" s="23"/>
-      <c r="J11" s="39">
+      <c r="J11" s="37">
         <v>1</v>
       </c>
-      <c r="K11" s="39">
+      <c r="K11" s="37">
         <v>1</v>
       </c>
       <c r="L11" s="23"/>
@@ -15665,32 +16963,32 @@
       <c r="N11" s="23"/>
       <c r="O11" s="23"/>
       <c r="P11" s="23"/>
-      <c r="Q11" s="38">
+      <c r="Q11" s="36">
         <v>2</v>
       </c>
-      <c r="R11" s="33" t="str">
+      <c r="R11" s="31" t="str">
         <f t="shared" si="0"/>
         <v>carbamazepine</v>
       </c>
-      <c r="S11" s="33" t="s">
+      <c r="S11" s="31" t="s">
         <v>410</v>
       </c>
-      <c r="T11" s="33" t="s">
+      <c r="T11" s="31" t="s">
         <v>460</v>
       </c>
-      <c r="U11" s="33" t="s">
+      <c r="U11" s="31" t="s">
         <v>455</v>
       </c>
-      <c r="V11" s="33" t="s">
+      <c r="V11" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="W11" s="33"/>
-      <c r="X11" s="33" t="s">
+      <c r="W11" s="31"/>
+      <c r="X11" s="31" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="29" t="s">
         <v>92</v>
       </c>
       <c r="B12" s="25"/>
@@ -15710,27 +17008,27 @@
       <c r="N12" s="23"/>
       <c r="O12" s="23"/>
       <c r="P12" s="23"/>
-      <c r="Q12" s="32">
+      <c r="Q12" s="30">
         <v>1</v>
       </c>
-      <c r="R12" s="35" t="str">
+      <c r="R12" s="33" t="str">
         <f t="shared" si="0"/>
         <v>citalopram</v>
       </c>
-      <c r="S12" s="35" t="s">
+      <c r="S12" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="T12" s="35" t="s">
+      <c r="T12" s="33" t="s">
         <v>421</v>
       </c>
-      <c r="U12" s="35" t="s">
+      <c r="U12" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="V12" s="35" t="s">
+      <c r="V12" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="W12" s="35"/>
-      <c r="X12" s="35"/>
+      <c r="W12" s="33"/>
+      <c r="X12" s="33"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
@@ -15765,7 +17063,7 @@
       <c r="S13" t="s">
         <v>413</v>
       </c>
-      <c r="U13" s="47" t="s">
+      <c r="U13" s="43" t="s">
         <v>427</v>
       </c>
       <c r="V13" t="s">
@@ -15776,7 +17074,7 @@
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="29" t="s">
         <v>38</v>
       </c>
       <c r="B14" s="25"/>
@@ -15796,30 +17094,30 @@
       <c r="N14" s="23"/>
       <c r="O14" s="23"/>
       <c r="P14" s="23"/>
-      <c r="Q14" s="32">
+      <c r="Q14" s="30">
         <v>1</v>
       </c>
-      <c r="R14" s="35" t="str">
+      <c r="R14" s="33" t="str">
         <f t="shared" si="0"/>
         <v>clopidogrel</v>
       </c>
-      <c r="S14" s="35" t="s">
+      <c r="S14" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="T14" s="35" t="s">
+      <c r="T14" s="33" t="s">
         <v>422</v>
       </c>
-      <c r="U14" s="35" t="s">
+      <c r="U14" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="V14" s="35" t="s">
+      <c r="V14" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="W14" s="35"/>
-      <c r="X14" s="35"/>
+      <c r="W14" s="33"/>
+      <c r="X14" s="33"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="29" t="s">
         <v>41</v>
       </c>
       <c r="B15" s="25"/>
@@ -15839,27 +17137,27 @@
       <c r="N15" s="23"/>
       <c r="O15" s="23"/>
       <c r="P15" s="23"/>
-      <c r="Q15" s="32">
+      <c r="Q15" s="30">
         <v>1</v>
       </c>
-      <c r="R15" s="35" t="str">
+      <c r="R15" s="33" t="str">
         <f t="shared" si="0"/>
         <v>codeine</v>
       </c>
-      <c r="S15" s="35" t="s">
+      <c r="S15" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="T15" s="35" t="s">
+      <c r="T15" s="33" t="s">
         <v>423</v>
       </c>
-      <c r="U15" s="35" t="s">
+      <c r="U15" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="V15" s="35" t="s">
+      <c r="V15" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="W15" s="35"/>
-      <c r="X15" s="35"/>
+      <c r="W15" s="33"/>
+      <c r="X15" s="33"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
@@ -15892,10 +17190,10 @@
       <c r="S16" t="s">
         <v>21</v>
       </c>
-      <c r="U16" s="47" t="s">
+      <c r="U16" s="43" t="s">
         <v>427</v>
       </c>
-      <c r="V16" s="47" t="s">
+      <c r="V16" s="43" t="s">
         <v>427</v>
       </c>
       <c r="W16" t="s">
@@ -15935,10 +17233,10 @@
       <c r="S17" t="s">
         <v>413</v>
       </c>
-      <c r="U17" s="47" t="s">
+      <c r="U17" s="43" t="s">
         <v>426</v>
       </c>
-      <c r="V17" s="47" t="s">
+      <c r="V17" s="43" t="s">
         <v>427</v>
       </c>
       <c r="W17" t="s">
@@ -15946,7 +17244,7 @@
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="29" t="s">
         <v>93</v>
       </c>
       <c r="B18" s="25"/>
@@ -15966,30 +17264,30 @@
       <c r="N18" s="23"/>
       <c r="O18" s="23"/>
       <c r="P18" s="23"/>
-      <c r="Q18" s="32">
+      <c r="Q18" s="30">
         <v>1</v>
       </c>
-      <c r="R18" s="35" t="str">
+      <c r="R18" s="33" t="str">
         <f t="shared" si="0"/>
         <v>escitalopram</v>
       </c>
-      <c r="S18" s="35" t="s">
+      <c r="S18" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="T18" s="35" t="s">
+      <c r="T18" s="33" t="s">
         <v>424</v>
       </c>
-      <c r="U18" s="35" t="s">
+      <c r="U18" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="V18" s="35" t="s">
+      <c r="V18" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="W18" s="35"/>
-      <c r="X18" s="35"/>
+      <c r="W18" s="33"/>
+      <c r="X18" s="33"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="53" t="s">
         <v>47</v>
       </c>
       <c r="B19" s="25"/>
@@ -15998,7 +17296,7 @@
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
       <c r="G19" s="23"/>
-      <c r="H19" s="28">
+      <c r="H19" s="70">
         <v>1</v>
       </c>
       <c r="I19" s="23"/>
@@ -16012,27 +17310,27 @@
       <c r="Q19" s="9">
         <v>1</v>
       </c>
-      <c r="R19" s="36" t="str">
+      <c r="R19" s="34" t="str">
         <f t="shared" si="0"/>
         <v>fluorouracil</v>
       </c>
-      <c r="S19" s="36" t="s">
+      <c r="S19" s="34" t="s">
         <v>415</v>
       </c>
-      <c r="T19" s="30"/>
-      <c r="U19" s="30"/>
-      <c r="V19" s="30"/>
-      <c r="W19" s="30"/>
-      <c r="X19" s="30"/>
+      <c r="T19" s="28"/>
+      <c r="U19" s="28"/>
+      <c r="V19" s="28"/>
+      <c r="W19" s="28"/>
+      <c r="X19" s="28"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="29" t="s">
         <v>48</v>
       </c>
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
       <c r="D20" s="23"/>
-      <c r="E20" s="24">
+      <c r="E20" s="21">
         <v>1</v>
       </c>
       <c r="F20" s="23"/>
@@ -16046,25 +17344,27 @@
       <c r="N20" s="23"/>
       <c r="O20" s="23"/>
       <c r="P20" s="23"/>
-      <c r="Q20" s="9">
+      <c r="Q20" s="30">
         <v>1</v>
       </c>
-      <c r="R20" t="str">
+      <c r="R20" s="33" t="str">
         <f t="shared" si="0"/>
         <v>fluvoxamine</v>
       </c>
-      <c r="S20" t="s">
+      <c r="S20" s="33" t="s">
         <v>417</v>
       </c>
-      <c r="T20" t="s">
+      <c r="T20" s="33" t="s">
         <v>479</v>
       </c>
-      <c r="U20" t="s">
+      <c r="U20" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="V20" t="s">
+      <c r="V20" s="33" t="s">
         <v>427</v>
       </c>
+      <c r="W20" s="33"/>
+      <c r="X20" s="33"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
@@ -16110,10 +17410,10 @@
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="69">
         <v>1</v>
       </c>
       <c r="C22" s="25"/>
@@ -16130,28 +17430,28 @@
       <c r="N22" s="23"/>
       <c r="O22" s="23"/>
       <c r="P22" s="23"/>
-      <c r="Q22" s="52">
+      <c r="Q22" s="64">
         <v>1</v>
       </c>
-      <c r="R22" s="44" t="str">
+      <c r="R22" s="51" t="str">
         <f t="shared" si="0"/>
         <v>ivacaftor</v>
       </c>
-      <c r="S22" s="44" t="s">
+      <c r="S22" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="T22" s="44"/>
-      <c r="U22" s="44" t="s">
+      <c r="T22" s="51"/>
+      <c r="U22" s="51" t="s">
         <v>427</v>
       </c>
-      <c r="V22" s="44" t="s">
+      <c r="V22" s="51" t="s">
         <v>427</v>
       </c>
-      <c r="W22" s="44"/>
-      <c r="X22" s="44"/>
+      <c r="W22" s="51"/>
+      <c r="X22" s="51"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="29" t="s">
         <v>56</v>
       </c>
       <c r="B23" s="25"/>
@@ -16166,32 +17466,32 @@
       <c r="K23" s="23"/>
       <c r="L23" s="23"/>
       <c r="M23" s="23"/>
-      <c r="N23" s="24">
+      <c r="N23" s="21">
         <v>1</v>
       </c>
       <c r="O23" s="23"/>
       <c r="P23" s="23"/>
-      <c r="Q23" s="32">
+      <c r="Q23" s="30">
         <v>1</v>
       </c>
-      <c r="R23" s="35" t="str">
+      <c r="R23" s="33" t="str">
         <f t="shared" si="0"/>
         <v>mercaptopurine</v>
       </c>
-      <c r="S23" s="35" t="s">
+      <c r="S23" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="T23" s="35" t="s">
+      <c r="T23" s="33" t="s">
         <v>475</v>
       </c>
-      <c r="U23" s="35" t="s">
+      <c r="U23" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="V23" s="35" t="s">
+      <c r="V23" s="33" t="s">
         <v>452</v>
       </c>
-      <c r="W23" s="35"/>
-      <c r="X23" s="35"/>
+      <c r="W23" s="33"/>
+      <c r="X23" s="33"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
@@ -16235,7 +17535,7 @@
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="29" t="s">
         <v>58</v>
       </c>
       <c r="B25" s="25"/>
@@ -16255,30 +17555,30 @@
       <c r="N25" s="23"/>
       <c r="O25" s="23"/>
       <c r="P25" s="23"/>
-      <c r="Q25" s="32">
+      <c r="Q25" s="30">
         <v>1</v>
       </c>
-      <c r="R25" s="35" t="str">
+      <c r="R25" s="33" t="str">
         <f t="shared" si="0"/>
         <v>ondansetron</v>
       </c>
-      <c r="S25" s="35" t="s">
+      <c r="S25" s="33" t="s">
         <v>417</v>
       </c>
-      <c r="T25" s="35" t="s">
+      <c r="T25" s="33" t="s">
         <v>450</v>
       </c>
-      <c r="U25" s="35" t="s">
+      <c r="U25" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="V25" s="35" t="s">
+      <c r="V25" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="W25" s="35"/>
-      <c r="X25" s="35"/>
+      <c r="W25" s="33"/>
+      <c r="X25" s="33"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B26" s="25"/>
@@ -16290,7 +17590,7 @@
       <c r="H26" s="23"/>
       <c r="I26" s="23"/>
       <c r="J26" s="23"/>
-      <c r="K26" s="39">
+      <c r="K26" s="37">
         <v>1</v>
       </c>
       <c r="L26" s="23"/>
@@ -16298,38 +17598,38 @@
       <c r="N26" s="23"/>
       <c r="O26" s="23"/>
       <c r="P26" s="23"/>
-      <c r="Q26" s="38">
+      <c r="Q26" s="36">
         <v>1</v>
       </c>
-      <c r="R26" s="33" t="str">
+      <c r="R26" s="31" t="str">
         <f t="shared" si="0"/>
         <v>oxcarbazepine</v>
       </c>
-      <c r="S26" s="33" t="s">
+      <c r="S26" s="31" t="s">
         <v>411</v>
       </c>
-      <c r="T26" s="33" t="s">
+      <c r="T26" s="31" t="s">
         <v>431</v>
       </c>
-      <c r="U26" s="33" t="s">
+      <c r="U26" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="V26" s="33" t="s">
+      <c r="V26" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="W26" s="33"/>
-      <c r="X26" s="33" t="s">
+      <c r="W26" s="31"/>
+      <c r="X26" s="31" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="29" t="s">
         <v>63</v>
       </c>
       <c r="B27" s="25"/>
       <c r="C27" s="25"/>
       <c r="D27" s="23"/>
-      <c r="E27" s="24">
+      <c r="E27" s="21">
         <v>1</v>
       </c>
       <c r="F27" s="23"/>
@@ -16343,28 +17643,30 @@
       <c r="N27" s="23"/>
       <c r="O27" s="23"/>
       <c r="P27" s="23"/>
-      <c r="Q27" s="9">
+      <c r="Q27" s="30">
         <v>1</v>
       </c>
-      <c r="R27" t="str">
+      <c r="R27" s="33" t="str">
         <f t="shared" si="0"/>
         <v>paroxetine</v>
       </c>
-      <c r="S27" t="s">
+      <c r="S27" s="33" t="s">
         <v>417</v>
       </c>
-      <c r="T27" t="s">
+      <c r="T27" s="33" t="s">
         <v>480</v>
       </c>
-      <c r="U27" t="s">
+      <c r="U27" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="V27" t="s">
+      <c r="V27" s="33" t="s">
         <v>427</v>
       </c>
+      <c r="W27" s="33"/>
+      <c r="X27" s="33"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="53" t="s">
         <v>95</v>
       </c>
       <c r="B28" s="25"/>
@@ -16377,35 +17679,35 @@
       <c r="I28" s="23"/>
       <c r="J28" s="23"/>
       <c r="K28" s="23"/>
-      <c r="L28" s="24">
+      <c r="L28" s="70">
         <v>1</v>
       </c>
       <c r="M28" s="23"/>
       <c r="N28" s="23"/>
       <c r="O28" s="23"/>
       <c r="P28" s="23"/>
-      <c r="Q28" s="52">
+      <c r="Q28" s="64">
         <v>1</v>
       </c>
-      <c r="R28" s="44" t="str">
+      <c r="R28" s="51" t="str">
         <f t="shared" si="0"/>
         <v>peginterferon alfa-2a</v>
       </c>
-      <c r="S28" s="44" t="s">
+      <c r="S28" s="51" t="s">
         <v>414</v>
       </c>
-      <c r="T28" s="44"/>
-      <c r="U28" s="44" t="s">
+      <c r="T28" s="51"/>
+      <c r="U28" s="51" t="s">
         <v>427</v>
       </c>
-      <c r="V28" s="44" t="s">
+      <c r="V28" s="51" t="s">
         <v>427</v>
       </c>
-      <c r="W28" s="44"/>
-      <c r="X28" s="44"/>
+      <c r="W28" s="51"/>
+      <c r="X28" s="51"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="53" t="s">
         <v>97</v>
       </c>
       <c r="B29" s="25"/>
@@ -16418,40 +17720,40 @@
       <c r="I29" s="23"/>
       <c r="J29" s="23"/>
       <c r="K29" s="23"/>
-      <c r="L29" s="24">
+      <c r="L29" s="70">
         <v>1</v>
       </c>
       <c r="M29" s="23"/>
       <c r="N29" s="23"/>
       <c r="O29" s="23"/>
       <c r="P29" s="23"/>
-      <c r="Q29" s="52">
+      <c r="Q29" s="64">
         <v>1</v>
       </c>
-      <c r="R29" s="44" t="str">
+      <c r="R29" s="51" t="str">
         <f t="shared" si="0"/>
         <v>peginterferon alfa-2b</v>
       </c>
-      <c r="S29" s="44" t="s">
+      <c r="S29" s="51" t="s">
         <v>414</v>
       </c>
-      <c r="T29" s="44"/>
-      <c r="U29" s="44" t="s">
+      <c r="T29" s="51"/>
+      <c r="U29" s="51" t="s">
         <v>427</v>
       </c>
-      <c r="V29" s="44" t="s">
+      <c r="V29" s="51" t="s">
         <v>427</v>
       </c>
-      <c r="W29" s="44"/>
-      <c r="X29" s="44"/>
+      <c r="W29" s="51"/>
+      <c r="X29" s="51"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="29" t="s">
         <v>65</v>
       </c>
       <c r="B30" s="25"/>
       <c r="C30" s="25"/>
-      <c r="D30" s="24">
+      <c r="D30" s="21">
         <v>1</v>
       </c>
       <c r="E30" s="23"/>
@@ -16460,7 +17762,7 @@
       <c r="H30" s="23"/>
       <c r="I30" s="23"/>
       <c r="J30" s="23"/>
-      <c r="K30" s="24">
+      <c r="K30" s="21">
         <v>1</v>
       </c>
       <c r="L30" s="23"/>
@@ -16468,30 +17770,30 @@
       <c r="N30" s="23"/>
       <c r="O30" s="23"/>
       <c r="P30" s="23"/>
-      <c r="Q30" s="32">
+      <c r="Q30" s="30">
         <v>2</v>
       </c>
-      <c r="R30" s="35" t="str">
+      <c r="R30" s="33" t="str">
         <f t="shared" si="0"/>
         <v>phenytoin</v>
       </c>
-      <c r="S30" s="35" t="s">
+      <c r="S30" s="33" t="s">
         <v>412</v>
       </c>
-      <c r="T30" s="35" t="s">
+      <c r="T30" s="33" t="s">
         <v>472</v>
       </c>
-      <c r="U30" s="35" t="s">
+      <c r="U30" s="33" t="s">
         <v>453</v>
       </c>
-      <c r="V30" s="35" t="s">
+      <c r="V30" s="33" t="s">
         <v>454</v>
       </c>
-      <c r="W30" s="35"/>
-      <c r="X30" s="35"/>
+      <c r="W30" s="33"/>
+      <c r="X30" s="33"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="53" t="s">
         <v>68</v>
       </c>
       <c r="B31" s="25"/>
@@ -16501,7 +17803,7 @@
       <c r="F31" s="23"/>
       <c r="G31" s="23"/>
       <c r="H31" s="23"/>
-      <c r="I31" s="24">
+      <c r="I31" s="70">
         <v>1</v>
       </c>
       <c r="J31" s="23"/>
@@ -16511,28 +17813,28 @@
       <c r="N31" s="23"/>
       <c r="O31" s="23"/>
       <c r="P31" s="23"/>
-      <c r="Q31" s="52">
+      <c r="Q31" s="64">
         <v>1</v>
       </c>
-      <c r="R31" s="44" t="str">
+      <c r="R31" s="51" t="str">
         <f t="shared" si="0"/>
         <v>rasburicase</v>
       </c>
-      <c r="S31" s="44" t="s">
+      <c r="S31" s="51" t="s">
         <v>418</v>
       </c>
-      <c r="T31" s="44"/>
-      <c r="U31" s="44" t="s">
+      <c r="T31" s="51"/>
+      <c r="U31" s="51" t="s">
         <v>427</v>
       </c>
-      <c r="V31" s="44" t="s">
+      <c r="V31" s="51" t="s">
         <v>427</v>
       </c>
-      <c r="W31" s="44"/>
-      <c r="X31" s="44"/>
+      <c r="W31" s="51"/>
+      <c r="X31" s="51"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="53" t="s">
         <v>98</v>
       </c>
       <c r="B32" s="25"/>
@@ -16545,39 +17847,39 @@
       <c r="I32" s="23"/>
       <c r="J32" s="23"/>
       <c r="K32" s="23"/>
-      <c r="L32" s="24">
+      <c r="L32" s="70">
         <v>1</v>
       </c>
       <c r="M32" s="23"/>
       <c r="N32" s="23"/>
       <c r="O32" s="23"/>
       <c r="P32" s="23"/>
-      <c r="Q32" s="52">
+      <c r="Q32" s="64">
         <v>1</v>
       </c>
-      <c r="R32" s="44" t="str">
+      <c r="R32" s="51" t="str">
         <f t="shared" si="0"/>
         <v>ribavirin</v>
       </c>
-      <c r="S32" s="44" t="s">
+      <c r="S32" s="51" t="s">
         <v>414</v>
       </c>
-      <c r="T32" s="44"/>
-      <c r="U32" s="44" t="s">
+      <c r="T32" s="51"/>
+      <c r="U32" s="51" t="s">
         <v>427</v>
       </c>
-      <c r="V32" s="44" t="s">
+      <c r="V32" s="51" t="s">
         <v>427</v>
       </c>
-      <c r="W32" s="44"/>
-      <c r="X32" s="44"/>
+      <c r="W32" s="51"/>
+      <c r="X32" s="51"/>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="29" t="s">
         <v>160</v>
       </c>
       <c r="B33" s="25"/>
-      <c r="C33" s="26">
+      <c r="C33" s="22">
         <v>1</v>
       </c>
       <c r="D33" s="23"/>
@@ -16593,30 +17895,30 @@
       <c r="N33" s="23"/>
       <c r="O33" s="23"/>
       <c r="P33" s="23"/>
-      <c r="Q33" s="32">
+      <c r="Q33" s="30">
         <v>1</v>
       </c>
-      <c r="R33" s="35" t="str">
+      <c r="R33" s="33" t="str">
         <f t="shared" si="0"/>
         <v>sertraline</v>
       </c>
-      <c r="S33" s="35" t="s">
+      <c r="S33" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="T33" s="35" t="s">
+      <c r="T33" s="33" t="s">
         <v>476</v>
       </c>
-      <c r="U33" s="35" t="s">
+      <c r="U33" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="V33" s="35" t="s">
+      <c r="V33" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="W33" s="35"/>
-      <c r="X33" s="35"/>
+      <c r="W33" s="33"/>
+      <c r="X33" s="33"/>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="29" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="25"/>
@@ -16630,43 +17932,43 @@
       <c r="J34" s="23"/>
       <c r="K34" s="23"/>
       <c r="L34" s="23"/>
-      <c r="M34" s="24">
+      <c r="M34" s="21">
         <v>1</v>
       </c>
       <c r="N34" s="23"/>
       <c r="O34" s="23"/>
       <c r="P34" s="23"/>
-      <c r="Q34" s="32">
+      <c r="Q34" s="30">
         <v>1</v>
       </c>
-      <c r="R34" s="35" t="str">
+      <c r="R34" s="33" t="str">
         <f t="shared" si="0"/>
         <v>simvastatin</v>
       </c>
-      <c r="S34" s="35" t="s">
+      <c r="S34" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="T34" s="35" t="s">
+      <c r="T34" s="33" t="s">
         <v>477</v>
       </c>
-      <c r="U34" s="35" t="s">
+      <c r="U34" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="V34" s="35" t="s">
+      <c r="V34" s="33" t="s">
         <v>452</v>
       </c>
-      <c r="W34" s="35"/>
-      <c r="X34" s="35"/>
+      <c r="W34" s="33"/>
+      <c r="X34" s="33"/>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="29" t="s">
         <v>77</v>
       </c>
       <c r="B35" s="25"/>
       <c r="C35" s="25"/>
       <c r="D35" s="23"/>
       <c r="E35" s="23"/>
-      <c r="F35" s="24">
+      <c r="F35" s="21">
         <v>1</v>
       </c>
       <c r="G35" s="23"/>
@@ -16679,36 +17981,36 @@
       <c r="N35" s="23"/>
       <c r="O35" s="23"/>
       <c r="P35" s="23"/>
-      <c r="Q35" s="32">
+      <c r="Q35" s="30">
         <v>1</v>
       </c>
-      <c r="R35" s="35" t="str">
+      <c r="R35" s="33" t="str">
         <f t="shared" si="0"/>
         <v>tacrolimus</v>
       </c>
-      <c r="S35" s="35" t="s">
+      <c r="S35" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="T35" s="35" t="s">
+      <c r="T35" s="33" t="s">
         <v>478</v>
       </c>
-      <c r="U35" s="35" t="s">
+      <c r="U35" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="V35" s="35" t="s">
+      <c r="V35" s="33" t="s">
         <v>452</v>
       </c>
-      <c r="W35" s="35"/>
-      <c r="X35" s="35"/>
+      <c r="W35" s="33"/>
+      <c r="X35" s="33"/>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A36" s="45" t="s">
+      <c r="A36" s="53" t="s">
         <v>79</v>
       </c>
       <c r="B36" s="25"/>
       <c r="C36" s="25"/>
       <c r="D36" s="23"/>
-      <c r="E36" s="24">
+      <c r="E36" s="70">
         <v>1</v>
       </c>
       <c r="F36" s="23"/>
@@ -16722,30 +18024,30 @@
       <c r="N36" s="23"/>
       <c r="O36" s="23"/>
       <c r="P36" s="23"/>
-      <c r="Q36" s="52">
+      <c r="Q36" s="64">
         <v>1</v>
       </c>
-      <c r="R36" s="44" t="str">
+      <c r="R36" s="51" t="str">
         <f t="shared" si="0"/>
         <v>tamoxifen</v>
       </c>
-      <c r="S36" s="44" t="s">
+      <c r="S36" s="51" t="s">
         <v>417</v>
       </c>
-      <c r="T36" s="44"/>
-      <c r="U36" s="44" t="s">
+      <c r="T36" s="51"/>
+      <c r="U36" s="51" t="s">
         <v>427</v>
       </c>
-      <c r="V36" s="44" t="s">
+      <c r="V36" s="51" t="s">
         <v>427</v>
       </c>
-      <c r="W36" s="44"/>
-      <c r="X36" s="44" t="s">
+      <c r="W36" s="51"/>
+      <c r="X36" s="51" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A37" s="27" t="s">
+      <c r="A37" s="53" t="s">
         <v>255</v>
       </c>
       <c r="B37" s="25"/>
@@ -16754,7 +18056,7 @@
       <c r="E37" s="23"/>
       <c r="F37" s="23"/>
       <c r="G37" s="23"/>
-      <c r="H37" s="28">
+      <c r="H37" s="70">
         <v>1</v>
       </c>
       <c r="I37" s="23"/>
@@ -16765,24 +18067,24 @@
       <c r="N37" s="23"/>
       <c r="O37" s="23"/>
       <c r="P37" s="23"/>
-      <c r="Q37" s="9">
+      <c r="Q37" s="64">
         <v>1</v>
       </c>
-      <c r="R37" s="36" t="str">
+      <c r="R37" s="34" t="str">
         <f t="shared" si="0"/>
         <v>tegafur</v>
       </c>
-      <c r="S37" s="36" t="s">
+      <c r="S37" s="34" t="s">
         <v>415</v>
       </c>
-      <c r="T37" s="30"/>
-      <c r="U37" s="30"/>
-      <c r="V37" s="30"/>
-      <c r="W37" s="30"/>
-      <c r="X37" s="30"/>
+      <c r="T37" s="28"/>
+      <c r="U37" s="28"/>
+      <c r="V37" s="28"/>
+      <c r="W37" s="28"/>
+      <c r="X37" s="28"/>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="29" t="s">
         <v>81</v>
       </c>
       <c r="B38" s="25"/>
@@ -16797,32 +18099,32 @@
       <c r="K38" s="23"/>
       <c r="L38" s="23"/>
       <c r="M38" s="23"/>
-      <c r="N38" s="24">
+      <c r="N38" s="21">
         <v>1</v>
       </c>
       <c r="O38" s="23"/>
       <c r="P38" s="23"/>
-      <c r="Q38" s="32">
+      <c r="Q38" s="30">
         <v>1</v>
       </c>
-      <c r="R38" s="35" t="str">
+      <c r="R38" s="33" t="str">
         <f t="shared" si="0"/>
         <v>thioguanine</v>
       </c>
-      <c r="S38" s="35" t="s">
+      <c r="S38" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="T38" s="35" t="s">
+      <c r="T38" s="33" t="s">
         <v>474</v>
       </c>
-      <c r="U38" s="35" t="s">
+      <c r="U38" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="V38" s="35" t="s">
+      <c r="V38" s="33" t="s">
         <v>452</v>
       </c>
-      <c r="W38" s="35"/>
-      <c r="X38" s="35"/>
+      <c r="W38" s="33"/>
+      <c r="X38" s="33"/>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
@@ -16868,7 +18170,7 @@
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="29" t="s">
         <v>84</v>
       </c>
       <c r="B40" s="25"/>
@@ -16888,32 +18190,32 @@
       <c r="N40" s="23"/>
       <c r="O40" s="23"/>
       <c r="P40" s="23"/>
-      <c r="Q40" s="32">
+      <c r="Q40" s="30">
         <v>1</v>
       </c>
-      <c r="R40" s="35" t="str">
+      <c r="R40" s="33" t="str">
         <f t="shared" si="0"/>
         <v>tropisetron</v>
       </c>
-      <c r="S40" s="35" t="s">
+      <c r="S40" s="33" t="s">
         <v>417</v>
       </c>
-      <c r="T40" s="35" t="s">
+      <c r="T40" s="33" t="s">
         <v>451</v>
       </c>
-      <c r="U40" s="35" t="s">
+      <c r="U40" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="V40" s="35"/>
-      <c r="W40" s="35"/>
-      <c r="X40" s="35"/>
+      <c r="V40" s="33"/>
+      <c r="W40" s="33"/>
+      <c r="X40" s="33"/>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="29" t="s">
         <v>85</v>
       </c>
       <c r="B41" s="25"/>
-      <c r="C41" s="26">
+      <c r="C41" s="22">
         <v>1</v>
       </c>
       <c r="D41" s="23"/>
@@ -16929,40 +18231,40 @@
       <c r="N41" s="23"/>
       <c r="O41" s="23"/>
       <c r="P41" s="23"/>
-      <c r="Q41" s="32">
+      <c r="Q41" s="30">
         <v>1</v>
       </c>
-      <c r="R41" s="35" t="str">
+      <c r="R41" s="33" t="str">
         <f t="shared" si="0"/>
         <v>voriconazole</v>
       </c>
-      <c r="S41" s="35" t="s">
+      <c r="S41" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="T41" s="35" t="s">
+      <c r="T41" s="33" t="s">
         <v>471</v>
       </c>
-      <c r="U41" s="35" t="s">
+      <c r="U41" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="V41" s="35" t="s">
+      <c r="V41" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="W41" s="35"/>
-      <c r="X41" s="35"/>
+      <c r="W41" s="33"/>
+      <c r="X41" s="33"/>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A42" s="27" t="s">
+      <c r="A42" s="53" t="s">
         <v>87</v>
       </c>
       <c r="B42" s="25"/>
       <c r="C42" s="25"/>
-      <c r="D42" s="28">
+      <c r="D42" s="70">
         <v>1</v>
       </c>
       <c r="E42" s="23"/>
       <c r="F42" s="23"/>
-      <c r="G42" s="28">
+      <c r="G42" s="70">
         <v>1</v>
       </c>
       <c r="H42" s="23"/>
@@ -16973,24 +18275,24 @@
       <c r="M42" s="23"/>
       <c r="N42" s="23"/>
       <c r="O42" s="23"/>
-      <c r="P42" s="28">
+      <c r="P42" s="71">
         <v>1</v>
       </c>
-      <c r="Q42" s="9">
+      <c r="Q42" s="64">
         <v>3</v>
       </c>
-      <c r="R42" s="36" t="str">
+      <c r="R42" s="34" t="str">
         <f t="shared" si="0"/>
         <v>warfarin</v>
       </c>
-      <c r="S42" s="36" t="s">
+      <c r="S42" s="34" t="s">
         <v>416</v>
       </c>
-      <c r="T42" s="30"/>
-      <c r="U42" s="30"/>
-      <c r="V42" s="30"/>
-      <c r="W42" s="30"/>
-      <c r="X42" s="68" t="s">
+      <c r="T42" s="28"/>
+      <c r="U42" s="28"/>
+      <c r="V42" s="28"/>
+      <c r="W42" s="28"/>
+      <c r="X42" s="51" t="s">
         <v>461</v>
       </c>
     </row>
@@ -17047,11 +18349,73 @@
         <v>47</v>
       </c>
     </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B45" s="65" t="str">
+        <f>B4</f>
+        <v>CFTR</v>
+      </c>
+      <c r="C45" s="4" t="str">
+        <f t="shared" ref="C45:P45" si="1">C4</f>
+        <v>CYP2C19</v>
+      </c>
+      <c r="D45" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>CYP2C9</v>
+      </c>
+      <c r="E45" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>CYP2D6</v>
+      </c>
+      <c r="F45" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>CYP3A5</v>
+      </c>
+      <c r="G45" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>CYP4F2</v>
+      </c>
+      <c r="H45" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>DPYD</v>
+      </c>
+      <c r="I45" s="65" t="str">
+        <f t="shared" si="1"/>
+        <v>G6PD</v>
+      </c>
+      <c r="J45" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>HLA-A</v>
+      </c>
+      <c r="K45" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>HLA-B</v>
+      </c>
+      <c r="L45" s="65" t="str">
+        <f t="shared" si="1"/>
+        <v>IFNL3</v>
+      </c>
+      <c r="M45" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>SLCO1B1</v>
+      </c>
+      <c r="N45" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>TPMT</v>
+      </c>
+      <c r="O45" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>UGT1A1</v>
+      </c>
+      <c r="P45" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>VKORC1</v>
+      </c>
+    </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" s="13" t="s">
         <v>433</v>
       </c>
-      <c r="B46" s="49" t="s">
+      <c r="B46" s="65" t="s">
         <v>443</v>
       </c>
       <c r="C46" s="4" t="s">
@@ -17066,13 +18430,13 @@
       <c r="F46" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="G46" s="51" t="s">
+      <c r="G46" s="45" t="s">
         <v>437</v>
       </c>
-      <c r="H46" s="51" t="s">
+      <c r="H46" s="45" t="s">
         <v>462</v>
       </c>
-      <c r="I46" s="50" t="s">
+      <c r="I46" s="66" t="s">
         <v>440</v>
       </c>
       <c r="J46" s="5" t="s">
@@ -17081,19 +18445,19 @@
       <c r="K46" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="L46" s="50" t="s">
+      <c r="L46" s="66" t="s">
         <v>446</v>
       </c>
-      <c r="M46" s="5" t="s">
+      <c r="M46" s="52" t="s">
         <v>437</v>
       </c>
       <c r="N46" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="O46" s="46" t="s">
+      <c r="O46" s="42" t="s">
         <v>437</v>
       </c>
-      <c r="P46" s="51" t="s">
+      <c r="P46" s="45" t="s">
         <v>462</v>
       </c>
     </row>
@@ -17101,7 +18465,7 @@
       <c r="A47" s="13" t="s">
         <v>434</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="65" t="s">
         <v>441</v>
       </c>
       <c r="C47" s="4" t="s">
@@ -17116,13 +18480,13 @@
       <c r="F47" s="5" t="s">
         <v>441</v>
       </c>
-      <c r="G47" s="51" t="s">
+      <c r="G47" s="45" t="s">
         <v>441</v>
       </c>
-      <c r="H47" s="51" t="s">
+      <c r="H47" s="45" t="s">
         <v>441</v>
       </c>
-      <c r="I47" s="5" t="s">
+      <c r="I47" s="66" t="s">
         <v>441</v>
       </c>
       <c r="J47" s="5" t="s">
@@ -17131,7 +18495,7 @@
       <c r="K47" s="5" t="s">
         <v>439</v>
       </c>
-      <c r="L47" s="5" t="s">
+      <c r="L47" s="66" t="s">
         <v>448</v>
       </c>
       <c r="M47" s="5" t="s">
@@ -17140,10 +18504,10 @@
       <c r="N47" s="5" t="s">
         <v>441</v>
       </c>
-      <c r="O47" s="46" t="s">
+      <c r="O47" s="42" t="s">
         <v>441</v>
       </c>
-      <c r="P47" s="51" t="s">
+      <c r="P47" s="45" t="s">
         <v>441</v>
       </c>
     </row>
@@ -17151,31 +18515,31 @@
       <c r="A48" s="13" t="s">
         <v>436</v>
       </c>
-      <c r="B48" s="43"/>
-      <c r="C48" s="43"/>
+      <c r="B48" s="65"/>
+      <c r="C48" s="41"/>
       <c r="D48" s="5" t="s">
         <v>436</v>
       </c>
-      <c r="E48" s="29"/>
+      <c r="E48" s="27"/>
       <c r="F48" s="5" t="s">
         <v>436</v>
       </c>
-      <c r="G48" s="51" t="s">
+      <c r="G48" s="45" t="s">
         <v>436</v>
       </c>
-      <c r="H48" s="51"/>
-      <c r="I48" s="29"/>
-      <c r="J48" s="29"/>
-      <c r="K48" s="29"/>
-      <c r="L48" s="29"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="66"/>
+      <c r="J48" s="27"/>
+      <c r="K48" s="27"/>
+      <c r="L48" s="66"/>
       <c r="M48" s="5" t="s">
         <v>436</v>
       </c>
       <c r="N48" s="5" t="s">
         <v>436</v>
       </c>
-      <c r="O48" s="29"/>
-      <c r="P48" s="51" t="s">
+      <c r="O48" s="27"/>
+      <c r="P48" s="45" t="s">
         <v>436</v>
       </c>
     </row>
@@ -17183,71 +18547,71 @@
       <c r="A49" s="13" t="s">
         <v>435</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="65" t="s">
         <v>444</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="D49" s="29"/>
+      <c r="D49" s="27"/>
       <c r="E49" s="5" t="s">
         <v>438</v>
       </c>
-      <c r="F49" s="29"/>
-      <c r="G49" s="51"/>
-      <c r="H49" s="51" t="s">
+      <c r="F49" s="27"/>
+      <c r="G49" s="45"/>
+      <c r="H49" s="45" t="s">
         <v>438</v>
       </c>
-      <c r="I49" s="5" t="s">
+      <c r="I49" s="66" t="s">
         <v>442</v>
       </c>
-      <c r="J49" s="29"/>
-      <c r="K49" s="29"/>
-      <c r="L49" s="5" t="s">
+      <c r="J49" s="27"/>
+      <c r="K49" s="27"/>
+      <c r="L49" s="66" t="s">
         <v>447</v>
       </c>
-      <c r="M49" s="29"/>
-      <c r="N49" s="29"/>
-      <c r="O49" s="46" t="s">
+      <c r="M49" s="27"/>
+      <c r="N49" s="27"/>
+      <c r="O49" s="42" t="s">
         <v>438</v>
       </c>
-      <c r="P49" s="29"/>
+      <c r="P49" s="27"/>
     </row>
     <row r="50" spans="1:16" ht="159" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="53"/>
-      <c r="B50" s="53"/>
-      <c r="C50" s="53" t="s">
+      <c r="A50" s="46"/>
+      <c r="B50" s="68"/>
+      <c r="C50" s="46" t="s">
         <v>463</v>
       </c>
-      <c r="D50" s="54" t="s">
+      <c r="D50" s="47" t="s">
         <v>470</v>
       </c>
-      <c r="E50" s="54" t="s">
+      <c r="E50" s="47" t="s">
         <v>464</v>
       </c>
-      <c r="F50" s="54" t="s">
+      <c r="F50" s="47" t="s">
         <v>465</v>
       </c>
-      <c r="G50" s="56"/>
-      <c r="H50" s="56"/>
-      <c r="I50" s="54"/>
-      <c r="J50" s="55" t="s">
+      <c r="G50" s="49"/>
+      <c r="H50" s="49"/>
+      <c r="I50" s="67"/>
+      <c r="J50" s="48" t="s">
         <v>469</v>
       </c>
-      <c r="K50" s="55" t="s">
+      <c r="K50" s="48" t="s">
         <v>469</v>
       </c>
-      <c r="L50" s="54"/>
-      <c r="M50" s="54" t="s">
+      <c r="L50" s="67"/>
+      <c r="M50" s="47" t="s">
         <v>466</v>
       </c>
-      <c r="N50" s="54" t="s">
+      <c r="N50" s="47" t="s">
         <v>467</v>
       </c>
-      <c r="O50" s="54" t="s">
+      <c r="O50" s="47" t="s">
         <v>468</v>
       </c>
-      <c r="P50" s="57"/>
+      <c r="P50" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17306,22 +18670,22 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="54" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="56" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="62"/>
+      <c r="A5" s="55"/>
       <c r="B5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="63"/>
+      <c r="C5" s="57"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
@@ -17371,10 +18735,10 @@
       <c r="A10" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="66" t="s">
+      <c r="C10" s="60" t="s">
         <v>407</v>
       </c>
     </row>
@@ -17382,26 +18746,26 @@
       <c r="A11" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="67"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="61"/>
     </row>
     <row r="12" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="54" t="s">
         <v>115</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="60" t="s">
+      <c r="C12" s="56" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="62"/>
+      <c r="A13" s="55"/>
       <c r="B13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="63"/>
+      <c r="C13" s="57"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
@@ -17437,22 +18801,22 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="58" t="s">
+      <c r="A17" s="54" t="s">
         <v>122</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="60" t="s">
+      <c r="C17" s="56" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="62"/>
+      <c r="A18" s="55"/>
       <c r="B18" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="63"/>
+      <c r="C18" s="57"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
@@ -17477,22 +18841,22 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="64" t="s">
+      <c r="A21" s="58" t="s">
         <v>131</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="66" t="s">
+      <c r="C21" s="60" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="65"/>
+      <c r="A22" s="59"/>
       <c r="B22" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="67"/>
+      <c r="C22" s="61"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
@@ -17564,10 +18928,10 @@
       <c r="A29" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="B29" s="58" t="s">
+      <c r="B29" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="60" t="s">
+      <c r="C29" s="56" t="s">
         <v>407</v>
       </c>
     </row>
@@ -17575,33 +18939,33 @@
       <c r="A30" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="59"/>
-      <c r="C30" s="61"/>
+      <c r="B30" s="62"/>
+      <c r="C30" s="63"/>
     </row>
     <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="62"/>
-      <c r="C31" s="63"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="57"/>
     </row>
     <row r="32" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="64" t="s">
+      <c r="A32" s="58" t="s">
         <v>65</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="66" t="s">
+      <c r="C32" s="60" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="65"/>
+      <c r="A33" s="59"/>
       <c r="B33" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="67"/>
+      <c r="C33" s="61"/>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
@@ -17681,22 +19045,22 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="64" t="s">
+      <c r="A41" s="58" t="s">
         <v>166</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="66" t="s">
+      <c r="C41" s="60" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="65"/>
+      <c r="A42" s="59"/>
       <c r="B42" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="67"/>
+      <c r="C42" s="61"/>
     </row>
     <row r="43" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
@@ -17721,32 +19085,38 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="58" t="s">
+      <c r="A45" s="54" t="s">
         <v>87</v>
       </c>
       <c r="B45" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C45" s="60" t="s">
+      <c r="C45" s="56" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="59"/>
+      <c r="A46" s="62"/>
       <c r="B46" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="61"/>
+      <c r="C46" s="63"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="59"/>
+      <c r="A47" s="62"/>
       <c r="B47" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="61"/>
+      <c r="C47" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="C32:C33"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B10:B11"/>
@@ -17759,12 +19129,6 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="C32:C33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://cpicpgx.org/guidelines/guideline-for-abacavir-and-hla-b/"/>

</xml_diff>